<commit_message>
Updates through 2210 Joan Davis Show
</commit_message>
<xml_diff>
--- a/_Biographies.xlsx
+++ b/_Biographies.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f94822a51e6e525e/OTRR/otrr-biographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62E50384-6B7C-4CBC-B0A9-57AD0D627C42}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B809F84F-71DA-4C46-8805-15B8A635E560}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="285" windowWidth="37710" windowHeight="21465" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
+    <workbookView xWindow="1830" yWindow="5175" windowWidth="22110" windowHeight="15000" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$198</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$197</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="680">
   <si>
     <t>File</t>
   </si>
@@ -123,12 +123,6 @@
     <t>Frank Lee Graham Biography.pdf</t>
   </si>
   <si>
-    <t>Blue Beetle (OTRR Certified - Version 1)</t>
-  </si>
-  <si>
-    <t>Frank Lovejoy Biography.doc</t>
-  </si>
-  <si>
     <t>Maintained Set Rocky Fortune</t>
   </si>
   <si>
@@ -852,9 +846,6 @@
     <t>Rogue's Gallery</t>
   </si>
   <si>
-    <t>Blue Beetle</t>
-  </si>
-  <si>
     <t>Luke Slaughter</t>
   </si>
   <si>
@@ -1260,9 +1251,6 @@
     <t>Lou Merrill.pdf</t>
   </si>
   <si>
-    <t>Elliott Lewis.pdf</t>
-  </si>
-  <si>
     <t>Merrill, Lou</t>
   </si>
   <si>
@@ -1551,9 +1539,6 @@
     <t>William Woodson.docx</t>
   </si>
   <si>
-    <t>Frank Lovejoy.docx</t>
-  </si>
-  <si>
     <t>Stacy Harris.docx</t>
   </si>
   <si>
@@ -2044,6 +2029,54 @@
   </si>
   <si>
     <t>Eve Arden Biography.pdf</t>
+  </si>
+  <si>
+    <t>Voyage of the Scarlet Queen</t>
+  </si>
+  <si>
+    <t>Voyage of the Scarlet Queen, The - OTRR Maintained v. 2209</t>
+  </si>
+  <si>
+    <t>Elliott Lewis Biography.pdf</t>
+  </si>
+  <si>
+    <t>Tallman, Bob</t>
+  </si>
+  <si>
+    <t>Bob Tallman Biography.pdf</t>
+  </si>
+  <si>
+    <t>Doud, Gil</t>
+  </si>
+  <si>
+    <t>Gil Doud Biography.pdf</t>
+  </si>
+  <si>
+    <t>Frank Lovejoy Biography.pdf</t>
+  </si>
+  <si>
+    <t>Amazing Mr. Malone</t>
+  </si>
+  <si>
+    <t>Amazing Mr. Malone, The - OTRR Maintained v. 2208</t>
+  </si>
+  <si>
+    <t>Rice, Craig</t>
+  </si>
+  <si>
+    <t>Craig Rice Biography.pdf</t>
+  </si>
+  <si>
+    <t>Raymond, Gene</t>
+  </si>
+  <si>
+    <t>Gene Raymond Biography.pdf</t>
+  </si>
+  <si>
+    <t>Wang, Gene</t>
+  </si>
+  <si>
+    <t>Gene Wang Biography.pdf</t>
   </si>
 </sst>
 </file>
@@ -2079,9 +2112,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2396,11 +2428,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-  <dimension ref="A1:D246"/>
+  <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,13 +2445,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2427,220 +2459,220 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" t="s">
         <v>384</v>
       </c>
-      <c r="B2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C2" t="s">
-        <v>387</v>
-      </c>
       <c r="D2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>659</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>668</v>
+        <v>654</v>
+      </c>
+      <c r="D3" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="B5" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="C5" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="D5" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B10" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="B12" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="C12" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="D12" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="B16" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="C16" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D16" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -2651,178 +2683,178 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B18" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" t="s">
         <v>148</v>
-      </c>
-      <c r="D18" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B19" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C19" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D19" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B20" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C20" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D20" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B21" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C21" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D21" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B22" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C22" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D22" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B23" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="B24" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="C24" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="D24" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="B25" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C25" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="D25" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B26" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C27" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" t="s">
         <v>184</v>
-      </c>
-      <c r="D27" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D28" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -2833,248 +2865,248 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="B31" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="C31" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D31" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B32" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C32" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D32" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="B33" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="C33" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D33" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="B34" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C34" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D34" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B36" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B38" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B39" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B40" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C40" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D40" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B41" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B42" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C42" t="s">
+        <v>461</v>
+      </c>
+      <c r="D42" t="s">
         <v>465</v>
-      </c>
-      <c r="D42" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B43" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="C43" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="D43" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B44" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D45" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B46" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C46" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D46" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="B47" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="C47" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D47" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -3085,374 +3117,374 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B49" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C50" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="D50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B51" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B52" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="B53" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="C53" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D53" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B54" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C54" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D54" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B55" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D55" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B56" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C56" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D56" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B57" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C57" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D57" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B58" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C58" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D58" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B59" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C59" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D59" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="B60" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="C60" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="D60" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="B61" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="C61" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D61" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B62" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C62" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B63" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D63" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="B64" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C64" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D64" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="B65" t="s">
+        <v>521</v>
+      </c>
+      <c r="C65" t="s">
+        <v>522</v>
+      </c>
+      <c r="D65" t="s">
         <v>526</v>
-      </c>
-      <c r="C65" t="s">
-        <v>527</v>
-      </c>
-      <c r="D65" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="B66" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="C66" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D66" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="B67" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="C67" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="D67" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="B68" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="C68" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D68" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="B70" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="C70" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D70" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="B71" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="C71" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D71" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B72" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C72" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D72" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>611</v>
+      </c>
+      <c r="B73" t="s">
+        <v>612</v>
+      </c>
+      <c r="C73" t="s">
         <v>616</v>
       </c>
-      <c r="B73" t="s">
-        <v>617</v>
-      </c>
-      <c r="C73" t="s">
-        <v>621</v>
-      </c>
       <c r="D73" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B74" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C74" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D74" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B75" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -3463,1018 +3495,1018 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>316</v>
+        <v>669</v>
       </c>
       <c r="B76" t="s">
-        <v>262</v>
+        <v>664</v>
       </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>665</v>
       </c>
       <c r="D76" t="s">
-        <v>160</v>
+        <v>670</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>374</v>
+        <v>313</v>
       </c>
       <c r="B77" t="s">
-        <v>371</v>
+        <v>260</v>
       </c>
       <c r="C77" t="s">
-        <v>515</v>
+        <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>373</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>318</v>
+        <v>371</v>
       </c>
       <c r="B78" t="s">
-        <v>262</v>
+        <v>368</v>
       </c>
       <c r="C78" t="s">
-        <v>159</v>
+        <v>510</v>
       </c>
       <c r="D78" t="s">
-        <v>167</v>
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>110</v>
+        <v>315</v>
       </c>
       <c r="B79" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="C79" t="s">
-        <v>523</v>
+        <v>157</v>
       </c>
       <c r="D79" t="s">
-        <v>55</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B80" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="C80" t="s">
-        <v>37</v>
+        <v>518</v>
       </c>
       <c r="D80" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>395</v>
+        <v>94</v>
       </c>
       <c r="B81" t="s">
-        <v>399</v>
+        <v>252</v>
       </c>
       <c r="C81" t="s">
-        <v>398</v>
+        <v>35</v>
       </c>
       <c r="D81" t="s">
-        <v>392</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="B82" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
       <c r="C82" t="s">
-        <v>515</v>
+        <v>395</v>
       </c>
       <c r="D82" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>376</v>
       </c>
       <c r="B83" t="s">
-        <v>245</v>
+        <v>368</v>
       </c>
       <c r="C83" t="s">
-        <v>14</v>
+        <v>510</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>377</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>514</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="C84" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="D84" t="s">
-        <v>509</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>319</v>
+        <v>509</v>
       </c>
       <c r="B85" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C85" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="D85" t="s">
-        <v>168</v>
+        <v>504</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>459</v>
+        <v>316</v>
       </c>
       <c r="B86" t="s">
-        <v>456</v>
+        <v>276</v>
       </c>
       <c r="C86" t="s">
-        <v>455</v>
+        <v>72</v>
       </c>
       <c r="D86" t="s">
-        <v>457</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>298</v>
+        <v>455</v>
       </c>
       <c r="B87" t="s">
-        <v>280</v>
+        <v>452</v>
       </c>
       <c r="C87" t="s">
-        <v>126</v>
+        <v>451</v>
       </c>
       <c r="D87" t="s">
-        <v>127</v>
+        <v>453</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>344</v>
+        <v>295</v>
       </c>
       <c r="B88" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C88" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="D88" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="B89" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C89" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="D89" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>484</v>
+        <v>359</v>
       </c>
       <c r="B90" t="s">
-        <v>478</v>
+        <v>284</v>
       </c>
       <c r="C90" t="s">
-        <v>465</v>
+        <v>144</v>
       </c>
       <c r="D90" t="s">
-        <v>472</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>322</v>
+        <v>480</v>
       </c>
       <c r="B91" t="s">
-        <v>288</v>
+        <v>474</v>
       </c>
       <c r="C91" t="s">
-        <v>148</v>
+        <v>461</v>
       </c>
       <c r="D91" t="s">
-        <v>173</v>
+        <v>468</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>319</v>
       </c>
       <c r="B92" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C92" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="D92" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C93" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D93" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C94" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D94" t="s">
-        <v>75</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>365</v>
+        <v>123</v>
       </c>
       <c r="B95" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C95" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D95" t="s">
-        <v>164</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>605</v>
+        <v>362</v>
       </c>
       <c r="B96" t="s">
-        <v>613</v>
+        <v>276</v>
       </c>
       <c r="C96" t="s">
-        <v>612</v>
+        <v>72</v>
       </c>
       <c r="D96" t="s">
-        <v>608</v>
+        <v>162</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>323</v>
+        <v>600</v>
       </c>
       <c r="B97" t="s">
-        <v>537</v>
+        <v>608</v>
       </c>
       <c r="C97" t="s">
-        <v>538</v>
+        <v>607</v>
       </c>
       <c r="D97" t="s">
-        <v>539</v>
+        <v>603</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>104</v>
+        <v>320</v>
       </c>
       <c r="B98" t="s">
-        <v>249</v>
+        <v>532</v>
       </c>
       <c r="C98" t="s">
-        <v>26</v>
+        <v>533</v>
       </c>
       <c r="D98" t="s">
-        <v>27</v>
+        <v>534</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>491</v>
+        <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>494</v>
+        <v>247</v>
       </c>
       <c r="C99" t="s">
-        <v>493</v>
+        <v>26</v>
       </c>
       <c r="D99" t="s">
-        <v>492</v>
+        <v>27</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>607</v>
+        <v>487</v>
       </c>
       <c r="B100" t="s">
-        <v>613</v>
+        <v>490</v>
       </c>
       <c r="C100" t="s">
-        <v>612</v>
+        <v>489</v>
       </c>
       <c r="D100" t="s">
-        <v>611</v>
+        <v>488</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>369</v>
+        <v>602</v>
       </c>
       <c r="B101" t="s">
-        <v>279</v>
+        <v>608</v>
       </c>
       <c r="C101" t="s">
-        <v>74</v>
+        <v>607</v>
       </c>
       <c r="D101" t="s">
-        <v>232</v>
+        <v>606</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>122</v>
+        <v>366</v>
       </c>
       <c r="B102" t="s">
-        <v>524</v>
+        <v>276</v>
       </c>
       <c r="C102" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="D102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B103" t="s">
-        <v>253</v>
+        <v>519</v>
       </c>
       <c r="C103" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="D103" t="s">
-        <v>70</v>
+        <v>229</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>120</v>
       </c>
       <c r="B104" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="C104" t="s">
-        <v>169</v>
+        <v>20</v>
       </c>
       <c r="D104" t="s">
-        <v>191</v>
+        <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>330</v>
       </c>
       <c r="B105" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="C105" t="s">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="D105" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B106" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C106" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D106" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>358</v>
+        <v>114</v>
       </c>
       <c r="B107" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="C107" t="s">
-        <v>233</v>
+        <v>35</v>
       </c>
       <c r="D107" t="s">
-        <v>234</v>
+        <v>61</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>665</v>
+        <v>355</v>
       </c>
       <c r="B108" t="s">
-        <v>667</v>
+        <v>231</v>
       </c>
       <c r="C108" t="s">
-        <v>666</v>
+        <v>231</v>
       </c>
       <c r="D108" t="s">
-        <v>664</v>
+        <v>232</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>348</v>
+        <v>660</v>
       </c>
       <c r="B109" t="s">
-        <v>280</v>
+        <v>662</v>
       </c>
       <c r="C109" t="s">
-        <v>126</v>
+        <v>661</v>
       </c>
       <c r="D109" t="s">
-        <v>216</v>
+        <v>659</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>507</v>
+        <v>345</v>
       </c>
       <c r="B110" t="s">
-        <v>502</v>
+        <v>277</v>
       </c>
       <c r="C110" t="s">
-        <v>501</v>
+        <v>124</v>
       </c>
       <c r="D110" t="s">
-        <v>505</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>119</v>
+        <v>502</v>
       </c>
       <c r="B111" t="s">
-        <v>250</v>
+        <v>498</v>
       </c>
       <c r="C111" t="s">
-        <v>32</v>
+        <v>497</v>
       </c>
       <c r="D111" t="s">
-        <v>67</v>
+        <v>500</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>454</v>
+        <v>117</v>
       </c>
       <c r="B112" t="s">
-        <v>449</v>
+        <v>248</v>
       </c>
       <c r="C112" t="s">
-        <v>450</v>
+        <v>30</v>
       </c>
       <c r="D112" t="s">
-        <v>452</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="B113" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="C113" t="s">
-        <v>465</v>
+        <v>446</v>
       </c>
       <c r="D113" t="s">
-        <v>467</v>
+        <v>448</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>310</v>
+        <v>476</v>
       </c>
       <c r="B114" t="s">
-        <v>288</v>
+        <v>474</v>
       </c>
       <c r="C114" t="s">
-        <v>148</v>
+        <v>461</v>
       </c>
       <c r="D114" t="s">
-        <v>149</v>
+        <v>463</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>84</v>
+        <v>307</v>
       </c>
       <c r="B115" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="C115" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D115" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B116" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>152</v>
       </c>
       <c r="D116" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>305</v>
+        <v>82</v>
       </c>
       <c r="B117" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
       <c r="C117" t="s">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="D117" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>302</v>
       </c>
       <c r="B118" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
       <c r="C118" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="D118" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="B119" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C119" t="s">
-        <v>134</v>
+        <v>24</v>
       </c>
       <c r="D119" t="s">
-        <v>218</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B120" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="C120" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="D120" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>427</v>
+        <v>110</v>
       </c>
       <c r="B121" t="s">
-        <v>430</v>
+        <v>245</v>
       </c>
       <c r="C121" t="s">
-        <v>429</v>
+        <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>425</v>
+        <v>56</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>357</v>
+        <v>423</v>
       </c>
       <c r="B122" t="s">
-        <v>264</v>
+        <v>426</v>
       </c>
       <c r="C122" t="s">
-        <v>175</v>
+        <v>425</v>
       </c>
       <c r="D122" t="s">
-        <v>230</v>
+        <v>421</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>99</v>
+        <v>354</v>
       </c>
       <c r="B123" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C123" t="s">
-        <v>18</v>
+        <v>173</v>
       </c>
       <c r="D123" t="s">
-        <v>43</v>
+        <v>228</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>462</v>
+        <v>245</v>
       </c>
       <c r="C124" t="s">
-        <v>461</v>
+        <v>18</v>
       </c>
       <c r="D124" t="s">
-        <v>463</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B125" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C125" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D125" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>453</v>
+        <v>97</v>
       </c>
       <c r="B126" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="C126" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="D126" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>86</v>
+        <v>449</v>
       </c>
       <c r="B127" t="s">
-        <v>246</v>
+        <v>445</v>
       </c>
       <c r="C127" t="s">
-        <v>16</v>
+        <v>446</v>
       </c>
       <c r="D127" t="s">
-        <v>17</v>
+        <v>447</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>482</v>
+        <v>84</v>
       </c>
       <c r="B128" t="s">
-        <v>478</v>
+        <v>244</v>
       </c>
       <c r="C128" t="s">
-        <v>465</v>
+        <v>16</v>
       </c>
       <c r="D128" t="s">
-        <v>470</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>435</v>
+        <v>478</v>
       </c>
       <c r="B129" t="s">
-        <v>432</v>
+        <v>474</v>
       </c>
       <c r="C129" t="s">
-        <v>431</v>
+        <v>461</v>
       </c>
       <c r="D129" t="s">
-        <v>433</v>
+        <v>466</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>375</v>
+        <v>431</v>
       </c>
       <c r="B130" t="s">
-        <v>371</v>
+        <v>428</v>
       </c>
       <c r="C130" t="s">
-        <v>515</v>
+        <v>427</v>
       </c>
       <c r="D130" t="s">
-        <v>376</v>
+        <v>429</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>350</v>
+        <v>372</v>
       </c>
       <c r="B131" t="s">
-        <v>269</v>
+        <v>368</v>
       </c>
       <c r="C131" t="s">
-        <v>213</v>
+        <v>510</v>
       </c>
       <c r="D131" t="s">
-        <v>219</v>
+        <v>373</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B132" t="s">
-        <v>569</v>
+        <v>267</v>
       </c>
       <c r="C132" t="s">
-        <v>568</v>
+        <v>211</v>
       </c>
       <c r="D132" t="s">
-        <v>567</v>
+        <v>217</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>402</v>
+        <v>347</v>
       </c>
       <c r="B133" t="s">
-        <v>405</v>
+        <v>564</v>
       </c>
       <c r="C133" t="s">
-        <v>404</v>
+        <v>563</v>
       </c>
       <c r="D133" t="s">
-        <v>400</v>
+        <v>562</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>525</v>
+        <v>399</v>
       </c>
       <c r="B134" t="s">
-        <v>526</v>
+        <v>402</v>
       </c>
       <c r="C134" t="s">
-        <v>527</v>
+        <v>401</v>
       </c>
       <c r="D134" t="s">
-        <v>528</v>
+        <v>397</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>79</v>
+        <v>520</v>
       </c>
       <c r="B135" t="s">
-        <v>241</v>
+        <v>521</v>
       </c>
       <c r="C135" t="s">
-        <v>1</v>
+        <v>522</v>
       </c>
       <c r="D135" t="s">
-        <v>2</v>
+        <v>523</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>306</v>
+        <v>77</v>
       </c>
       <c r="B136" t="s">
-        <v>285</v>
+        <v>239</v>
       </c>
       <c r="C136" t="s">
-        <v>140</v>
+        <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>442</v>
+        <v>303</v>
       </c>
       <c r="B137" t="s">
-        <v>441</v>
+        <v>282</v>
       </c>
       <c r="C137" t="s">
-        <v>440</v>
+        <v>138</v>
       </c>
       <c r="D137" t="s">
-        <v>444</v>
+        <v>139</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>317</v>
+        <v>438</v>
       </c>
       <c r="B138" t="s">
-        <v>263</v>
+        <v>437</v>
       </c>
       <c r="C138" t="s">
-        <v>165</v>
+        <v>436</v>
       </c>
       <c r="D138" t="s">
-        <v>166</v>
+        <v>440</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B139" t="s">
-        <v>410</v>
+        <v>261</v>
       </c>
       <c r="C139" t="s">
-        <v>409</v>
+        <v>163</v>
       </c>
       <c r="D139" t="s">
-        <v>407</v>
+        <v>164</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B140" t="s">
-        <v>441</v>
+        <v>664</v>
       </c>
       <c r="C140" t="s">
-        <v>440</v>
+        <v>665</v>
       </c>
       <c r="D140" t="s">
-        <v>443</v>
+        <v>666</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B141" t="s">
-        <v>478</v>
+        <v>437</v>
       </c>
       <c r="C141" t="s">
-        <v>465</v>
+        <v>436</v>
       </c>
       <c r="D141" t="s">
-        <v>468</v>
+        <v>439</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>622</v>
+        <v>314</v>
       </c>
       <c r="B142" t="s">
-        <v>624</v>
+        <v>474</v>
       </c>
       <c r="C142" t="s">
-        <v>625</v>
+        <v>461</v>
       </c>
       <c r="D142" t="s">
-        <v>623</v>
+        <v>464</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>542</v>
+        <v>617</v>
       </c>
       <c r="B143" t="s">
-        <v>543</v>
+        <v>619</v>
       </c>
       <c r="C143" t="s">
-        <v>544</v>
+        <v>620</v>
       </c>
       <c r="D143" t="s">
-        <v>545</v>
+        <v>618</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="B144" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C144" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D144" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>91</v>
+        <v>541</v>
       </c>
       <c r="B145" t="s">
-        <v>271</v>
+        <v>538</v>
       </c>
       <c r="C145" t="s">
-        <v>28</v>
+        <v>539</v>
       </c>
       <c r="D145" t="s">
-        <v>29</v>
+        <v>542</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B146" t="s">
-        <v>502</v>
+        <v>672</v>
       </c>
       <c r="C146" t="s">
-        <v>501</v>
+        <v>673</v>
       </c>
       <c r="D146" t="s">
-        <v>504</v>
+        <v>671</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B147" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C147" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D147" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B148" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C148" t="s">
         <v>7</v>
@@ -4485,612 +4517,612 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B149" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C149" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D149" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>393</v>
+      </c>
+      <c r="B150" t="s">
         <v>396</v>
       </c>
-      <c r="B150" t="s">
-        <v>399</v>
-      </c>
       <c r="C150" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D150" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B151" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C151" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D151" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B152" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C152" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D152" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B153" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C153" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D153" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B154" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C154" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D154" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B155" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C155" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D155" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B156" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C156" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D156" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="B157" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="C157" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D157" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B158" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C158" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="D158" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="B159" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="C159" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="D159" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B160" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C160" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D160" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B161" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C161" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D161" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="B162" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C162" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D162" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B163" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C163" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D163" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B164" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C164" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D164" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B165" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C165" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D165" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B166" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C166" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D166" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B167" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C167" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D167" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B168" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="C168" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D168" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B169" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C169" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D169" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B170" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C170" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D170" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B171" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C171" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D171" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="B172" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="C172" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="D172" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B173" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C173" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D173" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B174" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C174" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D174" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B175" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C175" t="s">
         <v>3</v>
       </c>
       <c r="D175" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B176" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C176" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D176" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B177" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C177" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D177" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="B178" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C178" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D178" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="B179" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="C179" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="D179" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B180" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C180" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D180" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B181" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C181" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D181" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B182" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C182" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D182" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="B183" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C183" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="D183" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B184" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C184" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D184" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B185" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C185" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D185" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B186" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C186" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D186" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B187" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C187" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D187" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="B188" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C188" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="D188" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B189" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C189" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D189" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B190" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C190" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D190" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B191" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C191" t="s">
         <v>22</v>
       </c>
       <c r="D191" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B192" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C192" t="s">
         <v>20</v>
@@ -5101,436 +5133,436 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="B193" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="C193" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="D193" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B194" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C194" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D194" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>411</v>
+      </c>
+      <c r="B195" t="s">
+        <v>416</v>
+      </c>
+      <c r="C195" t="s">
         <v>415</v>
       </c>
-      <c r="B195" t="s">
-        <v>420</v>
-      </c>
-      <c r="C195" t="s">
-        <v>419</v>
-      </c>
       <c r="D195" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>340</v>
+        <v>676</v>
       </c>
       <c r="B196" t="s">
-        <v>295</v>
+        <v>672</v>
       </c>
       <c r="C196" t="s">
-        <v>202</v>
+        <v>673</v>
       </c>
       <c r="D196" t="s">
-        <v>203</v>
+        <v>677</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>80</v>
+        <v>337</v>
       </c>
       <c r="B197" t="s">
-        <v>242</v>
+        <v>292</v>
       </c>
       <c r="C197" t="s">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="D197" t="s">
-        <v>4</v>
+        <v>201</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B198" t="s">
-        <v>34</v>
+        <v>240</v>
       </c>
       <c r="C198" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D198" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>321</v>
+        <v>674</v>
       </c>
       <c r="B199" t="s">
-        <v>287</v>
+        <v>672</v>
       </c>
       <c r="C199" t="s">
-        <v>146</v>
+        <v>673</v>
       </c>
       <c r="D199" t="s">
-        <v>172</v>
+        <v>675</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>488</v>
+        <v>92</v>
       </c>
       <c r="B200" t="s">
-        <v>478</v>
+        <v>32</v>
       </c>
       <c r="C200" t="s">
-        <v>465</v>
+        <v>32</v>
       </c>
       <c r="D200" t="s">
-        <v>476</v>
+        <v>33</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>460</v>
+        <v>318</v>
       </c>
       <c r="B201" t="s">
-        <v>456</v>
+        <v>284</v>
       </c>
       <c r="C201" t="s">
-        <v>455</v>
+        <v>144</v>
       </c>
       <c r="D201" t="s">
-        <v>458</v>
+        <v>170</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>576</v>
+        <v>484</v>
       </c>
       <c r="B202" t="s">
-        <v>578</v>
+        <v>474</v>
       </c>
       <c r="C202" t="s">
-        <v>579</v>
+        <v>461</v>
       </c>
       <c r="D202" t="s">
-        <v>580</v>
+        <v>472</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>346</v>
+        <v>456</v>
       </c>
       <c r="B203" t="s">
-        <v>269</v>
+        <v>452</v>
       </c>
       <c r="C203" t="s">
-        <v>213</v>
+        <v>451</v>
       </c>
       <c r="D203" t="s">
-        <v>214</v>
+        <v>454</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>490</v>
+        <v>571</v>
       </c>
       <c r="B204" t="s">
-        <v>494</v>
+        <v>573</v>
       </c>
       <c r="C204" t="s">
-        <v>493</v>
+        <v>574</v>
       </c>
       <c r="D204" t="s">
-        <v>492</v>
+        <v>575</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="B205" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="C205" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="D205" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>92</v>
+        <v>486</v>
       </c>
       <c r="B206" t="s">
-        <v>275</v>
+        <v>490</v>
       </c>
       <c r="C206" t="s">
-        <v>30</v>
+        <v>489</v>
       </c>
       <c r="D206" t="s">
-        <v>31</v>
+        <v>488</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="B207" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="C207" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="D207" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>343</v>
+        <v>90</v>
       </c>
       <c r="B208" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C208" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="D208" t="s">
-        <v>207</v>
+        <v>29</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>489</v>
+        <v>317</v>
       </c>
       <c r="B209" t="s">
-        <v>478</v>
+        <v>270</v>
       </c>
       <c r="C209" t="s">
-        <v>465</v>
+        <v>167</v>
       </c>
       <c r="D209" t="s">
-        <v>477</v>
+        <v>168</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>98</v>
+        <v>340</v>
       </c>
       <c r="B210" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="C210" t="s">
-        <v>41</v>
+        <v>144</v>
       </c>
       <c r="D210" t="s">
-        <v>42</v>
+        <v>205</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>341</v>
+        <v>485</v>
       </c>
       <c r="B211" t="s">
-        <v>281</v>
+        <v>474</v>
       </c>
       <c r="C211" t="s">
-        <v>128</v>
+        <v>461</v>
       </c>
       <c r="D211" t="s">
-        <v>204</v>
+        <v>473</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>347</v>
+        <v>96</v>
       </c>
       <c r="B212" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="C212" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="D212" t="s">
-        <v>215</v>
+        <v>40</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>586</v>
+        <v>338</v>
       </c>
       <c r="B213" t="s">
-        <v>588</v>
+        <v>278</v>
       </c>
       <c r="C213" t="s">
-        <v>591</v>
+        <v>126</v>
       </c>
       <c r="D213" t="s">
-        <v>590</v>
+        <v>202</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="B214" t="s">
-        <v>252</v>
+        <v>285</v>
       </c>
       <c r="C214" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
       <c r="D214" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>381</v>
+        <v>667</v>
       </c>
       <c r="B215" t="s">
-        <v>371</v>
+        <v>664</v>
       </c>
       <c r="C215" t="s">
-        <v>515</v>
+        <v>665</v>
       </c>
       <c r="D215" t="s">
-        <v>382</v>
+        <v>668</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>303</v>
+        <v>581</v>
       </c>
       <c r="B216" t="s">
-        <v>259</v>
+        <v>583</v>
       </c>
       <c r="C216" t="s">
-        <v>134</v>
+        <v>586</v>
       </c>
       <c r="D216" t="s">
-        <v>135</v>
+        <v>585</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>483</v>
+        <v>336</v>
       </c>
       <c r="B217" t="s">
-        <v>478</v>
+        <v>250</v>
       </c>
       <c r="C217" t="s">
-        <v>465</v>
+        <v>7</v>
       </c>
       <c r="D217" t="s">
-        <v>471</v>
+        <v>199</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>335</v>
+        <v>378</v>
       </c>
       <c r="B218" t="s">
-        <v>288</v>
+        <v>368</v>
       </c>
       <c r="C218" t="s">
-        <v>148</v>
+        <v>510</v>
       </c>
       <c r="D218" t="s">
-        <v>195</v>
+        <v>379</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>534</v>
+        <v>300</v>
       </c>
       <c r="B219" t="s">
-        <v>526</v>
+        <v>257</v>
       </c>
       <c r="C219" t="s">
-        <v>527</v>
+        <v>132</v>
       </c>
       <c r="D219" t="s">
-        <v>530</v>
+        <v>133</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>108</v>
+        <v>479</v>
       </c>
       <c r="B220" t="s">
-        <v>258</v>
+        <v>474</v>
       </c>
       <c r="C220" t="s">
-        <v>71</v>
+        <v>461</v>
       </c>
       <c r="D220" t="s">
-        <v>199</v>
+        <v>467</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>108</v>
+        <v>332</v>
       </c>
       <c r="B221" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="C221" t="s">
-        <v>37</v>
+        <v>146</v>
       </c>
       <c r="D221" t="s">
-        <v>52</v>
+        <v>193</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>353</v>
+        <v>529</v>
       </c>
       <c r="B222" t="s">
-        <v>274</v>
+        <v>521</v>
       </c>
       <c r="C222" t="s">
-        <v>224</v>
+        <v>522</v>
       </c>
       <c r="D222" t="s">
-        <v>225</v>
+        <v>525</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>555</v>
+        <v>106</v>
       </c>
       <c r="B223" t="s">
-        <v>551</v>
+        <v>256</v>
       </c>
       <c r="C223" t="s">
-        <v>552</v>
+        <v>69</v>
       </c>
       <c r="D223" t="s">
-        <v>554</v>
+        <v>197</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5538,331 +5570,387 @@
         <v>106</v>
       </c>
       <c r="B224" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C224" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D224" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>121</v>
+        <v>350</v>
       </c>
       <c r="B225" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="C225" t="s">
-        <v>18</v>
+        <v>222</v>
       </c>
       <c r="D225" t="s">
-        <v>69</v>
+        <v>223</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>397</v>
+        <v>550</v>
       </c>
       <c r="B226" t="s">
-        <v>399</v>
+        <v>546</v>
       </c>
       <c r="C226" t="s">
-        <v>398</v>
+        <v>547</v>
       </c>
       <c r="D226" t="s">
-        <v>394</v>
+        <v>549</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>325</v>
+        <v>104</v>
       </c>
       <c r="B227" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="C227" t="s">
-        <v>175</v>
+        <v>24</v>
       </c>
       <c r="D227" t="s">
-        <v>176</v>
+        <v>42</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>359</v>
+        <v>119</v>
       </c>
       <c r="B228" t="s">
-        <v>284</v>
+        <v>245</v>
       </c>
       <c r="C228" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="D228" t="s">
-        <v>237</v>
+        <v>67</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>359</v>
+        <v>394</v>
       </c>
       <c r="B229" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="C229" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="D229" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>314</v>
+        <v>678</v>
       </c>
       <c r="B230" t="s">
-        <v>281</v>
+        <v>672</v>
       </c>
       <c r="C230" t="s">
-        <v>128</v>
+        <v>673</v>
       </c>
       <c r="D230" t="s">
-        <v>157</v>
+        <v>679</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>97</v>
+        <v>322</v>
       </c>
       <c r="B231" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="C231" t="s">
-        <v>26</v>
+        <v>173</v>
       </c>
       <c r="D231" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>97</v>
+        <v>356</v>
       </c>
       <c r="B232" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C232" t="s">
         <v>136</v>
       </c>
       <c r="D232" t="s">
-        <v>187</v>
+        <v>235</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>97</v>
+        <v>356</v>
       </c>
       <c r="B233" t="s">
-        <v>294</v>
+        <v>416</v>
       </c>
       <c r="C233" t="s">
-        <v>50</v>
+        <v>415</v>
       </c>
       <c r="D233" t="s">
-        <v>188</v>
+        <v>414</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>97</v>
+        <v>311</v>
       </c>
       <c r="B234" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C234" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D234" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B235" t="s">
         <v>247</v>
       </c>
       <c r="C235" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D235" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B236" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="C236" t="s">
-        <v>208</v>
+        <v>134</v>
       </c>
       <c r="D236" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B237" t="s">
-        <v>256</v>
+        <v>291</v>
       </c>
       <c r="C237" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D237" t="s">
-        <v>54</v>
+        <v>186</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B238" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="C238" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="D238" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>601</v>
+        <v>87</v>
       </c>
       <c r="B239" t="s">
-        <v>600</v>
+        <v>245</v>
       </c>
       <c r="C239" t="s">
-        <v>604</v>
+        <v>18</v>
       </c>
       <c r="D239" t="s">
-        <v>602</v>
+        <v>23</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>601</v>
+        <v>107</v>
       </c>
       <c r="B240" t="s">
-        <v>600</v>
+        <v>265</v>
       </c>
       <c r="C240" t="s">
-        <v>604</v>
+        <v>206</v>
       </c>
       <c r="D240" t="s">
-        <v>603</v>
+        <v>207</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>389</v>
+        <v>107</v>
       </c>
       <c r="B241" t="s">
-        <v>391</v>
+        <v>254</v>
       </c>
       <c r="C241" t="s">
-        <v>390</v>
+        <v>51</v>
       </c>
       <c r="D241" t="s">
-        <v>388</v>
+        <v>52</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>338</v>
+        <v>121</v>
       </c>
       <c r="B242" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C242" t="s">
-        <v>154</v>
+        <v>69</v>
       </c>
       <c r="D242" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>506</v>
+        <v>596</v>
       </c>
       <c r="B243" t="s">
-        <v>502</v>
+        <v>595</v>
       </c>
       <c r="C243" t="s">
-        <v>501</v>
+        <v>599</v>
       </c>
       <c r="D243" t="s">
-        <v>503</v>
+        <v>597</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>304</v>
+        <v>596</v>
       </c>
       <c r="B244" t="s">
-        <v>283</v>
+        <v>595</v>
       </c>
       <c r="C244" t="s">
-        <v>136</v>
+        <v>599</v>
       </c>
       <c r="D244" t="s">
-        <v>137</v>
+        <v>598</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>114</v>
+        <v>386</v>
       </c>
       <c r="B245" t="s">
-        <v>248</v>
+        <v>388</v>
       </c>
       <c r="C245" t="s">
-        <v>24</v>
+        <v>387</v>
       </c>
       <c r="D245" t="s">
-        <v>60</v>
+        <v>385</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="B246" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="C246" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="D246" t="s">
-        <v>145</v>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>501</v>
+      </c>
+      <c r="B247" t="s">
+        <v>498</v>
+      </c>
+      <c r="C247" t="s">
+        <v>497</v>
+      </c>
+      <c r="D247" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>301</v>
+      </c>
+      <c r="B248" t="s">
+        <v>280</v>
+      </c>
+      <c r="C248" t="s">
+        <v>134</v>
+      </c>
+      <c r="D248" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>112</v>
+      </c>
+      <c r="B249" t="s">
+        <v>246</v>
+      </c>
+      <c r="C249" t="s">
+        <v>24</v>
+      </c>
+      <c r="D249" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>305</v>
+      </c>
+      <c r="B250" t="s">
+        <v>283</v>
+      </c>
+      <c r="C250" t="s">
+        <v>142</v>
+      </c>
+      <c r="D250" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D198" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D205">
-      <sortCondition ref="A1:A198"/>
+  <autoFilter ref="A1:D197" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D204">
+      <sortCondition ref="A1:A197"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D246">
-    <sortCondition ref="A2:A246"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D250">
+    <sortCondition ref="A2:A250"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates from Our Miss Brooks, 2000 Plus sets
</commit_message>
<xml_diff>
--- a/_Biographies.xlsx
+++ b/_Biographies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f94822a51e6e525e/OTRR/otrr-biographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="203" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B809F84F-71DA-4C46-8805-15B8A635E560}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70E45052-E479-4F06-85B7-168257DD40AF}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="5175" windowWidth="22110" windowHeight="15000" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
+    <workbookView xWindow="0" yWindow="5070" windowWidth="22845" windowHeight="20370" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1548,9 +1548,6 @@
     <t>Harris, Stacy</t>
   </si>
   <si>
-    <t>William Conrad.pdf</t>
-  </si>
-  <si>
     <t>GeorgiaEllis.pdf</t>
   </si>
   <si>
@@ -2077,6 +2074,9 @@
   </si>
   <si>
     <t>Gene Wang Biography.pdf</t>
+  </si>
+  <si>
+    <t>William Conrad Biography.docx</t>
   </si>
 </sst>
 </file>
@@ -2432,7 +2432,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,16 +2473,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B3" t="s">
         <v>244</v>
       </c>
       <c r="C3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2501,16 +2501,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>577</v>
+      </c>
+      <c r="B5" t="s">
+        <v>579</v>
+      </c>
+      <c r="C5" t="s">
         <v>578</v>
       </c>
-      <c r="B5" t="s">
-        <v>580</v>
-      </c>
-      <c r="C5" t="s">
-        <v>579</v>
-      </c>
       <c r="D5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2599,16 +2599,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>636</v>
+      </c>
+      <c r="B12" t="s">
+        <v>639</v>
+      </c>
+      <c r="C12" t="s">
+        <v>638</v>
+      </c>
+      <c r="D12" t="s">
         <v>637</v>
-      </c>
-      <c r="B12" t="s">
-        <v>640</v>
-      </c>
-      <c r="C12" t="s">
-        <v>639</v>
-      </c>
-      <c r="D12" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2655,16 +2655,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B16" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C16" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D16" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,13 +2728,13 @@
         <v>346</v>
       </c>
       <c r="B21" t="s">
+        <v>545</v>
+      </c>
+      <c r="C21" t="s">
         <v>546</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>547</v>
-      </c>
-      <c r="D21" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,30 +2767,30 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>591</v>
+      </c>
+      <c r="B24" t="s">
         <v>592</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>593</v>
       </c>
-      <c r="C24" t="s">
-        <v>594</v>
-      </c>
       <c r="D24" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>534</v>
+      </c>
+      <c r="B25" t="s">
+        <v>531</v>
+      </c>
+      <c r="C25" t="s">
+        <v>532</v>
+      </c>
+      <c r="D25" t="s">
         <v>535</v>
-      </c>
-      <c r="B25" t="s">
-        <v>532</v>
-      </c>
-      <c r="C25" t="s">
-        <v>533</v>
-      </c>
-      <c r="D25" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2865,16 +2865,16 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C31" t="s">
+        <v>615</v>
+      </c>
+      <c r="D31" t="s">
         <v>612</v>
-      </c>
-      <c r="C31" t="s">
-        <v>616</v>
-      </c>
-      <c r="D31" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2885,7 +2885,7 @@
         <v>368</v>
       </c>
       <c r="C32" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D32" t="s">
         <v>375</v>
@@ -2893,30 +2893,30 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>571</v>
+      </c>
+      <c r="B33" t="s">
         <v>572</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>573</v>
       </c>
-      <c r="C33" t="s">
-        <v>574</v>
-      </c>
       <c r="D33" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B34" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C34" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D34" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3033,16 +3033,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>628</v>
+      </c>
+      <c r="B43" t="s">
+        <v>631</v>
+      </c>
+      <c r="C43" t="s">
+        <v>630</v>
+      </c>
+      <c r="D43" t="s">
         <v>629</v>
-      </c>
-      <c r="B43" t="s">
-        <v>632</v>
-      </c>
-      <c r="C43" t="s">
-        <v>631</v>
-      </c>
-      <c r="D43" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3084,21 +3084,21 @@
         <v>433</v>
       </c>
       <c r="D46" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B47" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C47" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D47" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
         <v>274</v>
       </c>
       <c r="C50" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D50" t="s">
         <v>64</v>
@@ -3173,16 +3173,16 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B53" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C53" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D53" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3210,7 +3210,7 @@
         <v>126</v>
       </c>
       <c r="D55" t="s">
-        <v>503</v>
+        <v>679</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3271,30 +3271,30 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>581</v>
+      </c>
+      <c r="B60" t="s">
         <v>582</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>585</v>
+      </c>
+      <c r="D60" t="s">
         <v>583</v>
-      </c>
-      <c r="C60" t="s">
-        <v>586</v>
-      </c>
-      <c r="D60" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B61" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C61" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D61" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B64" t="s">
         <v>278</v>
@@ -3336,63 +3336,63 @@
         <v>126</v>
       </c>
       <c r="D64" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B65" t="s">
+        <v>520</v>
+      </c>
+      <c r="C65" t="s">
         <v>521</v>
       </c>
-      <c r="C65" t="s">
-        <v>522</v>
-      </c>
       <c r="D65" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>649</v>
+      </c>
+      <c r="B66" t="s">
+        <v>651</v>
+      </c>
+      <c r="C66" t="s">
         <v>650</v>
       </c>
-      <c r="B66" t="s">
-        <v>652</v>
-      </c>
-      <c r="C66" t="s">
-        <v>651</v>
-      </c>
       <c r="D66" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>640</v>
+      </c>
+      <c r="B67" t="s">
         <v>641</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>642</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>643</v>
-      </c>
-      <c r="D67" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>654</v>
+      </c>
+      <c r="B68" t="s">
+        <v>657</v>
+      </c>
+      <c r="C68" t="s">
+        <v>656</v>
+      </c>
+      <c r="D68" t="s">
         <v>655</v>
-      </c>
-      <c r="B68" t="s">
-        <v>658</v>
-      </c>
-      <c r="C68" t="s">
-        <v>657</v>
-      </c>
-      <c r="D68" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3411,30 +3411,30 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B70" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C70" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D70" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>567</v>
+      </c>
+      <c r="B71" t="s">
+        <v>569</v>
+      </c>
+      <c r="C71" t="s">
         <v>568</v>
       </c>
-      <c r="B71" t="s">
-        <v>570</v>
-      </c>
-      <c r="C71" t="s">
-        <v>569</v>
-      </c>
       <c r="D71" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,16 +3453,16 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>610</v>
+      </c>
+      <c r="B73" t="s">
         <v>611</v>
       </c>
-      <c r="B73" t="s">
-        <v>612</v>
-      </c>
       <c r="C73" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D73" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3495,16 +3495,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>668</v>
+      </c>
+      <c r="B76" t="s">
+        <v>663</v>
+      </c>
+      <c r="C76" t="s">
+        <v>664</v>
+      </c>
+      <c r="D76" t="s">
         <v>669</v>
-      </c>
-      <c r="B76" t="s">
-        <v>664</v>
-      </c>
-      <c r="C76" t="s">
-        <v>665</v>
-      </c>
-      <c r="D76" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3529,7 +3529,7 @@
         <v>368</v>
       </c>
       <c r="C78" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D78" t="s">
         <v>370</v>
@@ -3557,7 +3557,7 @@
         <v>274</v>
       </c>
       <c r="C80" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D80" t="s">
         <v>53</v>
@@ -3599,7 +3599,7 @@
         <v>368</v>
       </c>
       <c r="C83" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D83" t="s">
         <v>377</v>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B85" t="s">
         <v>278</v>
@@ -3630,7 +3630,7 @@
         <v>126</v>
       </c>
       <c r="D85" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3789,16 +3789,16 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B97" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C97" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D97" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3806,13 +3806,13 @@
         <v>320</v>
       </c>
       <c r="B98" t="s">
+        <v>531</v>
+      </c>
+      <c r="C98" t="s">
         <v>532</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>533</v>
-      </c>
-      <c r="D98" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3845,16 +3845,16 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B101" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C101" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D101" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,7 +3876,7 @@
         <v>120</v>
       </c>
       <c r="B103" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C103" t="s">
         <v>144</v>
@@ -3957,16 +3957,16 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>659</v>
+      </c>
+      <c r="B109" t="s">
+        <v>661</v>
+      </c>
+      <c r="C109" t="s">
         <v>660</v>
       </c>
-      <c r="B109" t="s">
-        <v>662</v>
-      </c>
-      <c r="C109" t="s">
-        <v>661</v>
-      </c>
       <c r="D109" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4271,7 +4271,7 @@
         <v>368</v>
       </c>
       <c r="C131" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D131" t="s">
         <v>373</v>
@@ -4296,13 +4296,13 @@
         <v>347</v>
       </c>
       <c r="B133" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C133" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D133" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4321,16 +4321,16 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>519</v>
+      </c>
+      <c r="B135" t="s">
         <v>520</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>521</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" t="s">
         <v>522</v>
-      </c>
-      <c r="D135" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -4394,13 +4394,13 @@
         <v>314</v>
       </c>
       <c r="B140" t="s">
+        <v>663</v>
+      </c>
+      <c r="C140" t="s">
         <v>664</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
         <v>665</v>
-      </c>
-      <c r="D140" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4433,44 +4433,44 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>616</v>
+      </c>
+      <c r="B143" t="s">
+        <v>618</v>
+      </c>
+      <c r="C143" t="s">
+        <v>619</v>
+      </c>
+      <c r="D143" t="s">
         <v>617</v>
-      </c>
-      <c r="B143" t="s">
-        <v>619</v>
-      </c>
-      <c r="C143" t="s">
-        <v>620</v>
-      </c>
-      <c r="D143" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>536</v>
+      </c>
+      <c r="B144" t="s">
         <v>537</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>538</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>539</v>
-      </c>
-      <c r="D144" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>540</v>
+      </c>
+      <c r="B145" t="s">
+        <v>537</v>
+      </c>
+      <c r="C145" t="s">
+        <v>538</v>
+      </c>
+      <c r="D145" t="s">
         <v>541</v>
-      </c>
-      <c r="B145" t="s">
-        <v>538</v>
-      </c>
-      <c r="C145" t="s">
-        <v>539</v>
-      </c>
-      <c r="D145" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4478,13 +4478,13 @@
         <v>89</v>
       </c>
       <c r="B146" t="s">
+        <v>671</v>
+      </c>
+      <c r="C146" t="s">
         <v>672</v>
       </c>
-      <c r="C146" t="s">
-        <v>673</v>
-      </c>
       <c r="D146" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4629,44 +4629,44 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>551</v>
+      </c>
+      <c r="B157" t="s">
         <v>552</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>553</v>
       </c>
-      <c r="C157" t="s">
-        <v>554</v>
-      </c>
       <c r="D157" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>510</v>
+      </c>
+      <c r="B158" t="s">
         <v>511</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>512</v>
       </c>
-      <c r="C158" t="s">
+      <c r="D158" t="s">
         <v>513</v>
-      </c>
-      <c r="D158" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>633</v>
+      </c>
+      <c r="B159" t="s">
         <v>634</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" t="s">
         <v>635</v>
       </c>
-      <c r="C159" t="s">
-        <v>636</v>
-      </c>
       <c r="D159" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4699,7 +4699,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B162" t="s">
         <v>278</v>
@@ -4708,21 +4708,21 @@
         <v>126</v>
       </c>
       <c r="D162" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B163" t="s">
+        <v>520</v>
+      </c>
+      <c r="C163" t="s">
         <v>521</v>
       </c>
-      <c r="C163" t="s">
-        <v>522</v>
-      </c>
       <c r="D163" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4786,13 +4786,13 @@
         <v>91</v>
       </c>
       <c r="B168" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C168" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D168" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4839,16 +4839,16 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B172" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C172" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D172" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4895,58 +4895,58 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>625</v>
+      </c>
+      <c r="B176" t="s">
+        <v>627</v>
+      </c>
+      <c r="C176" t="s">
         <v>626</v>
       </c>
-      <c r="B176" t="s">
-        <v>628</v>
-      </c>
-      <c r="C176" t="s">
-        <v>627</v>
-      </c>
       <c r="D176" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>625</v>
+      </c>
+      <c r="B177" t="s">
+        <v>627</v>
+      </c>
+      <c r="C177" t="s">
         <v>626</v>
       </c>
-      <c r="B177" t="s">
-        <v>628</v>
-      </c>
-      <c r="C177" t="s">
-        <v>627</v>
-      </c>
       <c r="D177" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>625</v>
+      </c>
+      <c r="B178" t="s">
+        <v>627</v>
+      </c>
+      <c r="C178" t="s">
         <v>626</v>
       </c>
-      <c r="B178" t="s">
-        <v>628</v>
-      </c>
-      <c r="C178" t="s">
-        <v>627</v>
-      </c>
       <c r="D178" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>644</v>
+      </c>
+      <c r="B179" t="s">
+        <v>646</v>
+      </c>
+      <c r="C179" t="s">
         <v>645</v>
       </c>
-      <c r="B179" t="s">
+      <c r="D179" t="s">
         <v>647</v>
-      </c>
-      <c r="C179" t="s">
-        <v>646</v>
-      </c>
-      <c r="D179" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4965,7 +4965,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B181" t="s">
         <v>291</v>
@@ -4974,7 +4974,7 @@
         <v>48</v>
       </c>
       <c r="D181" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4993,16 +4993,16 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B183" t="s">
         <v>287</v>
       </c>
       <c r="C183" t="s">
+        <v>515</v>
+      </c>
+      <c r="D183" t="s">
         <v>516</v>
-      </c>
-      <c r="D183" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,16 +5063,16 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B188" t="s">
+        <v>520</v>
+      </c>
+      <c r="C188" t="s">
         <v>521</v>
       </c>
-      <c r="C188" t="s">
-        <v>522</v>
-      </c>
       <c r="D188" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5097,7 +5097,7 @@
         <v>368</v>
       </c>
       <c r="C190" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D190" t="s">
         <v>369</v>
@@ -5133,16 +5133,16 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B193" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C193" t="s">
+        <v>586</v>
+      </c>
+      <c r="D193" t="s">
         <v>587</v>
-      </c>
-      <c r="D193" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -5175,16 +5175,16 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>675</v>
+      </c>
+      <c r="B196" t="s">
+        <v>671</v>
+      </c>
+      <c r="C196" t="s">
+        <v>672</v>
+      </c>
+      <c r="D196" t="s">
         <v>676</v>
-      </c>
-      <c r="B196" t="s">
-        <v>672</v>
-      </c>
-      <c r="C196" t="s">
-        <v>673</v>
-      </c>
-      <c r="D196" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5217,16 +5217,16 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>673</v>
+      </c>
+      <c r="B199" t="s">
+        <v>671</v>
+      </c>
+      <c r="C199" t="s">
+        <v>672</v>
+      </c>
+      <c r="D199" t="s">
         <v>674</v>
-      </c>
-      <c r="B199" t="s">
-        <v>672</v>
-      </c>
-      <c r="C199" t="s">
-        <v>673</v>
-      </c>
-      <c r="D199" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -5287,16 +5287,16 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B204" t="s">
+        <v>572</v>
+      </c>
+      <c r="C204" t="s">
         <v>573</v>
       </c>
-      <c r="C204" t="s">
+      <c r="D204" t="s">
         <v>574</v>
-      </c>
-      <c r="D204" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5441,30 +5441,30 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>666</v>
+      </c>
+      <c r="B215" t="s">
+        <v>663</v>
+      </c>
+      <c r="C215" t="s">
+        <v>664</v>
+      </c>
+      <c r="D215" t="s">
         <v>667</v>
-      </c>
-      <c r="B215" t="s">
-        <v>664</v>
-      </c>
-      <c r="C215" t="s">
-        <v>665</v>
-      </c>
-      <c r="D215" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B216" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C216" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D216" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5489,7 +5489,7 @@
         <v>368</v>
       </c>
       <c r="C218" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D218" t="s">
         <v>379</v>
@@ -5539,16 +5539,16 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B222" t="s">
+        <v>520</v>
+      </c>
+      <c r="C222" t="s">
         <v>521</v>
       </c>
-      <c r="C222" t="s">
-        <v>522</v>
-      </c>
       <c r="D222" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5595,16 +5595,16 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B226" t="s">
+        <v>545</v>
+      </c>
+      <c r="C226" t="s">
         <v>546</v>
       </c>
-      <c r="C226" t="s">
-        <v>547</v>
-      </c>
       <c r="D226" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5651,16 +5651,16 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
+        <v>677</v>
+      </c>
+      <c r="B230" t="s">
+        <v>671</v>
+      </c>
+      <c r="C230" t="s">
+        <v>672</v>
+      </c>
+      <c r="D230" t="s">
         <v>678</v>
-      </c>
-      <c r="B230" t="s">
-        <v>672</v>
-      </c>
-      <c r="C230" t="s">
-        <v>673</v>
-      </c>
-      <c r="D230" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5833,30 +5833,30 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
+        <v>595</v>
+      </c>
+      <c r="B243" t="s">
+        <v>594</v>
+      </c>
+      <c r="C243" t="s">
+        <v>598</v>
+      </c>
+      <c r="D243" t="s">
         <v>596</v>
-      </c>
-      <c r="B243" t="s">
-        <v>595</v>
-      </c>
-      <c r="C243" t="s">
-        <v>599</v>
-      </c>
-      <c r="D243" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B244" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C244" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D244" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates through Family Theater 2302
</commit_message>
<xml_diff>
--- a/_Biographies.xlsx
+++ b/_Biographies.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f94822a51e6e525e/OTRR/otrr-biographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70E45052-E479-4F06-85B7-168257DD40AF}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6DF1B16-45A3-4C6F-84B4-FC2FC5762E93}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5070" windowWidth="22845" windowHeight="20370" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
+    <workbookView xWindow="-11955" yWindow="-20790" windowWidth="16785" windowHeight="15690" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$197</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$195</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="680">
   <si>
     <t>File</t>
   </si>
@@ -99,15 +99,9 @@
     <t>David Brian Biography.pdf</t>
   </si>
   <si>
-    <t>Richard Diamond v. 3</t>
-  </si>
-  <si>
     <t>Dick Powell Biography.pdf</t>
   </si>
   <si>
-    <t>Rogue's Gallery (OTRR Certified - Ver 4)</t>
-  </si>
-  <si>
     <t>Dwight Weist Biography.pdf</t>
   </si>
   <si>
@@ -261,9 +255,6 @@
     <t>William Gargan Biography.doc</t>
   </si>
   <si>
-    <t>Dick Powell Biography (2).pdf</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -474,9 +465,6 @@
     <t>Let George Do It V3</t>
   </si>
   <si>
-    <t>Bob Bailey Bio.pdf</t>
-  </si>
-  <si>
     <t>Challenge of the Yukon v4</t>
   </si>
   <si>
@@ -516,9 +504,6 @@
     <t>Don+Douglas+-+bio.docx</t>
   </si>
   <si>
-    <t>Eddie Firestone Jr bio.pdf</t>
-  </si>
-  <si>
     <t>Tarzan V. 2 OTRR</t>
   </si>
   <si>
@@ -549,9 +534,6 @@
     <t>Fletcher Markle's Bio.pdf</t>
   </si>
   <si>
-    <t>Frances Robinson Bio.pdf</t>
-  </si>
-  <si>
     <t>Fred Foy Bio.pdf</t>
   </si>
   <si>
@@ -654,9 +636,6 @@
     <t>Norman Corwin bio.txt</t>
   </si>
   <si>
-    <t>Olan Soule bio.pdf</t>
-  </si>
-  <si>
     <t>Hello Americans - OTRR V 2</t>
   </si>
   <si>
@@ -726,9 +705,6 @@
     <t>Victor Jory Bio.txt</t>
   </si>
   <si>
-    <t>Virginia Gregg bio.pdf</t>
-  </si>
-  <si>
     <t>Virginia Gregg Burket Bio.doc</t>
   </si>
   <si>
@@ -792,9 +768,6 @@
     <t>Mysterious Traveler</t>
   </si>
   <si>
-    <t>Richard Diamond</t>
-  </si>
-  <si>
     <t>Sam Spade</t>
   </si>
   <si>
@@ -1593,9 +1566,6 @@
     <t>Adventures of Frank Race, The - OTRR Maintained 2201</t>
   </si>
   <si>
-    <t>Let George Do It [best version]</t>
-  </si>
-  <si>
     <t>Kroeger, Berry</t>
   </si>
   <si>
@@ -2077,6 +2047,36 @@
   </si>
   <si>
     <t>William Conrad Biography.docx</t>
+  </si>
+  <si>
+    <t>Peyton, Father Patrick</t>
+  </si>
+  <si>
+    <t>Family Theater</t>
+  </si>
+  <si>
+    <t>Family Theater - OTRR Maintained v. 2302</t>
+  </si>
+  <si>
+    <t>Father Patrick Peyton Biography.pdf</t>
+  </si>
+  <si>
+    <t>Bob Bailey Biography.pdf</t>
+  </si>
+  <si>
+    <t>Let George Do It - OTRR Maintained 2212</t>
+  </si>
+  <si>
+    <t>Eddie Firestone, Jr. Biography.pdf</t>
+  </si>
+  <si>
+    <t>Frances Robinson Biography.pdf</t>
+  </si>
+  <si>
+    <t>Olan Soule Biography.pdf</t>
+  </si>
+  <si>
+    <t>Rogues Gallery - OTRR Maintained v. 2211</t>
   </si>
 </sst>
 </file>
@@ -2428,11 +2428,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-  <dimension ref="A1:D250"/>
+  <dimension ref="A1:D249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,13 +2445,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2459,220 +2459,220 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="B2" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C2" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D2" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>643</v>
+      </c>
+      <c r="D3" t="s">
         <v>652</v>
-      </c>
-      <c r="B3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C3" t="s">
-        <v>653</v>
-      </c>
-      <c r="D3" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B4" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="B5" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="C5" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="D5" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D8" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>675</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>674</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="B12" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="C12" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="D12" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B14" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="B16" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="C16" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="D16" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -2683,178 +2683,178 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="B18" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="B19" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="C19" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="D19" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="B20" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="C20" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="D20" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B21" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="C21" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="D21" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="B22" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C22" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D22" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B23" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="B24" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="C24" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="D24" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="B25" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C25" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="D25" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B26" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B27" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C27" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -2865,248 +2865,248 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="B31" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="C31" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="D31" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="B32" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C32" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="D32" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="B33" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="C33" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="D33" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="B34" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="C34" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="D34" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="B38" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D38" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="B39" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C39" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D39" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="B40" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="C40" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D40" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="B42" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="C42" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D42" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="B43" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="C43" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="D43" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B45" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B46" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="C46" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="D46" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="B47" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="C47" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="D47" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B48" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -3117,374 +3117,374 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="B49" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D49" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B50" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C50" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B51" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D51" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B52" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D52" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="B53" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="C53" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="D53" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="B54" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="C54" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D54" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="B55" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C55" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D55" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="B56" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C56" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B57" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C57" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D57" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B58" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="C58" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D58" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D59" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="B60" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
       <c r="C60" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="D60" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="B61" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="C61" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="D61" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B62" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D62" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B63" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D63" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="B64" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D64" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="B65" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="C65" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="D65" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="B66" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="C66" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="D66" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="B67" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="C67" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="D67" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="B68" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="C68" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="D68" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B69" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="B70" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="C70" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="D70" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="B71" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="C71" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="D71" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="B72" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="C72" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="D72" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="B73" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="C73" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="D73" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B74" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C74" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D74" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C75" t="s">
         <v>9</v>
@@ -3495,122 +3495,122 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="B76" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="C76" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="D76" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B77" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D77" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B78" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C78" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="D78" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B79" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D79" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C80" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="D80" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C81" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D81" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="B82" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="C82" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D82" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B83" t="s">
+        <v>359</v>
+      </c>
+      <c r="C83" t="s">
+        <v>500</v>
+      </c>
+      <c r="D83" t="s">
         <v>368</v>
-      </c>
-      <c r="C83" t="s">
-        <v>509</v>
-      </c>
-      <c r="D83" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C84" t="s">
         <v>14</v>
@@ -3621,296 +3621,296 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B85" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C85" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D85" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B86" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C86" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D86" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B87" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="C87" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="D87" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="B88" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C88" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D88" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B89" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C89" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D89" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C90" t="s">
-        <v>144</v>
+        <v>675</v>
       </c>
       <c r="D90" t="s">
-        <v>159</v>
+        <v>676</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="B91" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="C91" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D91" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B92" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C92" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D92" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B93" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C93" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D93" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B94" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C94" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D94" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B95" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C95" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D95" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="B96" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C96" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D96" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="B97" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="C97" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="D97" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B98" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="C98" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="D98" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C99" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D99" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="B100" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="C100" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="D100" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="B101" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="C101" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="D101" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B102" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C102" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D102" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B103" t="s">
-        <v>518</v>
+        <v>275</v>
       </c>
       <c r="C103" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D103" t="s">
-        <v>229</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>120</v>
+        <v>321</v>
       </c>
       <c r="B104" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C104" t="s">
-        <v>20</v>
+        <v>162</v>
       </c>
       <c r="D104" t="s">
-        <v>68</v>
+        <v>183</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>330</v>
+        <v>108</v>
       </c>
       <c r="B105" t="s">
-        <v>270</v>
+        <v>241</v>
       </c>
       <c r="C105" t="s">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="D105" t="s">
-        <v>189</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -3918,2039 +3918,2025 @@
         <v>111</v>
       </c>
       <c r="B106" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C106" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D106" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>114</v>
+        <v>346</v>
       </c>
       <c r="B107" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="C107" t="s">
-        <v>35</v>
+        <v>223</v>
       </c>
       <c r="D107" t="s">
-        <v>61</v>
+        <v>224</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>355</v>
+        <v>649</v>
       </c>
       <c r="B108" t="s">
-        <v>231</v>
+        <v>651</v>
       </c>
       <c r="C108" t="s">
-        <v>231</v>
+        <v>650</v>
       </c>
       <c r="D108" t="s">
-        <v>232</v>
+        <v>648</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>659</v>
+        <v>336</v>
       </c>
       <c r="B109" t="s">
-        <v>661</v>
+        <v>268</v>
       </c>
       <c r="C109" t="s">
-        <v>660</v>
+        <v>121</v>
       </c>
       <c r="D109" t="s">
-        <v>658</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>345</v>
+        <v>493</v>
       </c>
       <c r="B110" t="s">
-        <v>277</v>
+        <v>489</v>
       </c>
       <c r="C110" t="s">
-        <v>124</v>
+        <v>488</v>
       </c>
       <c r="D110" t="s">
-        <v>214</v>
+        <v>491</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>502</v>
+        <v>114</v>
       </c>
       <c r="B111" t="s">
-        <v>498</v>
+        <v>240</v>
       </c>
       <c r="C111" t="s">
-        <v>497</v>
+        <v>28</v>
       </c>
       <c r="D111" t="s">
-        <v>500</v>
+        <v>63</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>441</v>
       </c>
       <c r="B112" t="s">
-        <v>248</v>
+        <v>436</v>
       </c>
       <c r="C112" t="s">
-        <v>30</v>
+        <v>437</v>
       </c>
       <c r="D112" t="s">
-        <v>65</v>
+        <v>439</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>450</v>
+        <v>467</v>
       </c>
       <c r="B113" t="s">
-        <v>445</v>
+        <v>465</v>
       </c>
       <c r="C113" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="D113" t="s">
-        <v>448</v>
+        <v>454</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>476</v>
+        <v>298</v>
       </c>
       <c r="B114" t="s">
-        <v>474</v>
+        <v>276</v>
       </c>
       <c r="C114" t="s">
-        <v>461</v>
+        <v>142</v>
       </c>
       <c r="D114" t="s">
-        <v>463</v>
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>307</v>
+        <v>79</v>
       </c>
       <c r="B115" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="C115" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D115" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B116" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
       <c r="C116" t="s">
-        <v>152</v>
+        <v>3</v>
       </c>
       <c r="D116" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>82</v>
+        <v>293</v>
       </c>
       <c r="B117" t="s">
-        <v>240</v>
+        <v>272</v>
       </c>
       <c r="C117" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="D117" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>302</v>
+        <v>85</v>
       </c>
       <c r="B118" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="C118" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
       <c r="D118" t="s">
-        <v>137</v>
+        <v>23</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B119" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C119" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="D119" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B120" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="C120" t="s">
-        <v>132</v>
+        <v>18</v>
       </c>
       <c r="D120" t="s">
-        <v>216</v>
+        <v>54</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>110</v>
+        <v>414</v>
       </c>
       <c r="B121" t="s">
-        <v>245</v>
+        <v>417</v>
       </c>
       <c r="C121" t="s">
-        <v>18</v>
+        <v>416</v>
       </c>
       <c r="D121" t="s">
-        <v>56</v>
+        <v>412</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>423</v>
+        <v>345</v>
       </c>
       <c r="B122" t="s">
-        <v>426</v>
+        <v>253</v>
       </c>
       <c r="C122" t="s">
-        <v>425</v>
+        <v>167</v>
       </c>
       <c r="D122" t="s">
-        <v>421</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>354</v>
+        <v>94</v>
       </c>
       <c r="B123" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="C123" t="s">
-        <v>173</v>
+        <v>18</v>
       </c>
       <c r="D123" t="s">
-        <v>228</v>
+        <v>39</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B124" t="s">
-        <v>245</v>
+        <v>449</v>
       </c>
       <c r="C124" t="s">
-        <v>18</v>
+        <v>448</v>
       </c>
       <c r="D124" t="s">
-        <v>41</v>
+        <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B125" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C125" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="D125" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>97</v>
+        <v>440</v>
       </c>
       <c r="B126" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C126" t="s">
-        <v>457</v>
+        <v>437</v>
       </c>
       <c r="D126" t="s">
-        <v>460</v>
+        <v>438</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>449</v>
+        <v>81</v>
       </c>
       <c r="B127" t="s">
-        <v>445</v>
+        <v>236</v>
       </c>
       <c r="C127" t="s">
-        <v>446</v>
+        <v>16</v>
       </c>
       <c r="D127" t="s">
-        <v>447</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>84</v>
+        <v>469</v>
       </c>
       <c r="B128" t="s">
-        <v>244</v>
+        <v>465</v>
       </c>
       <c r="C128" t="s">
-        <v>16</v>
+        <v>452</v>
       </c>
       <c r="D128" t="s">
-        <v>17</v>
+        <v>457</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>478</v>
+        <v>422</v>
       </c>
       <c r="B129" t="s">
-        <v>474</v>
+        <v>419</v>
       </c>
       <c r="C129" t="s">
-        <v>461</v>
+        <v>418</v>
       </c>
       <c r="D129" t="s">
-        <v>466</v>
+        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>431</v>
+        <v>363</v>
       </c>
       <c r="B130" t="s">
-        <v>428</v>
+        <v>359</v>
       </c>
       <c r="C130" t="s">
-        <v>427</v>
+        <v>500</v>
       </c>
       <c r="D130" t="s">
-        <v>429</v>
+        <v>364</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
       <c r="B131" t="s">
-        <v>368</v>
+        <v>258</v>
       </c>
       <c r="C131" t="s">
-        <v>509</v>
+        <v>204</v>
       </c>
       <c r="D131" t="s">
-        <v>373</v>
+        <v>210</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B132" t="s">
-        <v>267</v>
+        <v>553</v>
       </c>
       <c r="C132" t="s">
-        <v>211</v>
+        <v>552</v>
       </c>
       <c r="D132" t="s">
-        <v>217</v>
+        <v>551</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>347</v>
+        <v>390</v>
       </c>
       <c r="B133" t="s">
-        <v>563</v>
+        <v>393</v>
       </c>
       <c r="C133" t="s">
-        <v>562</v>
+        <v>392</v>
       </c>
       <c r="D133" t="s">
-        <v>561</v>
+        <v>388</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>399</v>
+        <v>509</v>
       </c>
       <c r="B134" t="s">
-        <v>402</v>
+        <v>510</v>
       </c>
       <c r="C134" t="s">
-        <v>401</v>
+        <v>511</v>
       </c>
       <c r="D134" t="s">
-        <v>397</v>
+        <v>512</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>519</v>
+        <v>74</v>
       </c>
       <c r="B135" t="s">
-        <v>520</v>
+        <v>231</v>
       </c>
       <c r="C135" t="s">
-        <v>521</v>
+        <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>522</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>77</v>
+        <v>294</v>
       </c>
       <c r="B136" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="C136" t="s">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="D136" t="s">
-        <v>2</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>303</v>
+        <v>429</v>
       </c>
       <c r="B137" t="s">
-        <v>282</v>
+        <v>428</v>
       </c>
       <c r="C137" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
       <c r="D137" t="s">
-        <v>139</v>
+        <v>431</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>438</v>
+        <v>305</v>
       </c>
       <c r="B138" t="s">
-        <v>437</v>
+        <v>252</v>
       </c>
       <c r="C138" t="s">
-        <v>436</v>
+        <v>158</v>
       </c>
       <c r="D138" t="s">
-        <v>440</v>
+        <v>159</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B139" t="s">
-        <v>261</v>
+        <v>653</v>
       </c>
       <c r="C139" t="s">
-        <v>163</v>
+        <v>654</v>
       </c>
       <c r="D139" t="s">
-        <v>164</v>
+        <v>655</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B140" t="s">
-        <v>663</v>
+        <v>428</v>
       </c>
       <c r="C140" t="s">
-        <v>664</v>
+        <v>427</v>
       </c>
       <c r="D140" t="s">
-        <v>665</v>
+        <v>430</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B141" t="s">
-        <v>437</v>
+        <v>465</v>
       </c>
       <c r="C141" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="D141" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>314</v>
+        <v>606</v>
       </c>
       <c r="B142" t="s">
-        <v>474</v>
+        <v>608</v>
       </c>
       <c r="C142" t="s">
-        <v>461</v>
+        <v>609</v>
       </c>
       <c r="D142" t="s">
-        <v>464</v>
+        <v>607</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>616</v>
+        <v>526</v>
       </c>
       <c r="B143" t="s">
-        <v>618</v>
+        <v>527</v>
       </c>
       <c r="C143" t="s">
-        <v>619</v>
+        <v>528</v>
       </c>
       <c r="D143" t="s">
-        <v>617</v>
+        <v>529</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="B144" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="C144" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="D144" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>540</v>
+        <v>86</v>
       </c>
       <c r="B145" t="s">
-        <v>537</v>
+        <v>661</v>
       </c>
       <c r="C145" t="s">
-        <v>538</v>
+        <v>662</v>
       </c>
       <c r="D145" t="s">
-        <v>541</v>
+        <v>660</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>89</v>
+        <v>472</v>
       </c>
       <c r="B146" t="s">
-        <v>671</v>
+        <v>465</v>
       </c>
       <c r="C146" t="s">
-        <v>672</v>
+        <v>452</v>
       </c>
       <c r="D146" t="s">
-        <v>670</v>
+        <v>460</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>481</v>
+        <v>98</v>
       </c>
       <c r="B147" t="s">
-        <v>474</v>
+        <v>242</v>
       </c>
       <c r="C147" t="s">
-        <v>461</v>
+        <v>7</v>
       </c>
       <c r="D147" t="s">
-        <v>469</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>101</v>
+        <v>391</v>
       </c>
       <c r="B148" t="s">
-        <v>250</v>
+        <v>393</v>
       </c>
       <c r="C148" t="s">
-        <v>7</v>
+        <v>392</v>
       </c>
       <c r="D148" t="s">
-        <v>8</v>
+        <v>389</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="B149" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="C149" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="D149" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>393</v>
+        <v>434</v>
       </c>
       <c r="B150" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
       <c r="C150" t="s">
-        <v>395</v>
+        <v>433</v>
       </c>
       <c r="D150" t="s">
-        <v>390</v>
+        <v>432</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>443</v>
+        <v>315</v>
       </c>
       <c r="B151" t="s">
-        <v>444</v>
+        <v>270</v>
       </c>
       <c r="C151" t="s">
-        <v>442</v>
+        <v>125</v>
       </c>
       <c r="D151" t="s">
-        <v>441</v>
+        <v>171</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>324</v>
+        <v>415</v>
       </c>
       <c r="B152" t="s">
-        <v>279</v>
+        <v>417</v>
       </c>
       <c r="C152" t="s">
-        <v>128</v>
+        <v>416</v>
       </c>
       <c r="D152" t="s">
-        <v>177</v>
+        <v>413</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>424</v>
+        <v>352</v>
       </c>
       <c r="B153" t="s">
-        <v>426</v>
+        <v>251</v>
       </c>
       <c r="C153" t="s">
-        <v>425</v>
+        <v>153</v>
       </c>
       <c r="D153" t="s">
-        <v>422</v>
+        <v>220</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B154" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C154" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D154" t="s">
-        <v>227</v>
+        <v>164</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>363</v>
+        <v>487</v>
       </c>
       <c r="B155" t="s">
-        <v>261</v>
+        <v>485</v>
       </c>
       <c r="C155" t="s">
-        <v>163</v>
+        <v>482</v>
       </c>
       <c r="D155" t="s">
-        <v>169</v>
+        <v>484</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>496</v>
+        <v>541</v>
       </c>
       <c r="B156" t="s">
-        <v>494</v>
+        <v>542</v>
       </c>
       <c r="C156" t="s">
-        <v>491</v>
+        <v>543</v>
       </c>
       <c r="D156" t="s">
-        <v>493</v>
+        <v>540</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>551</v>
+        <v>501</v>
       </c>
       <c r="B157" t="s">
-        <v>552</v>
+        <v>502</v>
       </c>
       <c r="C157" t="s">
-        <v>553</v>
+        <v>503</v>
       </c>
       <c r="D157" t="s">
-        <v>550</v>
+        <v>504</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>510</v>
+        <v>623</v>
       </c>
       <c r="B158" t="s">
-        <v>511</v>
+        <v>624</v>
       </c>
       <c r="C158" t="s">
-        <v>512</v>
+        <v>625</v>
       </c>
       <c r="D158" t="s">
-        <v>513</v>
+        <v>622</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>633</v>
+        <v>322</v>
       </c>
       <c r="B159" t="s">
-        <v>634</v>
+        <v>255</v>
       </c>
       <c r="C159" t="s">
-        <v>635</v>
+        <v>185</v>
       </c>
       <c r="D159" t="s">
-        <v>632</v>
+        <v>186</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="B160" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="C160" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D160" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>323</v>
+        <v>497</v>
       </c>
       <c r="B161" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="C161" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="D161" t="s">
-        <v>176</v>
+        <v>495</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="B162" t="s">
-        <v>278</v>
+        <v>510</v>
       </c>
       <c r="C162" t="s">
-        <v>126</v>
+        <v>511</v>
       </c>
       <c r="D162" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>527</v>
+        <v>400</v>
       </c>
       <c r="B163" t="s">
-        <v>520</v>
+        <v>407</v>
       </c>
       <c r="C163" t="s">
-        <v>521</v>
+        <v>406</v>
       </c>
       <c r="D163" t="s">
-        <v>523</v>
+        <v>401</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="B164" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="C164" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
       <c r="D164" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="B165" t="s">
+        <v>407</v>
+      </c>
+      <c r="C165" t="s">
         <v>406</v>
       </c>
-      <c r="C165" t="s">
-        <v>405</v>
-      </c>
       <c r="D165" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>407</v>
+        <v>88</v>
       </c>
       <c r="B166" t="s">
-        <v>416</v>
+        <v>240</v>
       </c>
       <c r="C166" t="s">
-        <v>415</v>
+        <v>28</v>
       </c>
       <c r="D166" t="s">
-        <v>410</v>
+        <v>29</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B167" t="s">
-        <v>248</v>
+        <v>597</v>
       </c>
       <c r="C167" t="s">
-        <v>30</v>
+        <v>596</v>
       </c>
       <c r="D167" t="s">
-        <v>31</v>
+        <v>593</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>91</v>
+        <v>356</v>
       </c>
       <c r="B168" t="s">
-        <v>607</v>
+        <v>251</v>
       </c>
       <c r="C168" t="s">
-        <v>606</v>
+        <v>153</v>
       </c>
       <c r="D168" t="s">
-        <v>603</v>
+        <v>211</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>365</v>
+        <v>473</v>
       </c>
       <c r="B169" t="s">
-        <v>260</v>
+        <v>465</v>
       </c>
       <c r="C169" t="s">
-        <v>157</v>
+        <v>452</v>
       </c>
       <c r="D169" t="s">
-        <v>218</v>
+        <v>461</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="B170" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="C170" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D170" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>475</v>
+        <v>554</v>
       </c>
       <c r="B171" t="s">
-        <v>474</v>
+        <v>553</v>
       </c>
       <c r="C171" t="s">
-        <v>461</v>
+        <v>552</v>
       </c>
       <c r="D171" t="s">
-        <v>462</v>
+        <v>550</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>564</v>
+        <v>349</v>
       </c>
       <c r="B172" t="s">
-        <v>563</v>
+        <v>277</v>
       </c>
       <c r="C172" t="s">
-        <v>562</v>
+        <v>146</v>
       </c>
       <c r="D172" t="s">
-        <v>560</v>
+        <v>147</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>358</v>
+        <v>289</v>
       </c>
       <c r="B173" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="C173" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="D173" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>298</v>
+        <v>100</v>
       </c>
       <c r="B174" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="C174" t="s">
-        <v>72</v>
+        <v>3</v>
       </c>
       <c r="D174" t="s">
-        <v>130</v>
+        <v>35</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>103</v>
+        <v>615</v>
       </c>
       <c r="B175" t="s">
-        <v>240</v>
+        <v>617</v>
       </c>
       <c r="C175" t="s">
-        <v>3</v>
+        <v>616</v>
       </c>
       <c r="D175" t="s">
-        <v>37</v>
+        <v>611</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="B176" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="C176" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="D176" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="B177" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="C177" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="D177" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="B178" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="C178" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="D178" t="s">
-        <v>623</v>
+        <v>637</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>644</v>
+        <v>342</v>
       </c>
       <c r="B179" t="s">
-        <v>646</v>
+        <v>267</v>
       </c>
       <c r="C179" t="s">
-        <v>645</v>
+        <v>70</v>
       </c>
       <c r="D179" t="s">
-        <v>647</v>
+        <v>217</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>351</v>
+        <v>532</v>
       </c>
       <c r="B180" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C180" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="D180" t="s">
-        <v>224</v>
+        <v>533</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>542</v>
+        <v>303</v>
       </c>
       <c r="B181" t="s">
-        <v>291</v>
+        <v>249</v>
       </c>
       <c r="C181" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="D181" t="s">
-        <v>543</v>
+        <v>152</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>312</v>
+        <v>505</v>
       </c>
       <c r="B182" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="C182" t="s">
-        <v>140</v>
+        <v>506</v>
       </c>
       <c r="D182" t="s">
-        <v>156</v>
+        <v>507</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>514</v>
+        <v>316</v>
       </c>
       <c r="B183" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="C183" t="s">
-        <v>515</v>
+        <v>172</v>
       </c>
       <c r="D183" t="s">
-        <v>516</v>
+        <v>173</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B184" t="s">
-        <v>263</v>
+        <v>407</v>
       </c>
       <c r="C184" t="s">
-        <v>178</v>
+        <v>406</v>
       </c>
       <c r="D184" t="s">
-        <v>179</v>
+        <v>404</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>325</v>
+        <v>115</v>
       </c>
       <c r="B185" t="s">
-        <v>416</v>
+        <v>266</v>
       </c>
       <c r="C185" t="s">
-        <v>415</v>
+        <v>52</v>
       </c>
       <c r="D185" t="s">
-        <v>413</v>
+        <v>64</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>118</v>
+        <v>324</v>
       </c>
       <c r="B186" t="s">
         <v>275</v>
       </c>
       <c r="C186" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="D186" t="s">
-        <v>66</v>
+        <v>188</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>333</v>
+        <v>516</v>
       </c>
       <c r="B187" t="s">
-        <v>284</v>
+        <v>510</v>
       </c>
       <c r="C187" t="s">
-        <v>144</v>
+        <v>511</v>
       </c>
       <c r="D187" t="s">
-        <v>194</v>
+        <v>520</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>526</v>
+        <v>670</v>
       </c>
       <c r="B188" t="s">
-        <v>520</v>
+        <v>671</v>
       </c>
       <c r="C188" t="s">
-        <v>521</v>
+        <v>672</v>
       </c>
       <c r="D188" t="s">
-        <v>530</v>
+        <v>673</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B189" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C189" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D189" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B190" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="C190" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="D190" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B191" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C191" t="s">
-        <v>22</v>
+        <v>679</v>
       </c>
       <c r="D191" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>86</v>
+        <v>579</v>
       </c>
       <c r="B192" t="s">
-        <v>251</v>
+        <v>578</v>
       </c>
       <c r="C192" t="s">
-        <v>20</v>
+        <v>576</v>
       </c>
       <c r="D192" t="s">
-        <v>21</v>
+        <v>577</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>589</v>
+        <v>300</v>
       </c>
       <c r="B193" t="s">
-        <v>588</v>
+        <v>248</v>
       </c>
       <c r="C193" t="s">
-        <v>586</v>
+        <v>129</v>
       </c>
       <c r="D193" t="s">
-        <v>587</v>
+        <v>145</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>309</v>
+        <v>402</v>
       </c>
       <c r="B194" t="s">
-        <v>257</v>
+        <v>407</v>
       </c>
       <c r="C194" t="s">
-        <v>132</v>
+        <v>406</v>
       </c>
       <c r="D194" t="s">
-        <v>149</v>
+        <v>403</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>411</v>
+        <v>665</v>
       </c>
       <c r="B195" t="s">
-        <v>416</v>
+        <v>661</v>
       </c>
       <c r="C195" t="s">
-        <v>415</v>
+        <v>662</v>
       </c>
       <c r="D195" t="s">
-        <v>412</v>
+        <v>666</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>675</v>
+        <v>328</v>
       </c>
       <c r="B196" t="s">
-        <v>671</v>
+        <v>283</v>
       </c>
       <c r="C196" t="s">
-        <v>672</v>
+        <v>194</v>
       </c>
       <c r="D196" t="s">
-        <v>676</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>337</v>
+        <v>75</v>
       </c>
       <c r="B197" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
       <c r="C197" t="s">
-        <v>200</v>
+        <v>3</v>
       </c>
       <c r="D197" t="s">
-        <v>201</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>78</v>
+        <v>663</v>
       </c>
       <c r="B198" t="s">
-        <v>240</v>
+        <v>661</v>
       </c>
       <c r="C198" t="s">
-        <v>3</v>
+        <v>662</v>
       </c>
       <c r="D198" t="s">
-        <v>4</v>
+        <v>664</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>673</v>
+        <v>89</v>
       </c>
       <c r="B199" t="s">
-        <v>671</v>
+        <v>30</v>
       </c>
       <c r="C199" t="s">
-        <v>672</v>
+        <v>30</v>
       </c>
       <c r="D199" t="s">
-        <v>674</v>
+        <v>31</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>92</v>
+        <v>309</v>
       </c>
       <c r="B200" t="s">
-        <v>32</v>
+        <v>275</v>
       </c>
       <c r="C200" t="s">
-        <v>32</v>
+        <v>675</v>
       </c>
       <c r="D200" t="s">
-        <v>33</v>
+        <v>677</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>318</v>
+        <v>475</v>
       </c>
       <c r="B201" t="s">
-        <v>284</v>
+        <v>465</v>
       </c>
       <c r="C201" t="s">
-        <v>144</v>
+        <v>452</v>
       </c>
       <c r="D201" t="s">
-        <v>170</v>
+        <v>463</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>484</v>
+        <v>447</v>
       </c>
       <c r="B202" t="s">
-        <v>474</v>
+        <v>443</v>
       </c>
       <c r="C202" t="s">
-        <v>461</v>
+        <v>442</v>
       </c>
       <c r="D202" t="s">
-        <v>472</v>
+        <v>445</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>456</v>
+        <v>560</v>
       </c>
       <c r="B203" t="s">
-        <v>452</v>
+        <v>562</v>
       </c>
       <c r="C203" t="s">
-        <v>451</v>
+        <v>563</v>
       </c>
       <c r="D203" t="s">
-        <v>454</v>
+        <v>564</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>570</v>
+        <v>334</v>
       </c>
       <c r="B204" t="s">
-        <v>572</v>
+        <v>258</v>
       </c>
       <c r="C204" t="s">
-        <v>573</v>
+        <v>204</v>
       </c>
       <c r="D204" t="s">
-        <v>574</v>
+        <v>205</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>343</v>
+        <v>477</v>
       </c>
       <c r="B205" t="s">
-        <v>267</v>
+        <v>481</v>
       </c>
       <c r="C205" t="s">
-        <v>211</v>
+        <v>480</v>
       </c>
       <c r="D205" t="s">
-        <v>212</v>
+        <v>479</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>486</v>
+        <v>317</v>
       </c>
       <c r="B206" t="s">
-        <v>490</v>
+        <v>248</v>
       </c>
       <c r="C206" t="s">
-        <v>489</v>
+        <v>129</v>
       </c>
       <c r="D206" t="s">
-        <v>488</v>
+        <v>174</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>326</v>
+        <v>87</v>
       </c>
       <c r="B207" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C207" t="s">
-        <v>132</v>
+        <v>26</v>
       </c>
       <c r="D207" t="s">
-        <v>180</v>
+        <v>27</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>90</v>
+        <v>308</v>
       </c>
       <c r="B208" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C208" t="s">
-        <v>28</v>
+        <v>162</v>
       </c>
       <c r="D208" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="B209" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="C209" t="s">
-        <v>167</v>
+        <v>675</v>
       </c>
       <c r="D209" t="s">
-        <v>168</v>
+        <v>678</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>340</v>
+        <v>476</v>
       </c>
       <c r="B210" t="s">
-        <v>284</v>
+        <v>465</v>
       </c>
       <c r="C210" t="s">
-        <v>144</v>
+        <v>452</v>
       </c>
       <c r="D210" t="s">
-        <v>205</v>
+        <v>464</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>485</v>
+        <v>93</v>
       </c>
       <c r="B211" t="s">
-        <v>474</v>
+        <v>244</v>
       </c>
       <c r="C211" t="s">
-        <v>461</v>
+        <v>37</v>
       </c>
       <c r="D211" t="s">
-        <v>473</v>
+        <v>38</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>96</v>
+        <v>329</v>
       </c>
       <c r="B212" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="C212" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="D212" t="s">
-        <v>40</v>
+        <v>196</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B213" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C213" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="D213" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>344</v>
+        <v>656</v>
       </c>
       <c r="B214" t="s">
-        <v>285</v>
+        <v>653</v>
       </c>
       <c r="C214" t="s">
-        <v>146</v>
+        <v>654</v>
       </c>
       <c r="D214" t="s">
-        <v>213</v>
+        <v>657</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>666</v>
+        <v>570</v>
       </c>
       <c r="B215" t="s">
-        <v>663</v>
+        <v>572</v>
       </c>
       <c r="C215" t="s">
-        <v>664</v>
+        <v>575</v>
       </c>
       <c r="D215" t="s">
-        <v>667</v>
+        <v>574</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>580</v>
+        <v>327</v>
       </c>
       <c r="B216" t="s">
-        <v>582</v>
+        <v>242</v>
       </c>
       <c r="C216" t="s">
-        <v>585</v>
+        <v>7</v>
       </c>
       <c r="D216" t="s">
-        <v>584</v>
+        <v>193</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>336</v>
+        <v>369</v>
       </c>
       <c r="B217" t="s">
-        <v>250</v>
+        <v>359</v>
       </c>
       <c r="C217" t="s">
-        <v>7</v>
+        <v>500</v>
       </c>
       <c r="D217" t="s">
-        <v>199</v>
+        <v>370</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>378</v>
+        <v>291</v>
       </c>
       <c r="B218" t="s">
-        <v>368</v>
+        <v>248</v>
       </c>
       <c r="C218" t="s">
-        <v>509</v>
+        <v>129</v>
       </c>
       <c r="D218" t="s">
-        <v>379</v>
+        <v>130</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>300</v>
+        <v>470</v>
       </c>
       <c r="B219" t="s">
-        <v>257</v>
+        <v>465</v>
       </c>
       <c r="C219" t="s">
-        <v>132</v>
+        <v>452</v>
       </c>
       <c r="D219" t="s">
-        <v>133</v>
+        <v>458</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>479</v>
+        <v>323</v>
       </c>
       <c r="B220" t="s">
-        <v>474</v>
+        <v>276</v>
       </c>
       <c r="C220" t="s">
-        <v>461</v>
+        <v>142</v>
       </c>
       <c r="D220" t="s">
-        <v>467</v>
+        <v>187</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>332</v>
+        <v>518</v>
       </c>
       <c r="B221" t="s">
-        <v>285</v>
+        <v>510</v>
       </c>
       <c r="C221" t="s">
-        <v>146</v>
+        <v>511</v>
       </c>
       <c r="D221" t="s">
-        <v>193</v>
+        <v>514</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>528</v>
+        <v>103</v>
       </c>
       <c r="B222" t="s">
-        <v>520</v>
+        <v>247</v>
       </c>
       <c r="C222" t="s">
-        <v>521</v>
+        <v>67</v>
       </c>
       <c r="D222" t="s">
-        <v>524</v>
+        <v>191</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B223" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C223" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="D223" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>106</v>
+        <v>341</v>
       </c>
       <c r="B224" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C224" t="s">
-        <v>35</v>
+        <v>215</v>
       </c>
       <c r="D224" t="s">
-        <v>50</v>
+        <v>216</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>350</v>
+        <v>539</v>
       </c>
       <c r="B225" t="s">
-        <v>271</v>
+        <v>535</v>
       </c>
       <c r="C225" t="s">
-        <v>222</v>
+        <v>536</v>
       </c>
       <c r="D225" t="s">
-        <v>223</v>
+        <v>538</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>549</v>
+        <v>101</v>
       </c>
       <c r="B226" t="s">
-        <v>545</v>
+        <v>238</v>
       </c>
       <c r="C226" t="s">
-        <v>546</v>
+        <v>22</v>
       </c>
       <c r="D226" t="s">
-        <v>548</v>
+        <v>40</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B227" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C227" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D227" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>119</v>
+        <v>385</v>
       </c>
       <c r="B228" t="s">
-        <v>245</v>
+        <v>387</v>
       </c>
       <c r="C228" t="s">
-        <v>18</v>
+        <v>386</v>
       </c>
       <c r="D228" t="s">
-        <v>67</v>
+        <v>382</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>394</v>
+        <v>667</v>
       </c>
       <c r="B229" t="s">
-        <v>396</v>
+        <v>661</v>
       </c>
       <c r="C229" t="s">
-        <v>395</v>
+        <v>662</v>
       </c>
       <c r="D229" t="s">
-        <v>391</v>
+        <v>668</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>677</v>
+        <v>313</v>
       </c>
       <c r="B230" t="s">
-        <v>671</v>
+        <v>253</v>
       </c>
       <c r="C230" t="s">
-        <v>672</v>
+        <v>167</v>
       </c>
       <c r="D230" t="s">
-        <v>678</v>
+        <v>168</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="B231" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="C231" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="D231" t="s">
-        <v>174</v>
+        <v>227</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="B232" t="s">
-        <v>281</v>
+        <v>407</v>
       </c>
       <c r="C232" t="s">
-        <v>136</v>
+        <v>406</v>
       </c>
       <c r="D232" t="s">
-        <v>235</v>
+        <v>405</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>356</v>
+        <v>302</v>
       </c>
       <c r="B233" t="s">
-        <v>416</v>
+        <v>269</v>
       </c>
       <c r="C233" t="s">
-        <v>415</v>
+        <v>123</v>
       </c>
       <c r="D233" t="s">
-        <v>414</v>
+        <v>151</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>311</v>
+        <v>92</v>
       </c>
       <c r="B234" t="s">
-        <v>278</v>
+        <v>239</v>
       </c>
       <c r="C234" t="s">
-        <v>126</v>
+        <v>24</v>
       </c>
       <c r="D234" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B235" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="C235" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="D235" t="s">
-        <v>38</v>
+        <v>179</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B236" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C236" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="D236" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B237" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="C237" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="D237" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B238" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="C238" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="D238" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B239" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="C239" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="D239" t="s">
-        <v>23</v>
+        <v>200</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B240" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="C240" t="s">
-        <v>206</v>
+        <v>49</v>
       </c>
       <c r="D240" t="s">
-        <v>207</v>
+        <v>50</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B241" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C241" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D241" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>121</v>
+        <v>585</v>
       </c>
       <c r="B242" t="s">
-        <v>256</v>
+        <v>584</v>
       </c>
       <c r="C242" t="s">
-        <v>69</v>
+        <v>588</v>
       </c>
       <c r="D242" t="s">
-        <v>70</v>
+        <v>586</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="B243" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="C243" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="D243" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>595</v>
+        <v>377</v>
       </c>
       <c r="B244" t="s">
-        <v>594</v>
+        <v>379</v>
       </c>
       <c r="C244" t="s">
-        <v>598</v>
+        <v>378</v>
       </c>
       <c r="D244" t="s">
-        <v>597</v>
+        <v>376</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>386</v>
+        <v>326</v>
       </c>
       <c r="B245" t="s">
-        <v>388</v>
+        <v>250</v>
       </c>
       <c r="C245" t="s">
-        <v>387</v>
+        <v>148</v>
       </c>
       <c r="D245" t="s">
-        <v>385</v>
+        <v>192</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>335</v>
+        <v>492</v>
       </c>
       <c r="B246" t="s">
-        <v>259</v>
+        <v>489</v>
       </c>
       <c r="C246" t="s">
-        <v>152</v>
+        <v>488</v>
       </c>
       <c r="D246" t="s">
-        <v>198</v>
+        <v>490</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>501</v>
+        <v>292</v>
       </c>
       <c r="B247" t="s">
-        <v>498</v>
+        <v>271</v>
       </c>
       <c r="C247" t="s">
-        <v>497</v>
+        <v>131</v>
       </c>
       <c r="D247" t="s">
-        <v>499</v>
+        <v>132</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>301</v>
+        <v>109</v>
       </c>
       <c r="B248" t="s">
-        <v>280</v>
+        <v>238</v>
       </c>
       <c r="C248" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
       <c r="D248" t="s">
-        <v>135</v>
+        <v>56</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>112</v>
+        <v>296</v>
       </c>
       <c r="B249" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
       <c r="C249" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="D249" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>305</v>
-      </c>
-      <c r="B250" t="s">
-        <v>283</v>
-      </c>
-      <c r="C250" t="s">
-        <v>142</v>
-      </c>
-      <c r="D250" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D197" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D204">
-      <sortCondition ref="A1:A197"/>
+  <autoFilter ref="A1:D195" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D202">
+      <sortCondition ref="A1:A195"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D250">
-    <sortCondition ref="A2:A250"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D249">
+    <sortCondition ref="A2:A249"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates through Blue Beetle 2307
</commit_message>
<xml_diff>
--- a/_Biographies.xlsx
+++ b/_Biographies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f94822a51e6e525e/OTRR/otrr-biographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6DF1B16-45A3-4C6F-84B4-FC2FC5762E93}"/>
+  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ACA7106-1531-4E3F-A66C-A5144F1CCC28}"/>
   <bookViews>
-    <workbookView xWindow="-11955" yWindow="-20790" windowWidth="16785" windowHeight="15690" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
+    <workbookView xWindow="-35820" yWindow="-19305" windowWidth="16695" windowHeight="17865" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="686">
   <si>
     <t>File</t>
   </si>
   <si>
-    <t>Box 13 V. 2</t>
-  </si>
-  <si>
     <t>Alan Ladd Biography.pdf</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Lew Ayres Biography.doc</t>
   </si>
   <si>
-    <t>Lionel Barrymore Biography.doc</t>
-  </si>
-  <si>
     <t>Pat Novak for Hire v. 1</t>
   </si>
   <si>
@@ -2077,6 +2071,30 @@
   </si>
   <si>
     <t>Rogues Gallery - OTRR Maintained v. 2211</t>
+  </si>
+  <si>
+    <t>Box 13 - OTRR Maintained v. 2303</t>
+  </si>
+  <si>
+    <t>James Hilton Biography.pdf</t>
+  </si>
+  <si>
+    <t>Hallmark Playhouse</t>
+  </si>
+  <si>
+    <t>Hilton, James</t>
+  </si>
+  <si>
+    <t>Hallmark Playhouse and Hall of Fame - OTRR Maintained v. 2303</t>
+  </si>
+  <si>
+    <t>Lionel Barrymore Biography.pdf</t>
+  </si>
+  <si>
+    <t>Blue Beetle</t>
+  </si>
+  <si>
+    <t>Blue Beetle, The - Maintained 2307</t>
   </si>
 </sst>
 </file>
@@ -2428,30 +2446,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-  <dimension ref="A1:D249"/>
+  <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2459,3474 +2477,3488 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" t="s">
         <v>372</v>
       </c>
-      <c r="B2" t="s">
-        <v>374</v>
-      </c>
       <c r="C2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="B3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D3" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B5" t="s">
         <v>567</v>
       </c>
-      <c r="B5" t="s">
-        <v>569</v>
-      </c>
       <c r="C5" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D5" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
         <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C11" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>624</v>
+      </c>
+      <c r="B12" t="s">
+        <v>627</v>
+      </c>
+      <c r="C12" t="s">
         <v>626</v>
       </c>
-      <c r="B12" t="s">
-        <v>629</v>
-      </c>
-      <c r="C12" t="s">
-        <v>628</v>
-      </c>
       <c r="D12" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>680</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>682</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>683</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="B16" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C16" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D16" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
         <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B18" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" t="s">
         <v>142</v>
-      </c>
-      <c r="D18" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C19" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D19" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B20" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C20" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D20" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B21" t="s">
+        <v>533</v>
+      </c>
+      <c r="C21" t="s">
+        <v>534</v>
+      </c>
+      <c r="D21" t="s">
         <v>535</v>
-      </c>
-      <c r="C21" t="s">
-        <v>536</v>
-      </c>
-      <c r="D21" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>397</v>
+      </c>
+      <c r="B22" t="s">
+        <v>405</v>
+      </c>
+      <c r="C22" t="s">
+        <v>404</v>
+      </c>
+      <c r="D22" t="s">
         <v>399</v>
-      </c>
-      <c r="B22" t="s">
-        <v>407</v>
-      </c>
-      <c r="C22" t="s">
-        <v>406</v>
-      </c>
-      <c r="D22" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B23" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>579</v>
+      </c>
+      <c r="B24" t="s">
+        <v>580</v>
+      </c>
+      <c r="C24" t="s">
         <v>581</v>
       </c>
-      <c r="B24" t="s">
-        <v>582</v>
-      </c>
-      <c r="C24" t="s">
-        <v>583</v>
-      </c>
       <c r="D24" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B25" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C25" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D25" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B27" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C27" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" t="s">
         <v>176</v>
-      </c>
-      <c r="D27" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B28" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
         <v>18</v>
-      </c>
-      <c r="D30" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B31" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C31" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D31" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B32" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C32" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D32" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>559</v>
+      </c>
+      <c r="B33" t="s">
+        <v>560</v>
+      </c>
+      <c r="C33" t="s">
         <v>561</v>
       </c>
-      <c r="B33" t="s">
-        <v>562</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>563</v>
-      </c>
-      <c r="D33" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>612</v>
+      </c>
+      <c r="B34" t="s">
+        <v>615</v>
+      </c>
+      <c r="C34" t="s">
         <v>614</v>
       </c>
-      <c r="B34" t="s">
-        <v>617</v>
-      </c>
-      <c r="C34" t="s">
-        <v>616</v>
-      </c>
       <c r="D34" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B38" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B39" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>407</v>
+      </c>
+      <c r="B40" t="s">
         <v>409</v>
       </c>
-      <c r="B40" t="s">
-        <v>411</v>
-      </c>
       <c r="C40" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D40" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B41" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B42" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C42" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D42" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>616</v>
+      </c>
+      <c r="B43" t="s">
+        <v>619</v>
+      </c>
+      <c r="C43" t="s">
         <v>618</v>
       </c>
-      <c r="B43" t="s">
-        <v>621</v>
-      </c>
-      <c r="C43" t="s">
-        <v>620</v>
-      </c>
       <c r="D43" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
         <v>41</v>
-      </c>
-      <c r="D44" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B46" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C46" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D46" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="B47" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C47" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D47" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
         <v>5</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B49" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B50" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C50" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B51" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B52" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C52" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D52" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>597</v>
+      </c>
+      <c r="B53" t="s">
         <v>599</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>603</v>
+      </c>
+      <c r="D53" t="s">
         <v>601</v>
-      </c>
-      <c r="C53" t="s">
-        <v>605</v>
-      </c>
-      <c r="D53" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B54" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C54" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D54" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B55" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D55" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B56" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C56" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D56" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B57" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C57" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D57" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>371</v>
+      </c>
+      <c r="B58" t="s">
+        <v>372</v>
+      </c>
+      <c r="C58" t="s">
         <v>373</v>
       </c>
-      <c r="B58" t="s">
-        <v>374</v>
-      </c>
-      <c r="C58" t="s">
-        <v>375</v>
-      </c>
       <c r="D58" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B59" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>569</v>
+      </c>
+      <c r="B60" t="s">
+        <v>570</v>
+      </c>
+      <c r="C60" t="s">
+        <v>573</v>
+      </c>
+      <c r="D60" t="s">
         <v>571</v>
-      </c>
-      <c r="B60" t="s">
-        <v>572</v>
-      </c>
-      <c r="C60" t="s">
-        <v>575</v>
-      </c>
-      <c r="D60" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B61" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C61" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D61" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B62" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D62" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D63" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B64" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D64" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B65" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C65" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D65" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>637</v>
+      </c>
+      <c r="B66" t="s">
         <v>639</v>
       </c>
-      <c r="B66" t="s">
-        <v>641</v>
-      </c>
       <c r="C66" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D66" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>628</v>
+      </c>
+      <c r="B67" t="s">
+        <v>629</v>
+      </c>
+      <c r="C67" t="s">
         <v>630</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>631</v>
-      </c>
-      <c r="C67" t="s">
-        <v>632</v>
-      </c>
-      <c r="D67" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>642</v>
+      </c>
+      <c r="B68" t="s">
+        <v>645</v>
+      </c>
+      <c r="C68" t="s">
         <v>644</v>
       </c>
-      <c r="B68" t="s">
-        <v>647</v>
-      </c>
-      <c r="C68" t="s">
-        <v>646</v>
-      </c>
       <c r="D68" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B69" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D69" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>554</v>
+      </c>
+      <c r="B70" t="s">
+        <v>557</v>
+      </c>
+      <c r="C70" t="s">
         <v>556</v>
       </c>
-      <c r="B70" t="s">
-        <v>559</v>
-      </c>
-      <c r="C70" t="s">
-        <v>558</v>
-      </c>
       <c r="D70" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>555</v>
+      </c>
+      <c r="B71" t="s">
         <v>557</v>
       </c>
-      <c r="B71" t="s">
-        <v>559</v>
-      </c>
       <c r="C71" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D71" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B72" t="s">
+        <v>417</v>
+      </c>
+      <c r="C72" t="s">
+        <v>416</v>
+      </c>
+      <c r="D72" t="s">
         <v>419</v>
-      </c>
-      <c r="C72" t="s">
-        <v>418</v>
-      </c>
-      <c r="D72" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B73" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C73" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D73" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B74" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C74" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D74" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
         <v>9</v>
-      </c>
-      <c r="D75" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B76" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C76" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D76" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B77" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D77" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B78" t="s">
+        <v>357</v>
+      </c>
+      <c r="C78" t="s">
+        <v>498</v>
+      </c>
+      <c r="D78" t="s">
         <v>359</v>
-      </c>
-      <c r="C78" t="s">
-        <v>500</v>
-      </c>
-      <c r="D78" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B79" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D79" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C80" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D80" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B81" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C81" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81" t="s">
         <v>33</v>
-      </c>
-      <c r="D81" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B82" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C82" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D82" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B83" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C83" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D83" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" t="s">
         <v>14</v>
-      </c>
-      <c r="D84" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B85" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C85" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D85" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B86" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C86" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D86" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B87" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C87" t="s">
+        <v>440</v>
+      </c>
+      <c r="D87" t="s">
         <v>442</v>
-      </c>
-      <c r="D87" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B88" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C88" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D88" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B89" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C89" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D89" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B90" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C90" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D90" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B91" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C91" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D91" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B92" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C92" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D92" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D93" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B94" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C94" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D94" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B95" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C95" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D95" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B96" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C96" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B97" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C97" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D97" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B98" t="s">
+        <v>519</v>
+      </c>
+      <c r="C98" t="s">
+        <v>520</v>
+      </c>
+      <c r="D98" t="s">
         <v>521</v>
-      </c>
-      <c r="C98" t="s">
-        <v>522</v>
-      </c>
-      <c r="D98" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C99" t="s">
+        <v>23</v>
+      </c>
+      <c r="D99" t="s">
         <v>24</v>
-      </c>
-      <c r="D99" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>476</v>
+      </c>
+      <c r="B100" t="s">
+        <v>479</v>
+      </c>
+      <c r="C100" t="s">
         <v>478</v>
       </c>
-      <c r="B100" t="s">
-        <v>481</v>
-      </c>
-      <c r="C100" t="s">
-        <v>480</v>
-      </c>
       <c r="D100" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B101" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C101" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D101" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B102" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C102" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D102" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B103" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D103" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B104" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C104" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D104" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D105" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B106" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C106" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D106" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B107" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C107" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D107" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>647</v>
+      </c>
+      <c r="B108" t="s">
         <v>649</v>
       </c>
-      <c r="B108" t="s">
-        <v>651</v>
-      </c>
       <c r="C108" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D108" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B109" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C109" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D109" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B110" t="s">
+        <v>487</v>
+      </c>
+      <c r="C110" t="s">
+        <v>486</v>
+      </c>
+      <c r="D110" t="s">
         <v>489</v>
-      </c>
-      <c r="C110" t="s">
-        <v>488</v>
-      </c>
-      <c r="D110" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C111" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D111" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B112" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C112" t="s">
+        <v>435</v>
+      </c>
+      <c r="D112" t="s">
         <v>437</v>
-      </c>
-      <c r="D112" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B113" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C113" t="s">
+        <v>450</v>
+      </c>
+      <c r="D113" t="s">
         <v>452</v>
-      </c>
-      <c r="D113" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B114" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C114" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D114" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B115" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C115" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D115" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B116" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B117" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C117" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D117" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C118" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118" t="s">
         <v>22</v>
-      </c>
-      <c r="D118" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B119" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C119" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D119" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C120" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D120" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>412</v>
+      </c>
+      <c r="B121" t="s">
+        <v>415</v>
+      </c>
+      <c r="C121" t="s">
         <v>414</v>
       </c>
-      <c r="B121" t="s">
-        <v>417</v>
-      </c>
-      <c r="C121" t="s">
-        <v>416</v>
-      </c>
       <c r="D121" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B122" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C122" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D122" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B123" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C123" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D123" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B124" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C124" t="s">
+        <v>446</v>
+      </c>
+      <c r="D124" t="s">
         <v>448</v>
-      </c>
-      <c r="D124" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B125" t="s">
+        <v>447</v>
+      </c>
+      <c r="C125" t="s">
+        <v>446</v>
+      </c>
+      <c r="D125" t="s">
         <v>449</v>
-      </c>
-      <c r="C125" t="s">
-        <v>448</v>
-      </c>
-      <c r="D125" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B126" t="s">
+        <v>434</v>
+      </c>
+      <c r="C126" t="s">
+        <v>435</v>
+      </c>
+      <c r="D126" t="s">
         <v>436</v>
-      </c>
-      <c r="C126" t="s">
-        <v>437</v>
-      </c>
-      <c r="D126" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B127" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C127" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" t="s">
         <v>16</v>
-      </c>
-      <c r="D127" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B128" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C128" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D128" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B129" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C129" t="s">
+        <v>416</v>
+      </c>
+      <c r="D129" t="s">
         <v>418</v>
-      </c>
-      <c r="D129" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B130" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C130" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D130" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B131" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C131" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D131" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B132" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C132" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D132" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>388</v>
+      </c>
+      <c r="B133" t="s">
+        <v>391</v>
+      </c>
+      <c r="C133" t="s">
         <v>390</v>
       </c>
-      <c r="B133" t="s">
-        <v>393</v>
-      </c>
-      <c r="C133" t="s">
-        <v>392</v>
-      </c>
       <c r="D133" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>507</v>
+      </c>
+      <c r="B134" t="s">
+        <v>508</v>
+      </c>
+      <c r="C134" t="s">
         <v>509</v>
       </c>
-      <c r="B134" t="s">
+      <c r="D134" t="s">
         <v>510</v>
-      </c>
-      <c r="C134" t="s">
-        <v>511</v>
-      </c>
-      <c r="D134" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C135" t="s">
+        <v>678</v>
+      </c>
+      <c r="D135" t="s">
         <v>1</v>
-      </c>
-      <c r="D135" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C136" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D136" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>427</v>
+      </c>
+      <c r="B137" t="s">
+        <v>426</v>
+      </c>
+      <c r="C137" t="s">
+        <v>425</v>
+      </c>
+      <c r="D137" t="s">
         <v>429</v>
-      </c>
-      <c r="B137" t="s">
-        <v>428</v>
-      </c>
-      <c r="C137" t="s">
-        <v>427</v>
-      </c>
-      <c r="D137" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B138" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C138" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D138" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B139" t="s">
+        <v>651</v>
+      </c>
+      <c r="C139" t="s">
+        <v>652</v>
+      </c>
+      <c r="D139" t="s">
         <v>653</v>
-      </c>
-      <c r="C139" t="s">
-        <v>654</v>
-      </c>
-      <c r="D139" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B140" t="s">
+        <v>426</v>
+      </c>
+      <c r="C140" t="s">
+        <v>425</v>
+      </c>
+      <c r="D140" t="s">
         <v>428</v>
-      </c>
-      <c r="C140" t="s">
-        <v>427</v>
-      </c>
-      <c r="D140" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B141" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C141" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D141" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>604</v>
+      </c>
+      <c r="B142" t="s">
         <v>606</v>
       </c>
-      <c r="B142" t="s">
-        <v>608</v>
-      </c>
       <c r="C142" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D142" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>524</v>
+      </c>
+      <c r="B143" t="s">
+        <v>525</v>
+      </c>
+      <c r="C143" t="s">
         <v>526</v>
       </c>
-      <c r="B143" t="s">
+      <c r="D143" t="s">
         <v>527</v>
-      </c>
-      <c r="C143" t="s">
-        <v>528</v>
-      </c>
-      <c r="D143" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B144" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C144" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D144" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B145" t="s">
-        <v>661</v>
+        <v>684</v>
       </c>
       <c r="C145" t="s">
-        <v>662</v>
+        <v>685</v>
       </c>
       <c r="D145" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B146" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C146" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D146" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B147" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C147" t="s">
+        <v>6</v>
+      </c>
+      <c r="D147" t="s">
         <v>7</v>
-      </c>
-      <c r="D147" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>389</v>
+      </c>
+      <c r="B148" t="s">
         <v>391</v>
       </c>
-      <c r="B148" t="s">
-        <v>393</v>
-      </c>
       <c r="C148" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D148" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>382</v>
+      </c>
+      <c r="B149" t="s">
+        <v>385</v>
+      </c>
+      <c r="C149" t="s">
         <v>384</v>
       </c>
-      <c r="B149" t="s">
-        <v>387</v>
-      </c>
-      <c r="C149" t="s">
-        <v>386</v>
-      </c>
       <c r="D149" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B150" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C150" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D150" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B151" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C151" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D151" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>413</v>
+      </c>
+      <c r="B152" t="s">
         <v>415</v>
       </c>
-      <c r="B152" t="s">
-        <v>417</v>
-      </c>
       <c r="C152" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D152" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B153" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C153" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D153" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B154" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C154" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D154" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B155" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C155" t="s">
+        <v>480</v>
+      </c>
+      <c r="D155" t="s">
         <v>482</v>
-      </c>
-      <c r="D155" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>539</v>
+      </c>
+      <c r="B156" t="s">
+        <v>540</v>
+      </c>
+      <c r="C156" t="s">
         <v>541</v>
       </c>
-      <c r="B156" t="s">
-        <v>542</v>
-      </c>
-      <c r="C156" t="s">
-        <v>543</v>
-      </c>
       <c r="D156" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>499</v>
+      </c>
+      <c r="B157" t="s">
+        <v>500</v>
+      </c>
+      <c r="C157" t="s">
         <v>501</v>
       </c>
-      <c r="B157" t="s">
+      <c r="D157" t="s">
         <v>502</v>
-      </c>
-      <c r="C157" t="s">
-        <v>503</v>
-      </c>
-      <c r="D157" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>621</v>
+      </c>
+      <c r="B158" t="s">
+        <v>622</v>
+      </c>
+      <c r="C158" t="s">
         <v>623</v>
       </c>
-      <c r="B158" t="s">
-        <v>624</v>
-      </c>
-      <c r="C158" t="s">
-        <v>625</v>
-      </c>
       <c r="D158" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B159" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C159" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D159" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B160" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C160" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D160" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B161" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C161" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D161" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B162" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C162" t="s">
+        <v>509</v>
+      </c>
+      <c r="D162" t="s">
         <v>511</v>
-      </c>
-      <c r="D162" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B163" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C163" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D163" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>393</v>
+      </c>
+      <c r="B164" t="s">
         <v>395</v>
       </c>
-      <c r="B164" t="s">
-        <v>397</v>
-      </c>
       <c r="C164" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D164" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B165" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C165" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D165" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B166" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C166" t="s">
+        <v>27</v>
+      </c>
+      <c r="D166" t="s">
         <v>28</v>
-      </c>
-      <c r="D166" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B167" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C167" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D167" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B168" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C168" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D168" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B169" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C169" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D169" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B170" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C170" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D170" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B171" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C171" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D171" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B172" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C172" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D172" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B173" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C173" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D173" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B174" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C174" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D174" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>613</v>
+      </c>
+      <c r="B175" t="s">
         <v>615</v>
       </c>
-      <c r="B175" t="s">
-        <v>617</v>
-      </c>
       <c r="C175" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D175" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>613</v>
+      </c>
+      <c r="B176" t="s">
         <v>615</v>
       </c>
-      <c r="B176" t="s">
-        <v>617</v>
-      </c>
       <c r="C176" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D176" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>613</v>
+      </c>
+      <c r="B177" t="s">
         <v>615</v>
       </c>
-      <c r="B177" t="s">
-        <v>617</v>
-      </c>
       <c r="C177" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D177" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>632</v>
+      </c>
+      <c r="B178" t="s">
         <v>634</v>
       </c>
-      <c r="B178" t="s">
-        <v>636</v>
-      </c>
       <c r="C178" t="s">
+        <v>633</v>
+      </c>
+      <c r="D178" t="s">
         <v>635</v>
-      </c>
-      <c r="D178" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B179" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C179" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D179" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B180" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C180" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D180" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B181" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C181" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D181" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>503</v>
+      </c>
+      <c r="B182" t="s">
+        <v>276</v>
+      </c>
+      <c r="C182" t="s">
+        <v>504</v>
+      </c>
+      <c r="D182" t="s">
         <v>505</v>
-      </c>
-      <c r="B182" t="s">
-        <v>278</v>
-      </c>
-      <c r="C182" t="s">
-        <v>506</v>
-      </c>
-      <c r="D182" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B183" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C183" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D183" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B184" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C184" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D184" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B185" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C185" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D185" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B186" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C186" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D186" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B187" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C187" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D187" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>668</v>
+      </c>
+      <c r="B188" t="s">
+        <v>669</v>
+      </c>
+      <c r="C188" t="s">
         <v>670</v>
       </c>
-      <c r="B188" t="s">
+      <c r="D188" t="s">
         <v>671</v>
-      </c>
-      <c r="C188" t="s">
-        <v>672</v>
-      </c>
-      <c r="D188" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B189" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C189" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D189" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>356</v>
+      </c>
+      <c r="B190" t="s">
+        <v>357</v>
+      </c>
+      <c r="C190" t="s">
+        <v>498</v>
+      </c>
+      <c r="D190" t="s">
         <v>358</v>
-      </c>
-      <c r="B190" t="s">
-        <v>359</v>
-      </c>
-      <c r="C190" t="s">
-        <v>500</v>
-      </c>
-      <c r="D190" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B191" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C191" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D191" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B192" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C192" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D192" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B193" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C193" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D193" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B194" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C194" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D194" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B195" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C195" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D195" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B196" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C196" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D196" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B197" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C197" t="s">
+        <v>2</v>
+      </c>
+      <c r="D197" t="s">
         <v>3</v>
-      </c>
-      <c r="D197" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B198" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C198" t="s">
+        <v>660</v>
+      </c>
+      <c r="D198" t="s">
         <v>662</v>
-      </c>
-      <c r="D198" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B199" t="s">
+        <v>29</v>
+      </c>
+      <c r="C199" t="s">
+        <v>29</v>
+      </c>
+      <c r="D199" t="s">
         <v>30</v>
-      </c>
-      <c r="C199" t="s">
-        <v>30</v>
-      </c>
-      <c r="D199" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B200" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C200" t="s">
+        <v>673</v>
+      </c>
+      <c r="D200" t="s">
         <v>675</v>
-      </c>
-      <c r="D200" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B201" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C201" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D201" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B202" t="s">
+        <v>441</v>
+      </c>
+      <c r="C202" t="s">
+        <v>440</v>
+      </c>
+      <c r="D202" t="s">
         <v>443</v>
-      </c>
-      <c r="C202" t="s">
-        <v>442</v>
-      </c>
-      <c r="D202" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>558</v>
+      </c>
+      <c r="B203" t="s">
         <v>560</v>
       </c>
-      <c r="B203" t="s">
+      <c r="C203" t="s">
+        <v>561</v>
+      </c>
+      <c r="D203" t="s">
         <v>562</v>
-      </c>
-      <c r="C203" t="s">
-        <v>563</v>
-      </c>
-      <c r="D203" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B204" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C204" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D204" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>475</v>
+      </c>
+      <c r="B205" t="s">
+        <v>479</v>
+      </c>
+      <c r="C205" t="s">
+        <v>478</v>
+      </c>
+      <c r="D205" t="s">
         <v>477</v>
-      </c>
-      <c r="B205" t="s">
-        <v>481</v>
-      </c>
-      <c r="C205" t="s">
-        <v>480</v>
-      </c>
-      <c r="D205" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B206" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C206" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D206" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B207" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C207" t="s">
+        <v>25</v>
+      </c>
+      <c r="D207" t="s">
         <v>26</v>
-      </c>
-      <c r="D207" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B208" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C208" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D208" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B209" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C209" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="D209" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B210" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C210" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D210" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B211" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C211" t="s">
+        <v>36</v>
+      </c>
+      <c r="D211" t="s">
         <v>37</v>
-      </c>
-      <c r="D211" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B212" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C212" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D212" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B213" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C213" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D213" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B214" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C214" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D214" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>568</v>
+      </c>
+      <c r="B215" t="s">
         <v>570</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
+        <v>573</v>
+      </c>
+      <c r="D215" t="s">
         <v>572</v>
-      </c>
-      <c r="C215" t="s">
-        <v>575</v>
-      </c>
-      <c r="D215" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B216" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C216" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D216" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B217" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C217" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D217" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B218" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C218" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D218" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B219" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C219" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D219" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B220" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C220" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D220" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B221" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C221" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D221" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B222" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C222" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D222" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B223" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C223" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D223" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B224" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C224" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D224" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B225" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C225" t="s">
+        <v>534</v>
+      </c>
+      <c r="D225" t="s">
         <v>536</v>
-      </c>
-      <c r="D225" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B226" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C226" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D226" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B227" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C227" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D227" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
+        <v>383</v>
+      </c>
+      <c r="B228" t="s">
         <v>385</v>
       </c>
-      <c r="B228" t="s">
-        <v>387</v>
-      </c>
       <c r="C228" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D228" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B229" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="C229" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D229" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B230" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C230" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D230" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B231" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C231" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D231" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B232" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C232" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D232" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B233" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C233" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D233" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B234" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C234" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D234" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B235" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C235" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D235" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B236" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C236" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D236" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B237" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C237" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D237" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B238" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C238" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D238" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B239" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C239" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D239" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B240" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C240" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D240" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B241" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C241" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D241" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B242" t="s">
+        <v>582</v>
+      </c>
+      <c r="C242" t="s">
+        <v>586</v>
+      </c>
+      <c r="D242" t="s">
         <v>584</v>
-      </c>
-      <c r="C242" t="s">
-        <v>588</v>
-      </c>
-      <c r="D242" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
+        <v>583</v>
+      </c>
+      <c r="B243" t="s">
+        <v>582</v>
+      </c>
+      <c r="C243" t="s">
+        <v>586</v>
+      </c>
+      <c r="D243" t="s">
         <v>585</v>
-      </c>
-      <c r="B243" t="s">
-        <v>584</v>
-      </c>
-      <c r="C243" t="s">
-        <v>588</v>
-      </c>
-      <c r="D243" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
+        <v>375</v>
+      </c>
+      <c r="B244" t="s">
         <v>377</v>
       </c>
-      <c r="B244" t="s">
-        <v>379</v>
-      </c>
       <c r="C244" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D244" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B245" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C245" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D245" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B246" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C246" t="s">
+        <v>486</v>
+      </c>
+      <c r="D246" t="s">
         <v>488</v>
-      </c>
-      <c r="D246" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B247" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C247" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D247" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B248" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C248" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D248" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B249" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C249" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D249" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>681</v>
+      </c>
+      <c r="B250" t="s">
+        <v>680</v>
+      </c>
+      <c r="C250" t="s">
+        <v>682</v>
+      </c>
+      <c r="D250" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates through Have Gun - Will Travel v2308
</commit_message>
<xml_diff>
--- a/_Biographies.xlsx
+++ b/_Biographies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f94822a51e6e525e/OTRR/otrr-biographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="240" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ACA7106-1531-4E3F-A66C-A5144F1CCC28}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BAEC9F0-C945-4E66-9876-3E10B14F25EE}"/>
   <bookViews>
-    <workbookView xWindow="-35820" yWindow="-19305" windowWidth="16695" windowHeight="17865" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
+    <workbookView xWindow="390" yWindow="0" windowWidth="19305" windowHeight="20835" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="688">
   <si>
     <t>File</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Vicki Vola Biography.pdf</t>
   </si>
   <si>
-    <t>Virginia Gregg Biography.pdf</t>
-  </si>
-  <si>
     <t>Strange Wills - OTRR Cert. V.1</t>
   </si>
   <si>
@@ -1968,15 +1965,6 @@
     <t>Dehner, John</t>
   </si>
   <si>
-    <t>John Dehner Biography.pdf</t>
-  </si>
-  <si>
-    <t>Frontier Gentleman - OTRR Maintained v. 2205</t>
-  </si>
-  <si>
-    <t>Frontier Gentleman</t>
-  </si>
-  <si>
     <t>Nick Harris Biography.pdf</t>
   </si>
   <si>
@@ -2095,6 +2083,24 @@
   </si>
   <si>
     <t>Blue Beetle, The - Maintained 2307</t>
+  </si>
+  <si>
+    <t>Have Gun - Will Travel</t>
+  </si>
+  <si>
+    <t>Have Gun - Will Travel - OTRR Maintained v2308</t>
+  </si>
+  <si>
+    <t>John Dehner Biography.docx</t>
+  </si>
+  <si>
+    <t>Virginia Gregg Biography.docx</t>
+  </si>
+  <si>
+    <t>Wright, Ben</t>
+  </si>
+  <si>
+    <t>Ben Wright Biography.docx</t>
   </si>
 </sst>
 </file>
@@ -2147,6 +2153,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2446,11 +2456,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-  <dimension ref="A1:D250"/>
+  <dimension ref="A1:D251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A252" sqref="A252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,13 +2473,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C1" t="s">
-        <v>71</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -2477,66 +2487,66 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" t="s">
         <v>372</v>
       </c>
-      <c r="C2" t="s">
-        <v>373</v>
-      </c>
       <c r="D2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>639</v>
+      </c>
+      <c r="B3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C3" t="s">
         <v>640</v>
       </c>
-      <c r="B3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" t="s">
-        <v>641</v>
-      </c>
       <c r="D3" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>564</v>
+      </c>
+      <c r="B5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" t="s">
         <v>565</v>
       </c>
-      <c r="B5" t="s">
-        <v>567</v>
-      </c>
-      <c r="C5" t="s">
-        <v>566</v>
-      </c>
       <c r="D5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -2547,94 +2557,94 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D11" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>623</v>
+      </c>
+      <c r="B12" t="s">
+        <v>626</v>
+      </c>
+      <c r="C12" t="s">
+        <v>625</v>
+      </c>
+      <c r="D12" t="s">
         <v>624</v>
-      </c>
-      <c r="B12" t="s">
-        <v>627</v>
-      </c>
-      <c r="C12" t="s">
-        <v>626</v>
-      </c>
-      <c r="D12" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C13" t="s">
         <v>58</v>
@@ -2645,52 +2655,52 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C15" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="D15" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C16" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D16" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -2701,178 +2711,178 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C20" t="s">
+        <v>479</v>
+      </c>
+      <c r="D20" t="s">
         <v>480</v>
-      </c>
-      <c r="D20" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B21" t="s">
+        <v>532</v>
+      </c>
+      <c r="C21" t="s">
         <v>533</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>534</v>
-      </c>
-      <c r="D21" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B22" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C22" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D22" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" t="s">
         <v>121</v>
-      </c>
-      <c r="D23" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>578</v>
+      </c>
+      <c r="B24" t="s">
         <v>579</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>580</v>
       </c>
-      <c r="C24" t="s">
-        <v>581</v>
-      </c>
       <c r="D24" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>521</v>
+      </c>
+      <c r="B25" t="s">
+        <v>518</v>
+      </c>
+      <c r="C25" t="s">
+        <v>519</v>
+      </c>
+      <c r="D25" t="s">
         <v>522</v>
-      </c>
-      <c r="B25" t="s">
-        <v>519</v>
-      </c>
-      <c r="C25" t="s">
-        <v>520</v>
-      </c>
-      <c r="D25" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" t="s">
         <v>174</v>
-      </c>
-      <c r="D26" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -2883,66 +2893,66 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B31" t="s">
+        <v>598</v>
+      </c>
+      <c r="C31" t="s">
+        <v>602</v>
+      </c>
+      <c r="D31" t="s">
         <v>599</v>
-      </c>
-      <c r="C31" t="s">
-        <v>603</v>
-      </c>
-      <c r="D31" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>362</v>
+      </c>
+      <c r="B32" t="s">
+        <v>356</v>
+      </c>
+      <c r="C32" t="s">
+        <v>497</v>
+      </c>
+      <c r="D32" t="s">
         <v>363</v>
-      </c>
-      <c r="B32" t="s">
-        <v>357</v>
-      </c>
-      <c r="C32" t="s">
-        <v>498</v>
-      </c>
-      <c r="D32" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>558</v>
+      </c>
+      <c r="B33" t="s">
         <v>559</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>560</v>
       </c>
-      <c r="C33" t="s">
-        <v>561</v>
-      </c>
       <c r="D33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B34" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C34" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D34" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C35" t="s">
         <v>55</v>
@@ -2953,24 +2963,24 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -2981,52 +2991,52 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" t="s">
         <v>153</v>
-      </c>
-      <c r="D39" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>406</v>
+      </c>
+      <c r="B40" t="s">
+        <v>408</v>
+      </c>
+      <c r="C40" t="s">
         <v>407</v>
       </c>
-      <c r="B40" t="s">
-        <v>409</v>
-      </c>
-      <c r="C40" t="s">
-        <v>408</v>
-      </c>
       <c r="D40" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
@@ -3037,38 +3047,38 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B42" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C42" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>615</v>
+      </c>
+      <c r="B43" t="s">
+        <v>618</v>
+      </c>
+      <c r="C43" t="s">
+        <v>617</v>
+      </c>
+      <c r="D43" t="s">
         <v>616</v>
-      </c>
-      <c r="B43" t="s">
-        <v>619</v>
-      </c>
-      <c r="C43" t="s">
-        <v>618</v>
-      </c>
-      <c r="D43" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C44" t="s">
         <v>40</v>
@@ -3079,52 +3089,52 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B45" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B46" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C46" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B47" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C47" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D47" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C48" t="s">
         <v>4</v>
@@ -3135,27 +3145,27 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B50" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C50" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D50" t="s">
         <v>60</v>
@@ -3163,262 +3173,262 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B52" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B53" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C53" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D53" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B54" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C54" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D54" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B55" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D55" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B56" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C56" t="s">
+        <v>225</v>
+      </c>
+      <c r="D56" t="s">
         <v>226</v>
-      </c>
-      <c r="D56" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B57" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C57" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" t="s">
         <v>195</v>
-      </c>
-      <c r="D57" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>370</v>
+      </c>
+      <c r="B58" t="s">
         <v>371</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>372</v>
       </c>
-      <c r="C58" t="s">
-        <v>373</v>
-      </c>
       <c r="D58" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B59" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D59" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>568</v>
+      </c>
+      <c r="B60" t="s">
         <v>569</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>572</v>
+      </c>
+      <c r="D60" t="s">
         <v>570</v>
-      </c>
-      <c r="C60" t="s">
-        <v>573</v>
-      </c>
-      <c r="D60" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B61" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C61" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D61" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C62" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" t="s">
         <v>135</v>
-      </c>
-      <c r="D62" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D64" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B65" t="s">
+        <v>507</v>
+      </c>
+      <c r="C65" t="s">
         <v>508</v>
       </c>
-      <c r="C65" t="s">
-        <v>509</v>
-      </c>
       <c r="D65" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>636</v>
+      </c>
+      <c r="B66" t="s">
+        <v>638</v>
+      </c>
+      <c r="C66" t="s">
         <v>637</v>
       </c>
-      <c r="B66" t="s">
-        <v>639</v>
-      </c>
-      <c r="C66" t="s">
-        <v>638</v>
-      </c>
       <c r="D66" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>627</v>
+      </c>
+      <c r="B67" t="s">
         <v>628</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>629</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>630</v>
-      </c>
-      <c r="D67" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B68" t="s">
-        <v>645</v>
+        <v>682</v>
       </c>
       <c r="C68" t="s">
-        <v>644</v>
+        <v>683</v>
       </c>
       <c r="D68" t="s">
-        <v>643</v>
+        <v>684</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C69" t="s">
         <v>44</v>
@@ -3429,80 +3439,80 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B70" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C70" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D70" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>554</v>
+      </c>
+      <c r="B71" t="s">
+        <v>556</v>
+      </c>
+      <c r="C71" t="s">
         <v>555</v>
       </c>
-      <c r="B71" t="s">
-        <v>557</v>
-      </c>
-      <c r="C71" t="s">
-        <v>556</v>
-      </c>
       <c r="D71" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B72" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C72" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D72" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>597</v>
+      </c>
+      <c r="B73" t="s">
         <v>598</v>
       </c>
-      <c r="B73" t="s">
-        <v>599</v>
-      </c>
       <c r="C73" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D73" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C74" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" t="s">
         <v>123</v>
-      </c>
-      <c r="D74" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C75" t="s">
         <v>8</v>
@@ -3513,69 +3523,69 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B76" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C76" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D76" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B77" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C77" t="s">
+        <v>150</v>
+      </c>
+      <c r="D77" t="s">
         <v>151</v>
-      </c>
-      <c r="D77" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B78" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C78" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D78" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B79" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D79" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C80" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D80" t="s">
         <v>49</v>
@@ -3583,10 +3593,10 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B81" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C81" t="s">
         <v>32</v>
@@ -3597,38 +3607,38 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B82" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C82" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>364</v>
+      </c>
+      <c r="B83" t="s">
+        <v>356</v>
+      </c>
+      <c r="C83" t="s">
+        <v>497</v>
+      </c>
+      <c r="D83" t="s">
         <v>365</v>
-      </c>
-      <c r="B83" t="s">
-        <v>357</v>
-      </c>
-      <c r="C83" t="s">
-        <v>498</v>
-      </c>
-      <c r="D83" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C84" t="s">
         <v>13</v>
@@ -3639,206 +3649,206 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D85" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C86" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D86" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B87" t="s">
+        <v>440</v>
+      </c>
+      <c r="C87" t="s">
+        <v>439</v>
+      </c>
+      <c r="D87" t="s">
         <v>441</v>
-      </c>
-      <c r="C87" t="s">
-        <v>440</v>
-      </c>
-      <c r="D87" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B88" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C88" t="s">
+        <v>118</v>
+      </c>
+      <c r="D88" t="s">
         <v>119</v>
-      </c>
-      <c r="D88" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B89" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C89" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B90" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C90" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D90" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B91" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C91" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D91" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B92" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B93" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D93" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D94" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B95" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C95" t="s">
+        <v>67</v>
+      </c>
+      <c r="D95" t="s">
         <v>68</v>
-      </c>
-      <c r="D95" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B96" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C96" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D96" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B97" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C97" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D97" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B98" t="s">
+        <v>518</v>
+      </c>
+      <c r="C98" t="s">
         <v>519</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>520</v>
-      </c>
-      <c r="D98" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C99" t="s">
         <v>23</v>
@@ -3849,80 +3859,80 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>475</v>
+      </c>
+      <c r="B100" t="s">
+        <v>478</v>
+      </c>
+      <c r="C100" t="s">
+        <v>477</v>
+      </c>
+      <c r="D100" t="s">
         <v>476</v>
-      </c>
-      <c r="B100" t="s">
-        <v>479</v>
-      </c>
-      <c r="C100" t="s">
-        <v>478</v>
-      </c>
-      <c r="D100" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B101" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C101" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D101" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B102" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C102" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D102" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B103" t="s">
-        <v>273</v>
+        <v>682</v>
       </c>
       <c r="C103" t="s">
-        <v>139</v>
+        <v>683</v>
       </c>
       <c r="D103" t="s">
-        <v>64</v>
+        <v>685</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C104" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D104" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C105" t="s">
         <v>40</v>
@@ -3933,10 +3943,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C106" t="s">
         <v>32</v>
@@ -3947,66 +3957,66 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B107" t="s">
+        <v>220</v>
+      </c>
+      <c r="C107" t="s">
+        <v>220</v>
+      </c>
+      <c r="D107" t="s">
         <v>221</v>
-      </c>
-      <c r="C107" t="s">
-        <v>221</v>
-      </c>
-      <c r="D107" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B108" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C108" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D108" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B109" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C109" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D109" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B110" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C110" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D110" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C111" t="s">
         <v>27</v>
@@ -4017,66 +4027,66 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B112" t="s">
+        <v>433</v>
+      </c>
+      <c r="C112" t="s">
         <v>434</v>
       </c>
-      <c r="C112" t="s">
-        <v>435</v>
-      </c>
       <c r="D112" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B113" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C113" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D113" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B114" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C114" t="s">
+        <v>139</v>
+      </c>
+      <c r="D114" t="s">
         <v>140</v>
-      </c>
-      <c r="D114" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B115" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C115" t="s">
+        <v>145</v>
+      </c>
+      <c r="D115" t="s">
         <v>146</v>
-      </c>
-      <c r="D115" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C116" t="s">
         <v>2</v>
@@ -4087,24 +4097,24 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B117" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C117" t="s">
+        <v>130</v>
+      </c>
+      <c r="D117" t="s">
         <v>131</v>
-      </c>
-      <c r="D117" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B118" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C118" t="s">
         <v>21</v>
@@ -4115,24 +4125,24 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C119" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D119" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C120" t="s">
         <v>17</v>
@@ -4143,38 +4153,38 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B121" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C121" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D121" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B122" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C122" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D122" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B123" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C123" t="s">
         <v>17</v>
@@ -4185,52 +4195,52 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B124" t="s">
+        <v>446</v>
+      </c>
+      <c r="C124" t="s">
+        <v>445</v>
+      </c>
+      <c r="D124" t="s">
         <v>447</v>
-      </c>
-      <c r="C124" t="s">
-        <v>446</v>
-      </c>
-      <c r="D124" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B125" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C125" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D125" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B126" t="s">
+        <v>433</v>
+      </c>
+      <c r="C126" t="s">
         <v>434</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>435</v>
-      </c>
-      <c r="D126" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B127" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C127" t="s">
         <v>15</v>
@@ -4241,111 +4251,111 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B128" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C128" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D128" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B129" t="s">
+        <v>416</v>
+      </c>
+      <c r="C129" t="s">
+        <v>415</v>
+      </c>
+      <c r="D129" t="s">
         <v>417</v>
-      </c>
-      <c r="C129" t="s">
-        <v>416</v>
-      </c>
-      <c r="D129" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>360</v>
+      </c>
+      <c r="B130" t="s">
+        <v>356</v>
+      </c>
+      <c r="C130" t="s">
+        <v>497</v>
+      </c>
+      <c r="D130" t="s">
         <v>361</v>
-      </c>
-      <c r="B130" t="s">
-        <v>357</v>
-      </c>
-      <c r="C130" t="s">
-        <v>498</v>
-      </c>
-      <c r="D130" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B131" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C131" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D131" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B132" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C132" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D132" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B133" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C133" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D133" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>506</v>
+      </c>
+      <c r="B134" t="s">
         <v>507</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>508</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>509</v>
-      </c>
-      <c r="D134" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B135" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C135" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="D135" t="s">
         <v>1</v>
@@ -4353,164 +4363,164 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B136" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C136" t="s">
+        <v>132</v>
+      </c>
+      <c r="D136" t="s">
         <v>133</v>
-      </c>
-      <c r="D136" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B137" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C137" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D137" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B138" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C138" t="s">
+        <v>155</v>
+      </c>
+      <c r="D138" t="s">
         <v>156</v>
-      </c>
-      <c r="D138" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B139" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C139" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D139" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B140" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C140" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D140" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B141" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C141" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D141" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>603</v>
+      </c>
+      <c r="B142" t="s">
+        <v>605</v>
+      </c>
+      <c r="C142" t="s">
+        <v>606</v>
+      </c>
+      <c r="D142" t="s">
         <v>604</v>
-      </c>
-      <c r="B142" t="s">
-        <v>606</v>
-      </c>
-      <c r="C142" t="s">
-        <v>607</v>
-      </c>
-      <c r="D142" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>523</v>
+      </c>
+      <c r="B143" t="s">
         <v>524</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>525</v>
       </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
         <v>526</v>
-      </c>
-      <c r="D143" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>527</v>
+      </c>
+      <c r="B144" t="s">
+        <v>524</v>
+      </c>
+      <c r="C144" t="s">
+        <v>525</v>
+      </c>
+      <c r="D144" t="s">
         <v>528</v>
-      </c>
-      <c r="B144" t="s">
-        <v>525</v>
-      </c>
-      <c r="C144" t="s">
-        <v>526</v>
-      </c>
-      <c r="D144" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B145" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C145" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="D145" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B146" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C146" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D146" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B147" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C147" t="s">
         <v>6</v>
@@ -4521,262 +4531,262 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>388</v>
+      </c>
+      <c r="B148" t="s">
+        <v>390</v>
+      </c>
+      <c r="C148" t="s">
         <v>389</v>
       </c>
-      <c r="B148" t="s">
-        <v>391</v>
-      </c>
-      <c r="C148" t="s">
-        <v>390</v>
-      </c>
       <c r="D148" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B149" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C149" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D149" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>431</v>
+      </c>
+      <c r="B150" t="s">
         <v>432</v>
       </c>
-      <c r="B150" t="s">
-        <v>433</v>
-      </c>
       <c r="C150" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D150" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B151" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C151" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D151" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>412</v>
+      </c>
+      <c r="B152" t="s">
+        <v>414</v>
+      </c>
+      <c r="C152" t="s">
         <v>413</v>
       </c>
-      <c r="B152" t="s">
-        <v>415</v>
-      </c>
-      <c r="C152" t="s">
-        <v>414</v>
-      </c>
       <c r="D152" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B153" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C153" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D153" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B154" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C154" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D154" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B155" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C155" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D155" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>538</v>
+      </c>
+      <c r="B156" t="s">
         <v>539</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" t="s">
         <v>540</v>
       </c>
-      <c r="C156" t="s">
-        <v>541</v>
-      </c>
       <c r="D156" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>498</v>
+      </c>
+      <c r="B157" t="s">
         <v>499</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>500</v>
       </c>
-      <c r="C157" t="s">
+      <c r="D157" t="s">
         <v>501</v>
-      </c>
-      <c r="D157" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>620</v>
+      </c>
+      <c r="B158" t="s">
         <v>621</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>622</v>
       </c>
-      <c r="C158" t="s">
-        <v>623</v>
-      </c>
       <c r="D158" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B159" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C159" t="s">
+        <v>182</v>
+      </c>
+      <c r="D159" t="s">
         <v>183</v>
-      </c>
-      <c r="D159" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B160" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C160" t="s">
+        <v>166</v>
+      </c>
+      <c r="D160" t="s">
         <v>167</v>
-      </c>
-      <c r="D160" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B161" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C161" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D161" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B162" t="s">
+        <v>507</v>
+      </c>
+      <c r="C162" t="s">
         <v>508</v>
       </c>
-      <c r="C162" t="s">
-        <v>509</v>
-      </c>
       <c r="D162" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>397</v>
+      </c>
+      <c r="B163" t="s">
+        <v>404</v>
+      </c>
+      <c r="C163" t="s">
+        <v>403</v>
+      </c>
+      <c r="D163" t="s">
         <v>398</v>
-      </c>
-      <c r="B163" t="s">
-        <v>405</v>
-      </c>
-      <c r="C163" t="s">
-        <v>404</v>
-      </c>
-      <c r="D163" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>392</v>
+      </c>
+      <c r="B164" t="s">
+        <v>394</v>
+      </c>
+      <c r="C164" t="s">
         <v>393</v>
       </c>
-      <c r="B164" t="s">
-        <v>395</v>
-      </c>
-      <c r="C164" t="s">
-        <v>394</v>
-      </c>
       <c r="D164" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B165" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C165" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D165" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B166" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C166" t="s">
         <v>27</v>
@@ -4787,108 +4797,108 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B167" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C167" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D167" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B168" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C168" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D168" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B169" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C169" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D169" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B170" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C170" t="s">
+        <v>449</v>
+      </c>
+      <c r="D170" t="s">
         <v>450</v>
-      </c>
-      <c r="D170" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B171" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C171" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D171" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B172" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C172" t="s">
+        <v>143</v>
+      </c>
+      <c r="D172" t="s">
         <v>144</v>
-      </c>
-      <c r="D172" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B173" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C173" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D173" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B174" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C174" t="s">
         <v>2</v>
@@ -4899,150 +4909,150 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>612</v>
+      </c>
+      <c r="B175" t="s">
+        <v>614</v>
+      </c>
+      <c r="C175" t="s">
         <v>613</v>
       </c>
-      <c r="B175" t="s">
-        <v>615</v>
-      </c>
-      <c r="C175" t="s">
-        <v>614</v>
-      </c>
       <c r="D175" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>612</v>
+      </c>
+      <c r="B176" t="s">
+        <v>614</v>
+      </c>
+      <c r="C176" t="s">
         <v>613</v>
       </c>
-      <c r="B176" t="s">
-        <v>615</v>
-      </c>
-      <c r="C176" t="s">
-        <v>614</v>
-      </c>
       <c r="D176" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>612</v>
+      </c>
+      <c r="B177" t="s">
+        <v>614</v>
+      </c>
+      <c r="C177" t="s">
         <v>613</v>
       </c>
-      <c r="B177" t="s">
-        <v>615</v>
-      </c>
-      <c r="C177" t="s">
-        <v>614</v>
-      </c>
       <c r="D177" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>631</v>
+      </c>
+      <c r="B178" t="s">
+        <v>633</v>
+      </c>
+      <c r="C178" t="s">
         <v>632</v>
       </c>
-      <c r="B178" t="s">
+      <c r="D178" t="s">
         <v>634</v>
-      </c>
-      <c r="C178" t="s">
-        <v>633</v>
-      </c>
-      <c r="D178" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B179" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C179" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D179" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B180" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C180" t="s">
         <v>44</v>
       </c>
       <c r="D180" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B181" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C181" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D181" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>502</v>
+      </c>
+      <c r="B182" t="s">
+        <v>275</v>
+      </c>
+      <c r="C182" t="s">
         <v>503</v>
       </c>
-      <c r="B182" t="s">
-        <v>276</v>
-      </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>504</v>
-      </c>
-      <c r="D182" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B183" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C183" t="s">
+        <v>169</v>
+      </c>
+      <c r="D183" t="s">
         <v>170</v>
-      </c>
-      <c r="D183" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B184" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C184" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D184" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B185" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C185" t="s">
         <v>50</v>
@@ -5053,83 +5063,83 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B186" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C186" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D186" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B187" t="s">
+        <v>507</v>
+      </c>
+      <c r="C187" t="s">
         <v>508</v>
       </c>
-      <c r="C187" t="s">
-        <v>509</v>
-      </c>
       <c r="D187" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B188" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C188" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D188" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B189" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C189" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D189" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>355</v>
+      </c>
+      <c r="B190" t="s">
         <v>356</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" t="s">
+        <v>497</v>
+      </c>
+      <c r="D190" t="s">
         <v>357</v>
-      </c>
-      <c r="C190" t="s">
-        <v>498</v>
-      </c>
-      <c r="D190" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B191" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C191" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D191" t="s">
         <v>19</v>
@@ -5137,80 +5147,80 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B192" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C192" t="s">
+        <v>573</v>
+      </c>
+      <c r="D192" t="s">
         <v>574</v>
-      </c>
-      <c r="D192" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B193" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C193" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D193" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>399</v>
+      </c>
+      <c r="B194" t="s">
+        <v>404</v>
+      </c>
+      <c r="C194" t="s">
+        <v>403</v>
+      </c>
+      <c r="D194" t="s">
         <v>400</v>
-      </c>
-      <c r="B194" t="s">
-        <v>405</v>
-      </c>
-      <c r="C194" t="s">
-        <v>404</v>
-      </c>
-      <c r="D194" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B195" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C195" t="s">
+        <v>656</v>
+      </c>
+      <c r="D195" t="s">
         <v>660</v>
-      </c>
-      <c r="D195" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B196" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C196" t="s">
+        <v>191</v>
+      </c>
+      <c r="D196" t="s">
         <v>192</v>
-      </c>
-      <c r="D196" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B197" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C197" t="s">
         <v>2</v>
@@ -5221,21 +5231,21 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B198" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C198" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D198" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B199" t="s">
         <v>29</v>
@@ -5249,108 +5259,108 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B200" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C200" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D200" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B201" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C201" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D201" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B202" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C202" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D202" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B203" t="s">
+        <v>559</v>
+      </c>
+      <c r="C203" t="s">
         <v>560</v>
       </c>
-      <c r="C203" t="s">
+      <c r="D203" t="s">
         <v>561</v>
-      </c>
-      <c r="D203" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B204" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C204" t="s">
+        <v>201</v>
+      </c>
+      <c r="D204" t="s">
         <v>202</v>
-      </c>
-      <c r="D204" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B205" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C205" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D205" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B206" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C206" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D206" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B207" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C207" t="s">
         <v>25</v>
@@ -5361,52 +5371,52 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B208" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C208" t="s">
+        <v>159</v>
+      </c>
+      <c r="D208" t="s">
         <v>160</v>
-      </c>
-      <c r="D208" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B209" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C209" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D209" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B210" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C210" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D210" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B211" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C211" t="s">
         <v>36</v>
@@ -5417,164 +5427,164 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B212" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C212" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D212" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B213" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C213" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D213" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B214" t="s">
+        <v>647</v>
+      </c>
+      <c r="C214" t="s">
+        <v>648</v>
+      </c>
+      <c r="D214" t="s">
         <v>651</v>
-      </c>
-      <c r="C214" t="s">
-        <v>652</v>
-      </c>
-      <c r="D214" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B215" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C215" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D215" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B216" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C216" t="s">
         <v>6</v>
       </c>
       <c r="D216" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
+        <v>366</v>
+      </c>
+      <c r="B217" t="s">
+        <v>356</v>
+      </c>
+      <c r="C217" t="s">
+        <v>497</v>
+      </c>
+      <c r="D217" t="s">
         <v>367</v>
-      </c>
-      <c r="B217" t="s">
-        <v>357</v>
-      </c>
-      <c r="C217" t="s">
-        <v>498</v>
-      </c>
-      <c r="D217" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B218" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C218" t="s">
+        <v>126</v>
+      </c>
+      <c r="D218" t="s">
         <v>127</v>
-      </c>
-      <c r="D218" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B219" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C219" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D219" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B220" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C220" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D220" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B221" t="s">
+        <v>507</v>
+      </c>
+      <c r="C221" t="s">
         <v>508</v>
       </c>
-      <c r="C221" t="s">
-        <v>509</v>
-      </c>
       <c r="D221" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B222" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C222" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D222" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B223" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C223" t="s">
         <v>32</v>
@@ -5585,38 +5595,38 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B224" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C224" t="s">
+        <v>212</v>
+      </c>
+      <c r="D224" t="s">
         <v>213</v>
-      </c>
-      <c r="D224" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B225" t="s">
+        <v>532</v>
+      </c>
+      <c r="C225" t="s">
         <v>533</v>
       </c>
-      <c r="C225" t="s">
-        <v>534</v>
-      </c>
       <c r="D225" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B226" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C226" t="s">
         <v>21</v>
@@ -5627,10 +5637,10 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B227" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C227" t="s">
         <v>17</v>
@@ -5641,94 +5651,94 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
+        <v>382</v>
+      </c>
+      <c r="B228" t="s">
+        <v>384</v>
+      </c>
+      <c r="C228" t="s">
         <v>383</v>
       </c>
-      <c r="B228" t="s">
-        <v>385</v>
-      </c>
-      <c r="C228" t="s">
-        <v>384</v>
-      </c>
       <c r="D228" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B229" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C229" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="D229" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B230" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C230" t="s">
+        <v>164</v>
+      </c>
+      <c r="D230" t="s">
         <v>165</v>
-      </c>
-      <c r="D230" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B231" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C231" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D231" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B232" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C232" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D232" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B233" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C233" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D233" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B234" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C234" t="s">
         <v>23</v>
@@ -5739,52 +5749,52 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B235" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C235" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D235" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B236" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C236" t="s">
         <v>44</v>
       </c>
       <c r="D236" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B237" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C237" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D237" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B238" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C238" t="s">
         <v>17</v>
@@ -5795,24 +5805,24 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B239" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C239" t="s">
+        <v>196</v>
+      </c>
+      <c r="D239" t="s">
         <v>197</v>
-      </c>
-      <c r="D239" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B240" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C240" t="s">
         <v>47</v>
@@ -5823,108 +5833,108 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B241" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C241" t="s">
+        <v>64</v>
+      </c>
+      <c r="D241" t="s">
         <v>65</v>
-      </c>
-      <c r="D241" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
+        <v>582</v>
+      </c>
+      <c r="B242" t="s">
+        <v>581</v>
+      </c>
+      <c r="C242" t="s">
+        <v>585</v>
+      </c>
+      <c r="D242" t="s">
         <v>583</v>
-      </c>
-      <c r="B242" t="s">
-        <v>582</v>
-      </c>
-      <c r="C242" t="s">
-        <v>586</v>
-      </c>
-      <c r="D242" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B243" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C243" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D243" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
+        <v>374</v>
+      </c>
+      <c r="B244" t="s">
+        <v>376</v>
+      </c>
+      <c r="C244" t="s">
         <v>375</v>
       </c>
-      <c r="B244" t="s">
-        <v>377</v>
-      </c>
-      <c r="C244" t="s">
-        <v>376</v>
-      </c>
       <c r="D244" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B245" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C245" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D245" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B246" t="s">
+        <v>486</v>
+      </c>
+      <c r="C246" t="s">
+        <v>485</v>
+      </c>
+      <c r="D246" t="s">
         <v>487</v>
-      </c>
-      <c r="C246" t="s">
-        <v>486</v>
-      </c>
-      <c r="D246" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B247" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C247" t="s">
+        <v>128</v>
+      </c>
+      <c r="D247" t="s">
         <v>129</v>
-      </c>
-      <c r="D247" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B248" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C248" t="s">
         <v>21</v>
@@ -5935,30 +5945,44 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B249" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C249" t="s">
+        <v>136</v>
+      </c>
+      <c r="D249" t="s">
         <v>137</v>
-      </c>
-      <c r="D249" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="B250" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C250" t="s">
+        <v>678</v>
+      </c>
+      <c r="D250" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>686</v>
+      </c>
+      <c r="B251" t="s">
         <v>682</v>
       </c>
-      <c r="D250" t="s">
-        <v>679</v>
+      <c r="C251" t="s">
+        <v>683</v>
+      </c>
+      <c r="D251" t="s">
+        <v>687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bios through Ceiling Unlimited/Exploring Tomorrow
</commit_message>
<xml_diff>
--- a/_Biographies.xlsx
+++ b/_Biographies.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f94822a51e6e525e/OTRR/otrr-biographies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BAEC9F0-C945-4E66-9876-3E10B14F25EE}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{52FA0880-62CD-47D4-BB54-726011D8F962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BD93F64-CEFC-4303-9F0A-BDFCC43FACB1}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="0" windowWidth="19305" windowHeight="20835" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
+    <workbookView xWindow="-50340" yWindow="-21525" windowWidth="38550" windowHeight="20835" xr2:uid="{A807F244-7AAE-4344-B02D-A5956FDF1E7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$196</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="698">
   <si>
     <t>File</t>
   </si>
@@ -2101,6 +2101,36 @@
   </si>
   <si>
     <t>Ben Wright Biography.docx</t>
+  </si>
+  <si>
+    <t>Challenge of the Yukon</t>
+  </si>
+  <si>
+    <t>Ceiling Unlimited</t>
+  </si>
+  <si>
+    <t>Ceiling Unlimited - OTRR v2409</t>
+  </si>
+  <si>
+    <t>Orson Wells Biography.pdf</t>
+  </si>
+  <si>
+    <t>Silverberg, Robert</t>
+  </si>
+  <si>
+    <t>Exploring Tomorrow</t>
+  </si>
+  <si>
+    <t>Exploring Tomorrow - OTRR v. 24xx</t>
+  </si>
+  <si>
+    <t>Robert Silverberg Biography.docx</t>
+  </si>
+  <si>
+    <t>Campbell Jr., John W.</t>
+  </si>
+  <si>
+    <t>John Campbell Jr. Biography.docx</t>
   </si>
 </sst>
 </file>
@@ -2160,9 +2190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2200,7 +2230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2306,7 +2336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2448,7 +2478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2456,11 +2486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-  <dimension ref="A1:D251"/>
+  <dimension ref="A1:D254"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A252" sqref="A252"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,142 +3077,142 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>465</v>
+        <v>696</v>
       </c>
       <c r="B42" t="s">
-        <v>462</v>
+        <v>693</v>
       </c>
       <c r="C42" t="s">
-        <v>449</v>
+        <v>694</v>
       </c>
       <c r="D42" t="s">
-        <v>453</v>
+        <v>697</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>615</v>
+        <v>465</v>
       </c>
       <c r="B43" t="s">
-        <v>618</v>
+        <v>462</v>
       </c>
       <c r="C43" t="s">
-        <v>617</v>
+        <v>449</v>
       </c>
       <c r="D43" t="s">
-        <v>616</v>
+        <v>453</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>615</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>618</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>617</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>616</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>298</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>271</v>
+        <v>238</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>423</v>
+        <v>298</v>
       </c>
       <c r="B46" t="s">
-        <v>422</v>
+        <v>271</v>
       </c>
       <c r="C46" t="s">
-        <v>421</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>531</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>546</v>
+        <v>423</v>
       </c>
       <c r="B47" t="s">
-        <v>544</v>
+        <v>422</v>
       </c>
       <c r="C47" t="s">
-        <v>543</v>
+        <v>421</v>
       </c>
       <c r="D47" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>546</v>
       </c>
       <c r="B48" t="s">
-        <v>230</v>
+        <v>544</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>543</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>542</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>341</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="C49" t="s">
-        <v>126</v>
+        <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>216</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>110</v>
+        <v>341</v>
       </c>
       <c r="B50" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="C50" t="s">
-        <v>505</v>
+        <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>337</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>505</v>
       </c>
       <c r="D51" t="s">
-        <v>210</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3196,35 +3226,35 @@
         <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>596</v>
+        <v>337</v>
       </c>
       <c r="B53" t="s">
-        <v>598</v>
+        <v>269</v>
       </c>
       <c r="C53" t="s">
-        <v>602</v>
+        <v>130</v>
       </c>
       <c r="D53" t="s">
-        <v>600</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>471</v>
+        <v>596</v>
       </c>
       <c r="B54" t="s">
-        <v>462</v>
+        <v>598</v>
       </c>
       <c r="C54" t="s">
-        <v>449</v>
+        <v>602</v>
       </c>
       <c r="D54" t="s">
-        <v>459</v>
+        <v>600</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3232,228 +3262,228 @@
         <v>471</v>
       </c>
       <c r="B55" t="s">
-        <v>266</v>
+        <v>462</v>
       </c>
       <c r="C55" t="s">
-        <v>120</v>
+        <v>449</v>
       </c>
       <c r="D55" t="s">
-        <v>663</v>
+        <v>459</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>345</v>
+        <v>471</v>
       </c>
       <c r="B56" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="C56" t="s">
-        <v>225</v>
+        <v>120</v>
       </c>
       <c r="D56" t="s">
-        <v>226</v>
+        <v>663</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="B57" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C57" t="s">
-        <v>194</v>
+        <v>225</v>
       </c>
       <c r="D57" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="B58" t="s">
-        <v>371</v>
+        <v>281</v>
       </c>
       <c r="C58" t="s">
-        <v>372</v>
+        <v>194</v>
       </c>
       <c r="D58" t="s">
-        <v>368</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>340</v>
+        <v>370</v>
       </c>
       <c r="B59" t="s">
-        <v>246</v>
+        <v>371</v>
       </c>
       <c r="C59" t="s">
-        <v>134</v>
+        <v>372</v>
       </c>
       <c r="D59" t="s">
-        <v>215</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>568</v>
+        <v>340</v>
       </c>
       <c r="B60" t="s">
-        <v>569</v>
+        <v>246</v>
       </c>
       <c r="C60" t="s">
-        <v>572</v>
+        <v>134</v>
       </c>
       <c r="D60" t="s">
-        <v>570</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>545</v>
+        <v>568</v>
       </c>
       <c r="B61" t="s">
-        <v>544</v>
+        <v>569</v>
       </c>
       <c r="C61" t="s">
-        <v>543</v>
+        <v>572</v>
       </c>
       <c r="D61" t="s">
-        <v>541</v>
+        <v>570</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>292</v>
+        <v>545</v>
       </c>
       <c r="B62" t="s">
-        <v>246</v>
+        <v>544</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
+        <v>543</v>
       </c>
       <c r="D62" t="s">
-        <v>135</v>
+        <v>541</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>315</v>
+        <v>292</v>
       </c>
       <c r="B63" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="D63" t="s">
-        <v>172</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>495</v>
+        <v>315</v>
       </c>
       <c r="B64" t="s">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>493</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="B65" t="s">
-        <v>507</v>
+        <v>266</v>
       </c>
       <c r="C65" t="s">
-        <v>508</v>
+        <v>120</v>
       </c>
       <c r="D65" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>636</v>
+        <v>516</v>
       </c>
       <c r="B66" t="s">
-        <v>638</v>
+        <v>507</v>
       </c>
       <c r="C66" t="s">
-        <v>637</v>
+        <v>508</v>
       </c>
       <c r="D66" t="s">
-        <v>635</v>
+        <v>512</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="B67" t="s">
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="C67" t="s">
-        <v>629</v>
+        <v>637</v>
       </c>
       <c r="D67" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="B68" t="s">
-        <v>682</v>
+        <v>628</v>
       </c>
       <c r="C68" t="s">
-        <v>683</v>
+        <v>629</v>
       </c>
       <c r="D68" t="s">
-        <v>684</v>
+        <v>630</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>641</v>
       </c>
       <c r="B69" t="s">
-        <v>279</v>
+        <v>682</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>683</v>
       </c>
       <c r="D69" t="s">
-        <v>45</v>
+        <v>684</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>553</v>
+        <v>99</v>
       </c>
       <c r="B70" t="s">
-        <v>556</v>
+        <v>279</v>
       </c>
       <c r="C70" t="s">
-        <v>555</v>
+        <v>44</v>
       </c>
       <c r="D70" t="s">
-        <v>552</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B71" t="s">
         <v>556</v>
@@ -3467,310 +3497,310 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>420</v>
+        <v>554</v>
       </c>
       <c r="B72" t="s">
-        <v>416</v>
+        <v>556</v>
       </c>
       <c r="C72" t="s">
-        <v>415</v>
+        <v>555</v>
       </c>
       <c r="D72" t="s">
-        <v>418</v>
+        <v>552</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>597</v>
+        <v>420</v>
       </c>
       <c r="B73" t="s">
-        <v>598</v>
+        <v>416</v>
       </c>
       <c r="C73" t="s">
-        <v>602</v>
+        <v>415</v>
       </c>
       <c r="D73" t="s">
-        <v>601</v>
+        <v>418</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>285</v>
+        <v>597</v>
       </c>
       <c r="B74" t="s">
-        <v>267</v>
+        <v>598</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
+        <v>602</v>
       </c>
       <c r="D74" t="s">
-        <v>123</v>
+        <v>601</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>285</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>652</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>647</v>
+        <v>231</v>
       </c>
       <c r="C76" t="s">
-        <v>648</v>
+        <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>653</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>301</v>
+        <v>652</v>
       </c>
       <c r="B77" t="s">
-        <v>248</v>
+        <v>647</v>
       </c>
       <c r="C77" t="s">
-        <v>150</v>
+        <v>648</v>
       </c>
       <c r="D77" t="s">
-        <v>151</v>
+        <v>653</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>359</v>
+        <v>301</v>
       </c>
       <c r="B78" t="s">
-        <v>356</v>
+        <v>248</v>
       </c>
       <c r="C78" t="s">
-        <v>497</v>
+        <v>150</v>
       </c>
       <c r="D78" t="s">
-        <v>358</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>303</v>
+        <v>359</v>
       </c>
       <c r="B79" t="s">
-        <v>248</v>
+        <v>356</v>
       </c>
       <c r="C79" t="s">
-        <v>150</v>
+        <v>497</v>
       </c>
       <c r="D79" t="s">
-        <v>157</v>
+        <v>358</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>303</v>
       </c>
       <c r="B80" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C80" t="s">
-        <v>505</v>
+        <v>150</v>
       </c>
       <c r="D80" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B81" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="C81" t="s">
-        <v>32</v>
+        <v>505</v>
       </c>
       <c r="D81" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>380</v>
+        <v>88</v>
       </c>
       <c r="B82" t="s">
-        <v>384</v>
+        <v>240</v>
       </c>
       <c r="C82" t="s">
-        <v>383</v>
+        <v>32</v>
       </c>
       <c r="D82" t="s">
-        <v>377</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>364</v>
+        <v>380</v>
       </c>
       <c r="B83" t="s">
-        <v>356</v>
+        <v>384</v>
       </c>
       <c r="C83" t="s">
-        <v>497</v>
+        <v>383</v>
       </c>
       <c r="D83" t="s">
-        <v>365</v>
+        <v>377</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>77</v>
+        <v>364</v>
       </c>
       <c r="B84" t="s">
-        <v>232</v>
+        <v>356</v>
       </c>
       <c r="C84" t="s">
-        <v>13</v>
+        <v>497</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>365</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>496</v>
+        <v>77</v>
       </c>
       <c r="B85" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="C85" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="D85" t="s">
-        <v>491</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>304</v>
+        <v>496</v>
       </c>
       <c r="B86" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C86" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="D86" t="s">
-        <v>158</v>
+        <v>491</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>443</v>
+        <v>304</v>
       </c>
       <c r="B87" t="s">
-        <v>440</v>
+        <v>264</v>
       </c>
       <c r="C87" t="s">
-        <v>439</v>
+        <v>67</v>
       </c>
       <c r="D87" t="s">
-        <v>441</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>283</v>
+        <v>443</v>
       </c>
       <c r="B88" t="s">
-        <v>265</v>
+        <v>440</v>
       </c>
       <c r="C88" t="s">
-        <v>118</v>
+        <v>439</v>
       </c>
       <c r="D88" t="s">
-        <v>119</v>
+        <v>441</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>329</v>
+        <v>283</v>
       </c>
       <c r="B89" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C89" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="D89" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="B90" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C90" t="s">
-        <v>669</v>
+        <v>67</v>
       </c>
       <c r="D90" t="s">
-        <v>670</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>468</v>
+        <v>347</v>
       </c>
       <c r="B91" t="s">
-        <v>462</v>
+        <v>272</v>
       </c>
       <c r="C91" t="s">
-        <v>449</v>
+        <v>669</v>
       </c>
       <c r="D91" t="s">
-        <v>456</v>
+        <v>670</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>307</v>
+        <v>468</v>
       </c>
       <c r="B92" t="s">
-        <v>273</v>
+        <v>462</v>
       </c>
       <c r="C92" t="s">
-        <v>139</v>
+        <v>449</v>
       </c>
       <c r="D92" t="s">
-        <v>162</v>
+        <v>456</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>117</v>
+        <v>307</v>
       </c>
       <c r="B93" t="s">
-        <v>264</v>
+        <v>688</v>
       </c>
       <c r="C93" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="D93" t="s">
-        <v>222</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3784,7 +3814,7 @@
         <v>67</v>
       </c>
       <c r="D94" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,12 +3828,12 @@
         <v>67</v>
       </c>
       <c r="D95" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>350</v>
+        <v>117</v>
       </c>
       <c r="B96" t="s">
         <v>264</v>
@@ -3812,273 +3842,273 @@
         <v>67</v>
       </c>
       <c r="D96" t="s">
-        <v>154</v>
+        <v>68</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>586</v>
+        <v>350</v>
       </c>
       <c r="B97" t="s">
-        <v>594</v>
+        <v>264</v>
       </c>
       <c r="C97" t="s">
-        <v>593</v>
+        <v>67</v>
       </c>
       <c r="D97" t="s">
-        <v>589</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>308</v>
+        <v>586</v>
       </c>
       <c r="B98" t="s">
-        <v>518</v>
+        <v>594</v>
       </c>
       <c r="C98" t="s">
-        <v>519</v>
+        <v>593</v>
       </c>
       <c r="D98" t="s">
-        <v>520</v>
+        <v>589</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>308</v>
       </c>
       <c r="B99" t="s">
-        <v>236</v>
+        <v>518</v>
       </c>
       <c r="C99" t="s">
-        <v>23</v>
+        <v>519</v>
       </c>
       <c r="D99" t="s">
-        <v>24</v>
+        <v>520</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>475</v>
+        <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>478</v>
+        <v>236</v>
       </c>
       <c r="C100" t="s">
-        <v>477</v>
+        <v>23</v>
       </c>
       <c r="D100" t="s">
-        <v>476</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>588</v>
+        <v>475</v>
       </c>
       <c r="B101" t="s">
-        <v>594</v>
+        <v>478</v>
       </c>
       <c r="C101" t="s">
-        <v>593</v>
+        <v>477</v>
       </c>
       <c r="D101" t="s">
-        <v>592</v>
+        <v>476</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>354</v>
+        <v>588</v>
       </c>
       <c r="B102" t="s">
-        <v>264</v>
+        <v>594</v>
       </c>
       <c r="C102" t="s">
-        <v>67</v>
+        <v>593</v>
       </c>
       <c r="D102" t="s">
-        <v>219</v>
+        <v>592</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>354</v>
       </c>
       <c r="B103" t="s">
-        <v>682</v>
+        <v>264</v>
       </c>
       <c r="C103" t="s">
-        <v>683</v>
+        <v>67</v>
       </c>
       <c r="D103" t="s">
-        <v>685</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>318</v>
+        <v>114</v>
       </c>
       <c r="B104" t="s">
-        <v>258</v>
+        <v>682</v>
       </c>
       <c r="C104" t="s">
-        <v>159</v>
+        <v>683</v>
       </c>
       <c r="D104" t="s">
-        <v>180</v>
+        <v>685</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>318</v>
       </c>
       <c r="B105" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="C105" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="D105" t="s">
-        <v>53</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C106" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D106" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>343</v>
+        <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C107" t="s">
-        <v>220</v>
+        <v>32</v>
       </c>
       <c r="D107" t="s">
-        <v>221</v>
+        <v>57</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>643</v>
+        <v>343</v>
       </c>
       <c r="B108" t="s">
-        <v>645</v>
+        <v>220</v>
       </c>
       <c r="C108" t="s">
-        <v>644</v>
+        <v>220</v>
       </c>
       <c r="D108" t="s">
-        <v>642</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>333</v>
+        <v>643</v>
       </c>
       <c r="B109" t="s">
-        <v>265</v>
+        <v>645</v>
       </c>
       <c r="C109" t="s">
-        <v>118</v>
+        <v>644</v>
       </c>
       <c r="D109" t="s">
-        <v>204</v>
+        <v>642</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>490</v>
+        <v>333</v>
       </c>
       <c r="B110" t="s">
-        <v>486</v>
+        <v>265</v>
       </c>
       <c r="C110" t="s">
-        <v>485</v>
+        <v>118</v>
       </c>
       <c r="D110" t="s">
-        <v>488</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>490</v>
       </c>
       <c r="B111" t="s">
-        <v>237</v>
+        <v>486</v>
       </c>
       <c r="C111" t="s">
-        <v>27</v>
+        <v>485</v>
       </c>
       <c r="D111" t="s">
-        <v>61</v>
+        <v>488</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>438</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>433</v>
+        <v>237</v>
       </c>
       <c r="C112" t="s">
-        <v>434</v>
+        <v>27</v>
       </c>
       <c r="D112" t="s">
-        <v>436</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="B113" t="s">
-        <v>462</v>
+        <v>433</v>
       </c>
       <c r="C113" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="D113" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>295</v>
+        <v>464</v>
       </c>
       <c r="B114" t="s">
-        <v>273</v>
+        <v>462</v>
       </c>
       <c r="C114" t="s">
-        <v>139</v>
+        <v>449</v>
       </c>
       <c r="D114" t="s">
-        <v>140</v>
+        <v>451</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>76</v>
+        <v>295</v>
       </c>
       <c r="B115" t="s">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="C115" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D115" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4086,55 +4116,55 @@
         <v>76</v>
       </c>
       <c r="B116" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="C116" t="s">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="D116" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>290</v>
+        <v>76</v>
       </c>
       <c r="B117" t="s">
-        <v>269</v>
+        <v>229</v>
       </c>
       <c r="C117" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>82</v>
+        <v>290</v>
       </c>
       <c r="B118" t="s">
-        <v>235</v>
+        <v>269</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>130</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B119" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C119" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="D119" t="s">
-        <v>206</v>
+        <v>22</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4142,55 +4172,55 @@
         <v>104</v>
       </c>
       <c r="B120" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D120" t="s">
-        <v>52</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>411</v>
+        <v>104</v>
       </c>
       <c r="B121" t="s">
-        <v>414</v>
+        <v>234</v>
       </c>
       <c r="C121" t="s">
-        <v>413</v>
+        <v>17</v>
       </c>
       <c r="D121" t="s">
-        <v>409</v>
+        <v>52</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>342</v>
+        <v>411</v>
       </c>
       <c r="B122" t="s">
-        <v>250</v>
+        <v>414</v>
       </c>
       <c r="C122" t="s">
-        <v>164</v>
+        <v>413</v>
       </c>
       <c r="D122" t="s">
-        <v>218</v>
+        <v>409</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>91</v>
+        <v>342</v>
       </c>
       <c r="B123" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="C123" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="D123" t="s">
-        <v>38</v>
+        <v>218</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4198,13 +4228,13 @@
         <v>91</v>
       </c>
       <c r="B124" t="s">
-        <v>446</v>
+        <v>234</v>
       </c>
       <c r="C124" t="s">
-        <v>445</v>
+        <v>17</v>
       </c>
       <c r="D124" t="s">
-        <v>447</v>
+        <v>38</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,91 +4248,91 @@
         <v>445</v>
       </c>
       <c r="D125" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>437</v>
+        <v>91</v>
       </c>
       <c r="B126" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="C126" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="D126" t="s">
-        <v>435</v>
+        <v>448</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>78</v>
+        <v>437</v>
       </c>
       <c r="B127" t="s">
-        <v>233</v>
+        <v>433</v>
       </c>
       <c r="C127" t="s">
-        <v>15</v>
+        <v>434</v>
       </c>
       <c r="D127" t="s">
-        <v>16</v>
+        <v>435</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>466</v>
+        <v>78</v>
       </c>
       <c r="B128" t="s">
-        <v>462</v>
+        <v>233</v>
       </c>
       <c r="C128" t="s">
-        <v>449</v>
+        <v>15</v>
       </c>
       <c r="D128" t="s">
-        <v>454</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>419</v>
+        <v>466</v>
       </c>
       <c r="B129" t="s">
-        <v>416</v>
+        <v>462</v>
       </c>
       <c r="C129" t="s">
-        <v>415</v>
+        <v>449</v>
       </c>
       <c r="D129" t="s">
-        <v>417</v>
+        <v>454</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>360</v>
+        <v>419</v>
       </c>
       <c r="B130" t="s">
-        <v>356</v>
+        <v>416</v>
       </c>
       <c r="C130" t="s">
-        <v>497</v>
+        <v>415</v>
       </c>
       <c r="D130" t="s">
-        <v>361</v>
+        <v>417</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="B131" t="s">
-        <v>255</v>
+        <v>356</v>
       </c>
       <c r="C131" t="s">
-        <v>201</v>
+        <v>497</v>
       </c>
       <c r="D131" t="s">
-        <v>207</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4310,97 +4340,97 @@
         <v>335</v>
       </c>
       <c r="B132" t="s">
-        <v>550</v>
+        <v>255</v>
       </c>
       <c r="C132" t="s">
-        <v>549</v>
+        <v>201</v>
       </c>
       <c r="D132" t="s">
-        <v>548</v>
+        <v>207</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
-        <v>390</v>
+        <v>550</v>
       </c>
       <c r="C133" t="s">
-        <v>389</v>
+        <v>549</v>
       </c>
       <c r="D133" t="s">
-        <v>385</v>
+        <v>548</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>506</v>
+        <v>387</v>
       </c>
       <c r="B134" t="s">
-        <v>507</v>
+        <v>390</v>
       </c>
       <c r="C134" t="s">
-        <v>508</v>
+        <v>389</v>
       </c>
       <c r="D134" t="s">
-        <v>509</v>
+        <v>385</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>71</v>
+        <v>506</v>
       </c>
       <c r="B135" t="s">
-        <v>228</v>
+        <v>507</v>
       </c>
       <c r="C135" t="s">
-        <v>674</v>
+        <v>508</v>
       </c>
       <c r="D135" t="s">
-        <v>1</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>291</v>
+        <v>71</v>
       </c>
       <c r="B136" t="s">
-        <v>270</v>
+        <v>228</v>
       </c>
       <c r="C136" t="s">
-        <v>132</v>
+        <v>674</v>
       </c>
       <c r="D136" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>426</v>
+        <v>291</v>
       </c>
       <c r="B137" t="s">
-        <v>425</v>
+        <v>270</v>
       </c>
       <c r="C137" t="s">
-        <v>424</v>
+        <v>132</v>
       </c>
       <c r="D137" t="s">
-        <v>428</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>302</v>
+        <v>426</v>
       </c>
       <c r="B138" t="s">
-        <v>249</v>
+        <v>425</v>
       </c>
       <c r="C138" t="s">
-        <v>155</v>
+        <v>424</v>
       </c>
       <c r="D138" t="s">
-        <v>156</v>
+        <v>428</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4408,13 +4438,13 @@
         <v>302</v>
       </c>
       <c r="B139" t="s">
-        <v>647</v>
+        <v>249</v>
       </c>
       <c r="C139" t="s">
-        <v>648</v>
+        <v>155</v>
       </c>
       <c r="D139" t="s">
-        <v>649</v>
+        <v>156</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -4422,13 +4452,13 @@
         <v>302</v>
       </c>
       <c r="B140" t="s">
-        <v>425</v>
+        <v>647</v>
       </c>
       <c r="C140" t="s">
-        <v>424</v>
+        <v>648</v>
       </c>
       <c r="D140" t="s">
-        <v>427</v>
+        <v>649</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4436,46 +4466,46 @@
         <v>302</v>
       </c>
       <c r="B141" t="s">
-        <v>462</v>
+        <v>425</v>
       </c>
       <c r="C141" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="D141" t="s">
-        <v>452</v>
+        <v>427</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>603</v>
+        <v>302</v>
       </c>
       <c r="B142" t="s">
-        <v>605</v>
+        <v>462</v>
       </c>
       <c r="C142" t="s">
-        <v>606</v>
+        <v>449</v>
       </c>
       <c r="D142" t="s">
-        <v>604</v>
+        <v>452</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>523</v>
+        <v>603</v>
       </c>
       <c r="B143" t="s">
-        <v>524</v>
+        <v>605</v>
       </c>
       <c r="C143" t="s">
-        <v>525</v>
+        <v>606</v>
       </c>
       <c r="D143" t="s">
-        <v>526</v>
+        <v>604</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B144" t="s">
         <v>524</v>
@@ -4484,315 +4514,315 @@
         <v>525</v>
       </c>
       <c r="D144" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>83</v>
+        <v>527</v>
       </c>
       <c r="B145" t="s">
-        <v>680</v>
+        <v>524</v>
       </c>
       <c r="C145" t="s">
-        <v>681</v>
+        <v>525</v>
       </c>
       <c r="D145" t="s">
-        <v>654</v>
+        <v>528</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>469</v>
+        <v>83</v>
       </c>
       <c r="B146" t="s">
-        <v>462</v>
+        <v>680</v>
       </c>
       <c r="C146" t="s">
-        <v>449</v>
+        <v>681</v>
       </c>
       <c r="D146" t="s">
-        <v>457</v>
+        <v>654</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>95</v>
+        <v>469</v>
       </c>
       <c r="B147" t="s">
-        <v>239</v>
+        <v>462</v>
       </c>
       <c r="C147" t="s">
-        <v>6</v>
+        <v>449</v>
       </c>
       <c r="D147" t="s">
-        <v>7</v>
+        <v>457</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>388</v>
+        <v>95</v>
       </c>
       <c r="B148" t="s">
-        <v>390</v>
+        <v>239</v>
       </c>
       <c r="C148" t="s">
-        <v>389</v>
+        <v>6</v>
       </c>
       <c r="D148" t="s">
-        <v>386</v>
+        <v>7</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B149" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="C149" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="D149" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="B150" t="s">
-        <v>432</v>
+        <v>384</v>
       </c>
       <c r="C150" t="s">
-        <v>430</v>
+        <v>383</v>
       </c>
       <c r="D150" t="s">
-        <v>429</v>
+        <v>378</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>312</v>
+        <v>431</v>
       </c>
       <c r="B151" t="s">
-        <v>267</v>
+        <v>432</v>
       </c>
       <c r="C151" t="s">
-        <v>122</v>
+        <v>430</v>
       </c>
       <c r="D151" t="s">
-        <v>168</v>
+        <v>429</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>412</v>
+        <v>312</v>
       </c>
       <c r="B152" t="s">
-        <v>414</v>
+        <v>267</v>
       </c>
       <c r="C152" t="s">
-        <v>413</v>
+        <v>122</v>
       </c>
       <c r="D152" t="s">
-        <v>410</v>
+        <v>168</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>349</v>
+        <v>412</v>
       </c>
       <c r="B153" t="s">
-        <v>248</v>
+        <v>414</v>
       </c>
       <c r="C153" t="s">
-        <v>150</v>
+        <v>413</v>
       </c>
       <c r="D153" t="s">
-        <v>217</v>
+        <v>410</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B154" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C154" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D154" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>484</v>
+        <v>351</v>
       </c>
       <c r="B155" t="s">
-        <v>482</v>
+        <v>249</v>
       </c>
       <c r="C155" t="s">
-        <v>479</v>
+        <v>155</v>
       </c>
       <c r="D155" t="s">
-        <v>481</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>538</v>
+        <v>484</v>
       </c>
       <c r="B156" t="s">
-        <v>539</v>
+        <v>482</v>
       </c>
       <c r="C156" t="s">
-        <v>540</v>
+        <v>479</v>
       </c>
       <c r="D156" t="s">
-        <v>537</v>
+        <v>481</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>498</v>
+        <v>538</v>
       </c>
       <c r="B157" t="s">
-        <v>499</v>
+        <v>539</v>
       </c>
       <c r="C157" t="s">
-        <v>500</v>
+        <v>540</v>
       </c>
       <c r="D157" t="s">
-        <v>501</v>
+        <v>537</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>620</v>
+        <v>498</v>
       </c>
       <c r="B158" t="s">
-        <v>621</v>
+        <v>499</v>
       </c>
       <c r="C158" t="s">
-        <v>622</v>
+        <v>500</v>
       </c>
       <c r="D158" t="s">
-        <v>619</v>
+        <v>501</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>319</v>
+        <v>620</v>
       </c>
       <c r="B159" t="s">
-        <v>252</v>
+        <v>621</v>
       </c>
       <c r="C159" t="s">
-        <v>182</v>
+        <v>622</v>
       </c>
       <c r="D159" t="s">
-        <v>183</v>
+        <v>619</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="B160" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="C160" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="D160" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>494</v>
+        <v>311</v>
       </c>
       <c r="B161" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="C161" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="D161" t="s">
-        <v>492</v>
+        <v>167</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
       <c r="B162" t="s">
-        <v>507</v>
+        <v>266</v>
       </c>
       <c r="C162" t="s">
-        <v>508</v>
+        <v>120</v>
       </c>
       <c r="D162" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>397</v>
+        <v>514</v>
       </c>
       <c r="B163" t="s">
-        <v>404</v>
+        <v>507</v>
       </c>
       <c r="C163" t="s">
-        <v>403</v>
+        <v>508</v>
       </c>
       <c r="D163" t="s">
-        <v>398</v>
+        <v>510</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B164" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="C164" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="D164" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B165" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C165" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="D165" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>85</v>
+        <v>395</v>
       </c>
       <c r="B166" t="s">
-        <v>237</v>
+        <v>404</v>
       </c>
       <c r="C166" t="s">
-        <v>27</v>
+        <v>403</v>
       </c>
       <c r="D166" t="s">
-        <v>28</v>
+        <v>398</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4800,46 +4830,46 @@
         <v>85</v>
       </c>
       <c r="B167" t="s">
-        <v>594</v>
+        <v>237</v>
       </c>
       <c r="C167" t="s">
-        <v>593</v>
+        <v>27</v>
       </c>
       <c r="D167" t="s">
-        <v>590</v>
+        <v>28</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>353</v>
+        <v>85</v>
       </c>
       <c r="B168" t="s">
-        <v>248</v>
+        <v>594</v>
       </c>
       <c r="C168" t="s">
-        <v>150</v>
+        <v>593</v>
       </c>
       <c r="D168" t="s">
-        <v>208</v>
+        <v>590</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>470</v>
+        <v>353</v>
       </c>
       <c r="B169" t="s">
-        <v>462</v>
+        <v>248</v>
       </c>
       <c r="C169" t="s">
-        <v>449</v>
+        <v>150</v>
       </c>
       <c r="D169" t="s">
-        <v>458</v>
+        <v>208</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="B170" t="s">
         <v>462</v>
@@ -4848,77 +4878,77 @@
         <v>449</v>
       </c>
       <c r="D170" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>551</v>
+        <v>463</v>
       </c>
       <c r="B171" t="s">
-        <v>550</v>
+        <v>462</v>
       </c>
       <c r="C171" t="s">
-        <v>549</v>
+        <v>449</v>
       </c>
       <c r="D171" t="s">
-        <v>547</v>
+        <v>450</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>346</v>
+        <v>551</v>
       </c>
       <c r="B172" t="s">
-        <v>274</v>
+        <v>550</v>
       </c>
       <c r="C172" t="s">
-        <v>143</v>
+        <v>549</v>
       </c>
       <c r="D172" t="s">
-        <v>144</v>
+        <v>547</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>286</v>
+        <v>346</v>
       </c>
       <c r="B173" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C173" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
       <c r="D173" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>97</v>
+        <v>286</v>
       </c>
       <c r="B174" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
       <c r="C174" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="D174" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>612</v>
+        <v>97</v>
       </c>
       <c r="B175" t="s">
-        <v>614</v>
+        <v>229</v>
       </c>
       <c r="C175" t="s">
-        <v>613</v>
+        <v>2</v>
       </c>
       <c r="D175" t="s">
-        <v>608</v>
+        <v>34</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4932,7 +4962,7 @@
         <v>613</v>
       </c>
       <c r="D176" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -4946,91 +4976,91 @@
         <v>613</v>
       </c>
       <c r="D177" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>631</v>
+        <v>612</v>
       </c>
       <c r="B178" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="C178" t="s">
-        <v>632</v>
+        <v>613</v>
       </c>
       <c r="D178" t="s">
-        <v>634</v>
+        <v>610</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>339</v>
+        <v>631</v>
       </c>
       <c r="B179" t="s">
-        <v>264</v>
+        <v>633</v>
       </c>
       <c r="C179" t="s">
-        <v>67</v>
+        <v>632</v>
       </c>
       <c r="D179" t="s">
-        <v>214</v>
+        <v>634</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>529</v>
+        <v>339</v>
       </c>
       <c r="B180" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C180" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D180" t="s">
-        <v>530</v>
+        <v>214</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>300</v>
+        <v>529</v>
       </c>
       <c r="B181" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="C181" t="s">
-        <v>134</v>
+        <v>44</v>
       </c>
       <c r="D181" t="s">
-        <v>149</v>
+        <v>530</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>502</v>
+        <v>300</v>
       </c>
       <c r="B182" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="C182" t="s">
-        <v>503</v>
+        <v>134</v>
       </c>
       <c r="D182" t="s">
-        <v>504</v>
+        <v>149</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>313</v>
+        <v>502</v>
       </c>
       <c r="B183" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="C183" t="s">
-        <v>169</v>
+        <v>503</v>
       </c>
       <c r="D183" t="s">
-        <v>170</v>
+        <v>504</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5038,727 +5068,727 @@
         <v>313</v>
       </c>
       <c r="B184" t="s">
-        <v>404</v>
+        <v>251</v>
       </c>
       <c r="C184" t="s">
-        <v>403</v>
+        <v>169</v>
       </c>
       <c r="D184" t="s">
-        <v>401</v>
+        <v>170</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>112</v>
+        <v>313</v>
       </c>
       <c r="B185" t="s">
-        <v>263</v>
+        <v>404</v>
       </c>
       <c r="C185" t="s">
-        <v>50</v>
+        <v>403</v>
       </c>
       <c r="D185" t="s">
-        <v>62</v>
+        <v>401</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>321</v>
+        <v>112</v>
       </c>
       <c r="B186" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C186" t="s">
-        <v>138</v>
+        <v>50</v>
       </c>
       <c r="D186" t="s">
-        <v>185</v>
+        <v>62</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>513</v>
+        <v>321</v>
       </c>
       <c r="B187" t="s">
-        <v>507</v>
+        <v>272</v>
       </c>
       <c r="C187" t="s">
-        <v>508</v>
+        <v>138</v>
       </c>
       <c r="D187" t="s">
-        <v>517</v>
+        <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>664</v>
+        <v>513</v>
       </c>
       <c r="B188" t="s">
-        <v>665</v>
+        <v>507</v>
       </c>
       <c r="C188" t="s">
-        <v>666</v>
+        <v>508</v>
       </c>
       <c r="D188" t="s">
-        <v>667</v>
+        <v>517</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>287</v>
+        <v>664</v>
       </c>
       <c r="B189" t="s">
-        <v>264</v>
+        <v>665</v>
       </c>
       <c r="C189" t="s">
-        <v>67</v>
+        <v>666</v>
       </c>
       <c r="D189" t="s">
-        <v>125</v>
+        <v>667</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>355</v>
+        <v>287</v>
       </c>
       <c r="B190" t="s">
-        <v>356</v>
+        <v>264</v>
       </c>
       <c r="C190" t="s">
-        <v>497</v>
+        <v>67</v>
       </c>
       <c r="D190" t="s">
-        <v>357</v>
+        <v>125</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>80</v>
+        <v>355</v>
       </c>
       <c r="B191" t="s">
-        <v>256</v>
+        <v>356</v>
       </c>
       <c r="C191" t="s">
-        <v>673</v>
+        <v>497</v>
       </c>
       <c r="D191" t="s">
-        <v>19</v>
+        <v>357</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>576</v>
+        <v>80</v>
       </c>
       <c r="B192" t="s">
-        <v>575</v>
+        <v>256</v>
       </c>
       <c r="C192" t="s">
-        <v>573</v>
+        <v>673</v>
       </c>
       <c r="D192" t="s">
-        <v>574</v>
+        <v>19</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>297</v>
+        <v>576</v>
       </c>
       <c r="B193" t="s">
-        <v>245</v>
+        <v>575</v>
       </c>
       <c r="C193" t="s">
-        <v>126</v>
+        <v>573</v>
       </c>
       <c r="D193" t="s">
-        <v>142</v>
+        <v>574</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>399</v>
+        <v>297</v>
       </c>
       <c r="B194" t="s">
-        <v>404</v>
+        <v>245</v>
       </c>
       <c r="C194" t="s">
-        <v>403</v>
+        <v>126</v>
       </c>
       <c r="D194" t="s">
-        <v>400</v>
+        <v>142</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>659</v>
+        <v>399</v>
       </c>
       <c r="B195" t="s">
-        <v>655</v>
+        <v>404</v>
       </c>
       <c r="C195" t="s">
-        <v>656</v>
+        <v>403</v>
       </c>
       <c r="D195" t="s">
-        <v>660</v>
+        <v>400</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>325</v>
+        <v>659</v>
       </c>
       <c r="B196" t="s">
-        <v>280</v>
+        <v>655</v>
       </c>
       <c r="C196" t="s">
-        <v>191</v>
+        <v>656</v>
       </c>
       <c r="D196" t="s">
-        <v>192</v>
+        <v>660</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>72</v>
+        <v>325</v>
       </c>
       <c r="B197" t="s">
-        <v>229</v>
+        <v>280</v>
       </c>
       <c r="C197" t="s">
-        <v>2</v>
+        <v>191</v>
       </c>
       <c r="D197" t="s">
-        <v>3</v>
+        <v>192</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>657</v>
+        <v>72</v>
       </c>
       <c r="B198" t="s">
-        <v>655</v>
+        <v>229</v>
       </c>
       <c r="C198" t="s">
-        <v>656</v>
+        <v>2</v>
       </c>
       <c r="D198" t="s">
-        <v>658</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>86</v>
+        <v>657</v>
       </c>
       <c r="B199" t="s">
-        <v>29</v>
+        <v>655</v>
       </c>
       <c r="C199" t="s">
-        <v>29</v>
+        <v>656</v>
       </c>
       <c r="D199" t="s">
-        <v>30</v>
+        <v>658</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>306</v>
+        <v>86</v>
       </c>
       <c r="B200" t="s">
-        <v>272</v>
+        <v>29</v>
       </c>
       <c r="C200" t="s">
-        <v>669</v>
+        <v>29</v>
       </c>
       <c r="D200" t="s">
-        <v>671</v>
+        <v>30</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>472</v>
+        <v>306</v>
       </c>
       <c r="B201" t="s">
-        <v>462</v>
+        <v>272</v>
       </c>
       <c r="C201" t="s">
-        <v>449</v>
+        <v>669</v>
       </c>
       <c r="D201" t="s">
-        <v>460</v>
+        <v>671</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>444</v>
+        <v>472</v>
       </c>
       <c r="B202" t="s">
-        <v>440</v>
+        <v>462</v>
       </c>
       <c r="C202" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="D202" t="s">
-        <v>442</v>
+        <v>460</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>557</v>
+        <v>444</v>
       </c>
       <c r="B203" t="s">
-        <v>559</v>
+        <v>440</v>
       </c>
       <c r="C203" t="s">
-        <v>560</v>
+        <v>439</v>
       </c>
       <c r="D203" t="s">
-        <v>561</v>
+        <v>442</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>331</v>
+        <v>557</v>
       </c>
       <c r="B204" t="s">
-        <v>255</v>
+        <v>559</v>
       </c>
       <c r="C204" t="s">
-        <v>201</v>
+        <v>560</v>
       </c>
       <c r="D204" t="s">
-        <v>202</v>
+        <v>561</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>474</v>
+        <v>331</v>
       </c>
       <c r="B205" t="s">
-        <v>478</v>
+        <v>255</v>
       </c>
       <c r="C205" t="s">
-        <v>477</v>
+        <v>201</v>
       </c>
       <c r="D205" t="s">
-        <v>476</v>
+        <v>202</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>314</v>
+        <v>474</v>
       </c>
       <c r="B206" t="s">
-        <v>245</v>
+        <v>478</v>
       </c>
       <c r="C206" t="s">
-        <v>126</v>
+        <v>477</v>
       </c>
       <c r="D206" t="s">
-        <v>171</v>
+        <v>476</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>84</v>
+        <v>314</v>
       </c>
       <c r="B207" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C207" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="D207" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>305</v>
+        <v>692</v>
       </c>
       <c r="B208" t="s">
-        <v>258</v>
+        <v>693</v>
       </c>
       <c r="C208" t="s">
-        <v>159</v>
+        <v>694</v>
       </c>
       <c r="D208" t="s">
-        <v>160</v>
+        <v>695</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>328</v>
+        <v>84</v>
       </c>
       <c r="B209" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="C209" t="s">
-        <v>669</v>
+        <v>25</v>
       </c>
       <c r="D209" t="s">
-        <v>672</v>
+        <v>26</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>473</v>
+        <v>305</v>
       </c>
       <c r="B210" t="s">
-        <v>462</v>
+        <v>258</v>
       </c>
       <c r="C210" t="s">
-        <v>449</v>
+        <v>159</v>
       </c>
       <c r="D210" t="s">
-        <v>461</v>
+        <v>160</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>90</v>
+        <v>328</v>
       </c>
       <c r="B211" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="C211" t="s">
-        <v>36</v>
+        <v>669</v>
       </c>
       <c r="D211" t="s">
-        <v>37</v>
+        <v>672</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>326</v>
+        <v>473</v>
       </c>
       <c r="B212" t="s">
-        <v>266</v>
+        <v>462</v>
       </c>
       <c r="C212" t="s">
-        <v>120</v>
+        <v>449</v>
       </c>
       <c r="D212" t="s">
-        <v>193</v>
+        <v>461</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>332</v>
+        <v>90</v>
       </c>
       <c r="B213" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="C213" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="D213" t="s">
-        <v>203</v>
+        <v>37</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>650</v>
+        <v>326</v>
       </c>
       <c r="B214" t="s">
-        <v>647</v>
+        <v>266</v>
       </c>
       <c r="C214" t="s">
-        <v>648</v>
+        <v>120</v>
       </c>
       <c r="D214" t="s">
-        <v>651</v>
+        <v>193</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>567</v>
+        <v>332</v>
       </c>
       <c r="B215" t="s">
-        <v>569</v>
+        <v>273</v>
       </c>
       <c r="C215" t="s">
-        <v>572</v>
+        <v>139</v>
       </c>
       <c r="D215" t="s">
-        <v>571</v>
+        <v>203</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>324</v>
+        <v>650</v>
       </c>
       <c r="B216" t="s">
-        <v>239</v>
+        <v>647</v>
       </c>
       <c r="C216" t="s">
-        <v>6</v>
+        <v>648</v>
       </c>
       <c r="D216" t="s">
-        <v>190</v>
+        <v>651</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>366</v>
+        <v>567</v>
       </c>
       <c r="B217" t="s">
-        <v>356</v>
+        <v>569</v>
       </c>
       <c r="C217" t="s">
-        <v>497</v>
+        <v>572</v>
       </c>
       <c r="D217" t="s">
-        <v>367</v>
+        <v>571</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>288</v>
+        <v>324</v>
       </c>
       <c r="B218" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C218" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="D218" t="s">
-        <v>127</v>
+        <v>190</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>467</v>
+        <v>366</v>
       </c>
       <c r="B219" t="s">
-        <v>462</v>
+        <v>356</v>
       </c>
       <c r="C219" t="s">
-        <v>449</v>
+        <v>497</v>
       </c>
       <c r="D219" t="s">
-        <v>455</v>
+        <v>367</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="B220" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="C220" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D220" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>515</v>
+        <v>467</v>
       </c>
       <c r="B221" t="s">
-        <v>507</v>
+        <v>462</v>
       </c>
       <c r="C221" t="s">
-        <v>508</v>
+        <v>449</v>
       </c>
       <c r="D221" t="s">
-        <v>511</v>
+        <v>455</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>100</v>
+        <v>320</v>
       </c>
       <c r="B222" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="C222" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="D222" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>100</v>
+        <v>515</v>
       </c>
       <c r="B223" t="s">
-        <v>240</v>
+        <v>507</v>
       </c>
       <c r="C223" t="s">
-        <v>32</v>
+        <v>508</v>
       </c>
       <c r="D223" t="s">
-        <v>46</v>
+        <v>511</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>338</v>
+        <v>100</v>
       </c>
       <c r="B224" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C224" t="s">
-        <v>212</v>
+        <v>64</v>
       </c>
       <c r="D224" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>536</v>
+        <v>100</v>
       </c>
       <c r="B225" t="s">
-        <v>532</v>
+        <v>240</v>
       </c>
       <c r="C225" t="s">
-        <v>533</v>
+        <v>32</v>
       </c>
       <c r="D225" t="s">
-        <v>535</v>
+        <v>46</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>98</v>
+        <v>338</v>
       </c>
       <c r="B226" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="C226" t="s">
-        <v>21</v>
+        <v>212</v>
       </c>
       <c r="D226" t="s">
-        <v>39</v>
+        <v>213</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>113</v>
+        <v>536</v>
       </c>
       <c r="B227" t="s">
-        <v>234</v>
+        <v>532</v>
       </c>
       <c r="C227" t="s">
-        <v>17</v>
+        <v>533</v>
       </c>
       <c r="D227" t="s">
-        <v>63</v>
+        <v>535</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>382</v>
+        <v>98</v>
       </c>
       <c r="B228" t="s">
-        <v>384</v>
+        <v>235</v>
       </c>
       <c r="C228" t="s">
-        <v>383</v>
+        <v>21</v>
       </c>
       <c r="D228" t="s">
-        <v>379</v>
+        <v>39</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>661</v>
+        <v>113</v>
       </c>
       <c r="B229" t="s">
-        <v>655</v>
+        <v>234</v>
       </c>
       <c r="C229" t="s">
-        <v>656</v>
+        <v>17</v>
       </c>
       <c r="D229" t="s">
-        <v>662</v>
+        <v>63</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>310</v>
+        <v>382</v>
       </c>
       <c r="B230" t="s">
-        <v>250</v>
+        <v>384</v>
       </c>
       <c r="C230" t="s">
-        <v>164</v>
+        <v>383</v>
       </c>
       <c r="D230" t="s">
-        <v>165</v>
+        <v>379</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>344</v>
+        <v>661</v>
       </c>
       <c r="B231" t="s">
-        <v>269</v>
+        <v>655</v>
       </c>
       <c r="C231" t="s">
-        <v>130</v>
+        <v>656</v>
       </c>
       <c r="D231" t="s">
-        <v>224</v>
+        <v>662</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
       <c r="B232" t="s">
-        <v>404</v>
+        <v>250</v>
       </c>
       <c r="C232" t="s">
-        <v>403</v>
+        <v>164</v>
       </c>
       <c r="D232" t="s">
-        <v>402</v>
+        <v>165</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>299</v>
+        <v>344</v>
       </c>
       <c r="B233" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C233" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D233" t="s">
-        <v>148</v>
+        <v>224</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>89</v>
+        <v>344</v>
       </c>
       <c r="B234" t="s">
-        <v>236</v>
+        <v>404</v>
       </c>
       <c r="C234" t="s">
-        <v>23</v>
+        <v>403</v>
       </c>
       <c r="D234" t="s">
-        <v>35</v>
+        <v>402</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>89</v>
+        <v>299</v>
       </c>
       <c r="B235" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C235" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D235" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5766,13 +5796,13 @@
         <v>89</v>
       </c>
       <c r="B236" t="s">
-        <v>279</v>
+        <v>236</v>
       </c>
       <c r="C236" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D236" t="s">
-        <v>177</v>
+        <v>35</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5786,213 +5816,255 @@
         <v>128</v>
       </c>
       <c r="D237" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B238" t="s">
-        <v>234</v>
+        <v>279</v>
       </c>
       <c r="C238" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D238" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B239" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="C239" t="s">
-        <v>196</v>
+        <v>128</v>
       </c>
       <c r="D239" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B240" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C240" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D240" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B241" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C241" t="s">
-        <v>64</v>
+        <v>196</v>
       </c>
       <c r="D241" t="s">
-        <v>65</v>
+        <v>197</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>582</v>
+        <v>101</v>
       </c>
       <c r="B242" t="s">
-        <v>581</v>
+        <v>242</v>
       </c>
       <c r="C242" t="s">
-        <v>585</v>
+        <v>47</v>
       </c>
       <c r="D242" t="s">
-        <v>583</v>
+        <v>48</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>582</v>
+        <v>101</v>
       </c>
       <c r="B243" t="s">
-        <v>581</v>
+        <v>689</v>
       </c>
       <c r="C243" t="s">
-        <v>585</v>
+        <v>690</v>
       </c>
       <c r="D243" t="s">
-        <v>584</v>
+        <v>691</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>374</v>
+        <v>115</v>
       </c>
       <c r="B244" t="s">
-        <v>376</v>
+        <v>244</v>
       </c>
       <c r="C244" t="s">
-        <v>375</v>
+        <v>64</v>
       </c>
       <c r="D244" t="s">
-        <v>373</v>
+        <v>65</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>323</v>
+        <v>582</v>
       </c>
       <c r="B245" t="s">
-        <v>247</v>
+        <v>581</v>
       </c>
       <c r="C245" t="s">
-        <v>145</v>
+        <v>585</v>
       </c>
       <c r="D245" t="s">
-        <v>189</v>
+        <v>583</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>489</v>
+        <v>582</v>
       </c>
       <c r="B246" t="s">
-        <v>486</v>
+        <v>581</v>
       </c>
       <c r="C246" t="s">
-        <v>485</v>
+        <v>585</v>
       </c>
       <c r="D246" t="s">
-        <v>487</v>
+        <v>584</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>289</v>
+        <v>374</v>
       </c>
       <c r="B247" t="s">
-        <v>268</v>
+        <v>376</v>
       </c>
       <c r="C247" t="s">
-        <v>128</v>
+        <v>375</v>
       </c>
       <c r="D247" t="s">
-        <v>129</v>
+        <v>373</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>106</v>
+        <v>323</v>
       </c>
       <c r="B248" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C248" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="D248" t="s">
-        <v>54</v>
+        <v>189</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>293</v>
+        <v>489</v>
       </c>
       <c r="B249" t="s">
-        <v>271</v>
+        <v>486</v>
       </c>
       <c r="C249" t="s">
-        <v>136</v>
+        <v>485</v>
       </c>
       <c r="D249" t="s">
-        <v>137</v>
+        <v>487</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>677</v>
+        <v>289</v>
       </c>
       <c r="B250" t="s">
-        <v>676</v>
+        <v>268</v>
       </c>
       <c r="C250" t="s">
-        <v>678</v>
+        <v>128</v>
       </c>
       <c r="D250" t="s">
-        <v>675</v>
+        <v>129</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
+        <v>106</v>
+      </c>
+      <c r="B251" t="s">
+        <v>235</v>
+      </c>
+      <c r="C251" t="s">
+        <v>21</v>
+      </c>
+      <c r="D251" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>293</v>
+      </c>
+      <c r="B252" t="s">
+        <v>271</v>
+      </c>
+      <c r="C252" t="s">
+        <v>136</v>
+      </c>
+      <c r="D252" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>677</v>
+      </c>
+      <c r="B253" t="s">
+        <v>676</v>
+      </c>
+      <c r="C253" t="s">
+        <v>678</v>
+      </c>
+      <c r="D253" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
         <v>686</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B254" t="s">
         <v>682</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C254" t="s">
         <v>683</v>
       </c>
-      <c r="D251" t="s">
+      <c r="D254" t="s">
         <v>687</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D195" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D202">
-      <sortCondition ref="A1:A195"/>
+  <autoFilter ref="A1:D196" xr:uid="{F238FD4B-105D-484A-A0CF-9927340DFADE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D203">
+      <sortCondition ref="A1:A196"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D249">
-    <sortCondition ref="A2:A249"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D252">
+    <sortCondition ref="A2:A252"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>